<commit_message>
pilot 3 - updated results.
</commit_message>
<xml_diff>
--- a/UnityProject/results.xlsx
+++ b/UnityProject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="330" windowWidth="113955" windowHeight="16890" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="330" windowWidth="113955" windowHeight="16890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -136,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,8 +151,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +169,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,15 +186,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -244,7 +259,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.96666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -288,36 +303,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>0.93333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.43333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="68072576"/>
-        <c:axId val="68074112"/>
+        <c:axId val="131977984"/>
+        <c:axId val="131979520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68072576"/>
+        <c:axId val="131977984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68074112"/>
+        <c:crossAx val="131979520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68074112"/>
+        <c:axId val="131979520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -325,7 +340,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68072576"/>
+        <c:crossAx val="131977984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -338,7 +353,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -377,13 +392,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>46.948446903669378</c:v>
+                    <c:v>64.455967030398014</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>166.61855638953705</c:v>
+                    <c:v>92.245974068252778</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>248.39645953819692</c:v>
+                    <c:v>178.99620621104802</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -395,13 +410,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>46.948446903669378</c:v>
+                    <c:v>64.455967030398014</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>166.61855638953705</c:v>
+                    <c:v>92.245974068252778</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>248.39645953819692</c:v>
+                    <c:v>178.99620621104802</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -431,13 +446,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1179.3</c:v>
+                  <c:v>1248.7666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1084.0999999999999</c:v>
+                  <c:v>1175.1666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1216.7</c:v>
+                  <c:v>1297.5517241379309</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -467,13 +482,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>415.02998924813693</c:v>
+                    <c:v>185.09066885523671</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>87.498120614737289</c:v>
+                    <c:v>52.45479418250202</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>631.19683142423958</c:v>
+                    <c:v>382.46575435512898</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -485,13 +500,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>415.02998924813693</c:v>
+                    <c:v>185.09066885523671</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>87.498120614737289</c:v>
+                    <c:v>52.45479418250202</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>631.19683142423958</c:v>
+                    <c:v>382.46575435512898</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -521,36 +536,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1765.5555555555557</c:v>
+                  <c:v>1728.6785714285713</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1198.0999999999999</c:v>
+                  <c:v>1267.8214285714287</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2028.8</c:v>
+                  <c:v>1955.7692307692307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="129139840"/>
-        <c:axId val="129142144"/>
+        <c:axId val="133740416"/>
+        <c:axId val="133741952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129139840"/>
+        <c:axId val="133740416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129142144"/>
+        <c:crossAx val="133741952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129142144"/>
+        <c:axId val="133741952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -558,7 +573,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129139840"/>
+        <c:crossAx val="133740416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -571,7 +586,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -935,7 +950,7 @@
   <dimension ref="A1:BI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AQ11" sqref="AQ11"/>
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1925,7 +1940,7 @@
       </c>
     </row>
     <row r="5" spans="1:61">
-      <c r="A5">
+      <c r="A5" s="1">
         <f>error!A5</f>
         <v>2</v>
       </c>
@@ -2111,73 +2126,427 @@
       </c>
     </row>
     <row r="6" spans="1:61">
-      <c r="A6">
-        <f>error!A6</f>
-        <v>0</v>
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>31</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>56</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>13</v>
+      </c>
+      <c r="P6">
+        <v>7</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>7</v>
+      </c>
+      <c r="S6">
+        <v>61</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <v>9</v>
+      </c>
+      <c r="V6">
+        <v>6</v>
+      </c>
+      <c r="W6">
+        <v>3</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>6</v>
+      </c>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>6</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>7</v>
+      </c>
+      <c r="AD6">
+        <v>12</v>
+      </c>
+      <c r="AE6">
+        <v>6</v>
+      </c>
+      <c r="AF6">
+        <v>5</v>
+      </c>
+      <c r="AG6">
+        <v>4</v>
+      </c>
+      <c r="AH6">
+        <v>4</v>
+      </c>
+      <c r="AI6">
+        <v>7</v>
+      </c>
+      <c r="AJ6">
+        <v>2</v>
+      </c>
+      <c r="AK6">
+        <v>6</v>
+      </c>
+      <c r="AL6">
+        <v>5</v>
+      </c>
+      <c r="AM6">
+        <v>7</v>
+      </c>
+      <c r="AN6">
+        <v>7</v>
+      </c>
+      <c r="AO6">
+        <v>5</v>
+      </c>
+      <c r="AP6">
+        <v>6</v>
+      </c>
+      <c r="AQ6">
+        <v>-1</v>
+      </c>
+      <c r="AR6">
+        <v>8</v>
+      </c>
+      <c r="AS6">
+        <v>-1</v>
+      </c>
+      <c r="AT6">
+        <v>6</v>
+      </c>
+      <c r="AU6">
+        <v>-1</v>
+      </c>
+      <c r="AV6">
+        <v>11</v>
+      </c>
+      <c r="AW6">
+        <v>4</v>
+      </c>
+      <c r="AX6">
+        <v>4</v>
+      </c>
+      <c r="AY6">
+        <v>-1</v>
+      </c>
+      <c r="AZ6">
+        <v>10</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>9</v>
+      </c>
+      <c r="BC6">
+        <v>-1</v>
+      </c>
+      <c r="BD6">
+        <v>7</v>
+      </c>
+      <c r="BE6">
+        <v>-1</v>
+      </c>
+      <c r="BF6">
+        <v>6</v>
+      </c>
+      <c r="BG6">
+        <v>-1</v>
+      </c>
+      <c r="BH6">
+        <v>7</v>
+      </c>
+      <c r="BI6">
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:61">
-      <c r="A7">
-        <f>error!A7</f>
-        <v>0</v>
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>8</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>16</v>
+      </c>
+      <c r="T7">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>14</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7">
+        <v>3</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AB7">
+        <v>4</v>
+      </c>
+      <c r="AC7">
+        <v>8</v>
+      </c>
+      <c r="AD7">
+        <v>13</v>
+      </c>
+      <c r="AE7">
+        <v>11</v>
+      </c>
+      <c r="AF7">
+        <v>13</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7">
+        <v>8</v>
+      </c>
+      <c r="AI7">
+        <v>7</v>
+      </c>
+      <c r="AJ7">
+        <v>6</v>
+      </c>
+      <c r="AK7">
+        <v>3</v>
+      </c>
+      <c r="AL7">
+        <v>9</v>
+      </c>
+      <c r="AM7">
+        <v>22</v>
+      </c>
+      <c r="AN7">
+        <v>5</v>
+      </c>
+      <c r="AO7">
+        <v>13</v>
+      </c>
+      <c r="AP7">
+        <v>7</v>
+      </c>
+      <c r="AQ7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>17</v>
+      </c>
+      <c r="AS7">
+        <v>-1</v>
+      </c>
+      <c r="AT7">
+        <v>9</v>
+      </c>
+      <c r="AU7">
+        <v>13</v>
+      </c>
+      <c r="AV7">
+        <v>-1</v>
+      </c>
+      <c r="AW7">
+        <v>-1</v>
+      </c>
+      <c r="AX7">
+        <v>7</v>
+      </c>
+      <c r="AY7">
+        <v>-1</v>
+      </c>
+      <c r="AZ7">
+        <v>1</v>
+      </c>
+      <c r="BA7">
+        <v>-1</v>
+      </c>
+      <c r="BB7">
+        <v>17</v>
+      </c>
+      <c r="BC7">
+        <v>8</v>
+      </c>
+      <c r="BD7">
+        <v>2</v>
+      </c>
+      <c r="BE7">
+        <v>2</v>
+      </c>
+      <c r="BF7">
+        <v>13</v>
+      </c>
+      <c r="BG7">
+        <v>12</v>
+      </c>
+      <c r="BH7">
+        <v>12</v>
+      </c>
+      <c r="BI7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:61">
-      <c r="A8">
+      <c r="A8" s="1">
         <f>error!A8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:61">
-      <c r="A9">
+      <c r="A9" s="1">
         <f>error!A9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:61">
-      <c r="A10">
+      <c r="A10" s="1">
         <f>error!A10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:61">
-      <c r="A11">
+      <c r="A11" s="1">
         <f>error!A11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:61">
-      <c r="A12">
+      <c r="A12" s="1">
         <f>error!A12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:61">
-      <c r="A13">
+      <c r="A13" s="1">
         <f>error!A13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:61">
-      <c r="A14">
+      <c r="A14" s="1">
         <f>error!A14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:61">
-      <c r="A15">
+      <c r="A15" s="1">
         <f>error!A15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:61">
-      <c r="A16">
+      <c r="A16" s="1">
         <f>error!A16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="1">
         <f>error!A17</f>
         <v>0</v>
       </c>
@@ -2191,8 +2560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AJ26" sqref="AJ26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2671,7 +3040,7 @@
         <v>(para)foveal</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:V3" si="6">C3</f>
+        <f t="shared" ref="E3:U3" si="6">C3</f>
         <v>peripheral</v>
       </c>
       <c r="F3" t="str">
@@ -2962,249 +3331,760 @@
       </c>
     </row>
     <row r="5" spans="1:61">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5">
-        <f>IF(AND(distance!B5&lt;25,distance!B5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!B5&lt;80,distance!B5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(AND(distance!C5&lt;25,distance!C5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!C5&lt;80,distance!C5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="D5">
-        <f>IF(AND(distance!D5&lt;25,distance!D5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!D5&lt;80,distance!D5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="E5">
-        <f>IF(AND(distance!E5&lt;25,distance!E5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!E5&lt;80,distance!E5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="F5">
-        <f>IF(AND(distance!F5&lt;25,distance!F5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!F5&lt;80,distance!F5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="G5">
-        <f>IF(AND(distance!G5&lt;25,distance!G5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!G5&lt;80,distance!G5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="H5">
-        <f>IF(AND(distance!H5&lt;25,distance!H5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!H5&lt;80,distance!H5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="I5">
-        <f>IF(AND(distance!I5&lt;25,distance!I5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!I5&lt;80,distance!I5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="J5">
-        <f>IF(AND(distance!J5&lt;25,distance!J5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!J5&lt;80,distance!J5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>IF(AND(distance!K5&lt;25,distance!K5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!K5&lt;80,distance!K5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="L5">
-        <f>IF(AND(distance!L5&lt;25,distance!L5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!L5&lt;80,distance!L5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="M5">
-        <f>IF(AND(distance!M5&lt;25,distance!M5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!M5&lt;80,distance!M5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="N5">
-        <f>IF(AND(distance!N5&lt;25,distance!N5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!N5&lt;80,distance!N5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="O5">
-        <f>IF(AND(distance!O5&lt;25,distance!O5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!O5&lt;80,distance!O5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="P5">
-        <f>IF(AND(distance!P5&lt;25,distance!P5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!P5&lt;80,distance!P5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="Q5">
-        <f>IF(AND(distance!Q5&lt;25,distance!Q5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!Q5&lt;80,distance!Q5&gt;=0),1,0)</f>
         <v>0</v>
       </c>
       <c r="R5">
-        <f>IF(AND(distance!R5&lt;25,distance!R5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!R5&lt;80,distance!R5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="S5">
-        <f>IF(AND(distance!S5&lt;25,distance!S5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!S5&lt;80,distance!S5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="T5">
-        <f>IF(AND(distance!T5&lt;25,distance!T5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!T5&lt;80,distance!T5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="U5">
-        <f>IF(AND(distance!U5&lt;25,distance!U5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!U5&lt;80,distance!U5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="V5">
-        <f>IF(AND(distance!V5&lt;25,distance!V5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!V5&lt;80,distance!V5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="W5">
-        <f>IF(AND(distance!W5&lt;25,distance!W5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!W5&lt;80,distance!W5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="X5">
-        <f>IF(AND(distance!X5&lt;25,distance!X5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!X5&lt;80,distance!X5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="Y5">
-        <f>IF(AND(distance!Y5&lt;25,distance!Y5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!Y5&lt;80,distance!Y5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="Z5">
-        <f>IF(AND(distance!Z5&lt;25,distance!Z5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!Z5&lt;80,distance!Z5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AA5">
-        <f>IF(AND(distance!AA5&lt;25,distance!AA5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AA5&lt;80,distance!AA5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AB5">
-        <f>IF(AND(distance!AB5&lt;25,distance!AB5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AB5&lt;80,distance!AB5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AC5">
-        <f>IF(AND(distance!AC5&lt;25,distance!AC5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AC5&lt;80,distance!AC5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AD5">
-        <f>IF(AND(distance!AD5&lt;25,distance!AD5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AD5&lt;80,distance!AD5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AE5">
-        <f>IF(AND(distance!AE5&lt;25,distance!AE5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AE5&lt;80,distance!AE5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AF5">
-        <f>IF(AND(distance!AF5&lt;25,distance!AF5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AF5&lt;80,distance!AF5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AG5">
-        <f>IF(AND(distance!AG5&lt;25,distance!AG5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AG5&lt;80,distance!AG5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AH5">
-        <f>IF(AND(distance!AH5&lt;25,distance!AH5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AH5&lt;80,distance!AH5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AI5">
-        <f>IF(AND(distance!AI5&lt;25,distance!AI5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AI5&lt;80,distance!AI5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AJ5">
-        <f>IF(AND(distance!AJ5&lt;25,distance!AJ5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AJ5&lt;80,distance!AJ5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AK5">
-        <f>IF(AND(distance!AK5&lt;25,distance!AK5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AK5&lt;80,distance!AK5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AL5">
-        <f>IF(AND(distance!AL5&lt;25,distance!AL5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AL5&lt;80,distance!AL5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AM5">
-        <f>IF(AND(distance!AM5&lt;25,distance!AM5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AM5&lt;80,distance!AM5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AN5">
-        <f>IF(AND(distance!AN5&lt;25,distance!AN5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AN5&lt;80,distance!AN5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AO5">
-        <f>IF(AND(distance!AO5&lt;25,distance!AO5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AO5&lt;80,distance!AO5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AP5">
-        <f>IF(AND(distance!AP5&lt;25,distance!AP5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AP5&lt;80,distance!AP5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AQ5">
-        <f>IF(AND(distance!AQ5&lt;25,distance!AQ5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AQ5&lt;80,distance!AQ5&gt;=0),1,0)</f>
         <v>0</v>
       </c>
       <c r="AR5">
-        <f>IF(AND(distance!AR5&lt;25,distance!AR5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AR5&lt;80,distance!AR5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AS5">
-        <f>IF(AND(distance!AS5&lt;25,distance!AS5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AS5&lt;80,distance!AS5&gt;=0),1,0)</f>
         <v>0</v>
       </c>
       <c r="AT5">
-        <f>IF(AND(distance!AT5&lt;25,distance!AT5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AT5&lt;80,distance!AT5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AU5">
-        <f>IF(AND(distance!AU5&lt;25,distance!AU5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AU5&lt;80,distance!AU5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AV5">
-        <f>IF(AND(distance!AV5&lt;25,distance!AV5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AV5&lt;80,distance!AV5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AW5">
-        <f>IF(AND(distance!AW5&lt;25,distance!AW5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AW5&lt;80,distance!AW5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AX5">
-        <f>IF(AND(distance!AX5&lt;25,distance!AX5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AX5&lt;80,distance!AX5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AY5">
-        <f>IF(AND(distance!AY5&lt;25,distance!AY5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AY5&lt;80,distance!AY5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="AZ5">
-        <f>IF(AND(distance!AZ5&lt;25,distance!AZ5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!AZ5&lt;80,distance!AZ5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BA5">
-        <f>IF(AND(distance!BA5&lt;25,distance!BA5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BA5&lt;80,distance!BA5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BB5">
-        <f>IF(AND(distance!BB5&lt;25,distance!BB5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BB5&lt;80,distance!BB5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BC5">
-        <f>IF(AND(distance!BC5&lt;25,distance!BC5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BC5&lt;80,distance!BC5&gt;=0),1,0)</f>
         <v>0</v>
       </c>
       <c r="BD5">
-        <f>IF(AND(distance!BD5&lt;25,distance!BD5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BD5&lt;80,distance!BD5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BE5">
-        <f>IF(AND(distance!BE5&lt;25,distance!BE5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BE5&lt;80,distance!BE5&gt;=0),1,0)</f>
         <v>0</v>
       </c>
       <c r="BF5">
-        <f>IF(AND(distance!BF5&lt;25,distance!BF5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BF5&lt;80,distance!BF5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BG5">
-        <f>IF(AND(distance!BG5&lt;25,distance!BG5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BG5&lt;80,distance!BG5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BH5">
-        <f>IF(AND(distance!BH5&lt;25,distance!BH5&gt;=0),1,0)</f>
+        <f>IF(AND(distance!BH5&lt;80,distance!BH5&gt;=0),1,0)</f>
         <v>1</v>
       </c>
       <c r="BI5">
-        <f>IF(AND(distance!BI5&lt;25,distance!BI5&gt;=0),1,0)</f>
-        <v>0</v>
-      </c>
+        <f>IF(AND(distance!BI5&lt;80,distance!BI5&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f>IF(AND(distance!B6&lt;80,distance!B6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>IF(AND(distance!C6&lt;80,distance!C6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>IF(AND(distance!D6&lt;80,distance!D6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>IF(AND(distance!E6&lt;80,distance!E6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>IF(AND(distance!F6&lt;80,distance!F6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f>IF(AND(distance!G6&lt;80,distance!G6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>IF(AND(distance!H6&lt;80,distance!H6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>IF(AND(distance!I6&lt;80,distance!I6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>IF(AND(distance!J6&lt;80,distance!J6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f>IF(AND(distance!K6&lt;80,distance!K6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f>IF(AND(distance!L6&lt;80,distance!L6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <f>IF(AND(distance!M6&lt;80,distance!M6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f>IF(AND(distance!N6&lt;80,distance!N6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <f>IF(AND(distance!O6&lt;80,distance!O6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <f>IF(AND(distance!P6&lt;80,distance!P6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <f>IF(AND(distance!Q6&lt;80,distance!Q6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <f>IF(AND(distance!R6&lt;80,distance!R6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <f>IF(AND(distance!S6&lt;80,distance!S6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <f>IF(AND(distance!T6&lt;80,distance!T6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <f>IF(AND(distance!U6&lt;80,distance!U6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <f>IF(AND(distance!V6&lt;80,distance!V6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <f>IF(AND(distance!W6&lt;80,distance!W6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <f>IF(AND(distance!X6&lt;80,distance!X6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <f>IF(AND(distance!Y6&lt;80,distance!Y6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <f>IF(AND(distance!Z6&lt;80,distance!Z6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <f>IF(AND(distance!AA6&lt;80,distance!AA6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <f>IF(AND(distance!AB6&lt;80,distance!AB6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <f>IF(AND(distance!AC6&lt;80,distance!AC6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <f>IF(AND(distance!AD6&lt;80,distance!AD6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <f>IF(AND(distance!AE6&lt;80,distance!AE6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <f>IF(AND(distance!AF6&lt;80,distance!AF6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <f>IF(AND(distance!AG6&lt;80,distance!AG6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <f>IF(AND(distance!AH6&lt;80,distance!AH6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <f>IF(AND(distance!AI6&lt;80,distance!AI6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <f>IF(AND(distance!AJ6&lt;80,distance!AJ6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <f>IF(AND(distance!AK6&lt;80,distance!AK6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <f>IF(AND(distance!AL6&lt;80,distance!AL6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM6">
+        <f>IF(AND(distance!AM6&lt;80,distance!AM6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN6">
+        <f>IF(AND(distance!AN6&lt;80,distance!AN6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO6">
+        <f>IF(AND(distance!AO6&lt;80,distance!AO6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AP6">
+        <f>IF(AND(distance!AP6&lt;80,distance!AP6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ6">
+        <f>IF(AND(distance!AQ6&lt;80,distance!AQ6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <f>IF(AND(distance!AR6&lt;80,distance!AR6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AS6">
+        <f>IF(AND(distance!AS6&lt;80,distance!AS6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <f>IF(AND(distance!AT6&lt;80,distance!AT6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <f>IF(AND(distance!AU6&lt;80,distance!AU6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <f>IF(AND(distance!AV6&lt;80,distance!AV6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AW6">
+        <f>IF(AND(distance!AW6&lt;80,distance!AW6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AX6">
+        <f>IF(AND(distance!AX6&lt;80,distance!AX6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY6">
+        <f>IF(AND(distance!AY6&lt;80,distance!AY6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ6">
+        <f>IF(AND(distance!AZ6&lt;80,distance!AZ6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <f>IF(AND(distance!BA6&lt;80,distance!BA6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <f>IF(AND(distance!BB6&lt;80,distance!BB6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC6">
+        <f>IF(AND(distance!BC6&lt;80,distance!BC6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BD6">
+        <f>IF(AND(distance!BD6&lt;80,distance!BD6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE6">
+        <f>IF(AND(distance!BE6&lt;80,distance!BE6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <f>IF(AND(distance!BF6&lt;80,distance!BF6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG6">
+        <f>IF(AND(distance!BG6&lt;80,distance!BG6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BH6">
+        <f>IF(AND(distance!BH6&lt;80,distance!BH6&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI6">
+        <f>IF(AND(distance!BI6&lt;80,distance!BI6&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <f>IF(AND(distance!B7&lt;80,distance!B7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>IF(AND(distance!C7&lt;80,distance!C7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>IF(AND(distance!D7&lt;80,distance!D7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>IF(AND(distance!E7&lt;80,distance!E7&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>IF(AND(distance!F7&lt;80,distance!F7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f>IF(AND(distance!G7&lt;80,distance!G7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f>IF(AND(distance!H7&lt;80,distance!H7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>IF(AND(distance!I7&lt;80,distance!I7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f>IF(AND(distance!J7&lt;80,distance!J7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f>IF(AND(distance!K7&lt;80,distance!K7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f>IF(AND(distance!L7&lt;80,distance!L7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f>IF(AND(distance!M7&lt;80,distance!M7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f>IF(AND(distance!N7&lt;80,distance!N7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f>IF(AND(distance!O7&lt;80,distance!O7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <f>IF(AND(distance!P7&lt;80,distance!P7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f>IF(AND(distance!Q7&lt;80,distance!Q7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f>IF(AND(distance!R7&lt;80,distance!R7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f>IF(AND(distance!S7&lt;80,distance!S7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f>IF(AND(distance!T7&lt;80,distance!T7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <f>IF(AND(distance!U7&lt;80,distance!U7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <f>IF(AND(distance!V7&lt;80,distance!V7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7">
+        <f>IF(AND(distance!X7&lt;80,distance!X7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <f>IF(AND(distance!Y7&lt;80,distance!Y7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <f>IF(AND(distance!Z7&lt;80,distance!Z7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <f>IF(AND(distance!AA7&lt;80,distance!AA7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <f>IF(AND(distance!AB7&lt;80,distance!AB7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <f>IF(AND(distance!AC7&lt;80,distance!AC7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <f>IF(AND(distance!AD7&lt;80,distance!AD7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <f>IF(AND(distance!AE7&lt;80,distance!AE7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <f>IF(AND(distance!AF7&lt;80,distance!AF7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7">
+        <f>IF(AND(distance!AH7&lt;80,distance!AH7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <f>IF(AND(distance!AI7&lt;80,distance!AI7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <f>IF(AND(distance!AJ7&lt;80,distance!AJ7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <f>IF(AND(distance!AK7&lt;80,distance!AK7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <f>IF(AND(distance!AL7&lt;80,distance!AL7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM7">
+        <f>IF(AND(distance!AM7&lt;80,distance!AM7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN7">
+        <f>IF(AND(distance!AN7&lt;80,distance!AN7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO7">
+        <f>IF(AND(distance!AO7&lt;80,distance!AO7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AP7">
+        <f>IF(AND(distance!AP7&lt;80,distance!AP7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ7">
+        <f>IF(AND(distance!AQ7&lt;80,distance!AQ7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <f>IF(AND(distance!AR7&lt;80,distance!AR7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AS7">
+        <f>IF(AND(distance!AS7&lt;80,distance!AS7&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <f>IF(AND(distance!AT7&lt;80,distance!AT7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU7">
+        <f>IF(AND(distance!AU7&lt;80,distance!AU7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AV7">
+        <f>IF(AND(distance!AV7&lt;80,distance!AV7&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <f>IF(AND(distance!AW7&lt;80,distance!AW7&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX7">
+        <f>IF(AND(distance!AX7&lt;80,distance!AX7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY7">
+        <f>IF(AND(distance!AY7&lt;80,distance!AY7&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ7">
+        <f>IF(AND(distance!AZ7&lt;80,distance!AZ7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BA7">
+        <f>IF(AND(distance!BA7&lt;80,distance!BA7&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <f>IF(AND(distance!BB7&lt;80,distance!BB7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <f>IF(AND(distance!BC7&lt;80,distance!BC7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BD7">
+        <f>IF(AND(distance!BD7&lt;80,distance!BD7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE7">
+        <f>IF(AND(distance!BE7&lt;80,distance!BE7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BF7">
+        <f>IF(AND(distance!BF7&lt;80,distance!BF7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG7">
+        <f>IF(AND(distance!BG7&lt;80,distance!BG7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BH7">
+        <f>IF(AND(distance!BH7&lt;80,distance!BH7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI7">
+        <f>IF(AND(distance!BI7&lt;80,distance!BI7&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:61">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:61">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:61">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:61">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:61">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:61">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:61">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:61">
+      <c r="A16" s="1"/>
     </row>
     <row r="20" spans="1:43">
       <c r="B20" t="str">
@@ -3212,11 +4092,11 @@
         <v>AF</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" ref="C20:F20" si="47">C1</f>
+        <f t="shared" ref="C20" si="47">C1</f>
         <v>AF</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" ref="G20:AS20" si="48">V1</f>
+        <f t="shared" ref="V20:AQ20" si="48">V1</f>
         <v>SL</v>
       </c>
       <c r="W20" t="str">
@@ -3238,11 +4118,11 @@
         <v>(para)foveal</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" ref="C21:F21" si="49">C3</f>
+        <f t="shared" ref="C21" si="49">C3</f>
         <v>peripheral</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" ref="G21:AS21" si="50">V3</f>
+        <f t="shared" ref="V21:AQ21" si="50">V3</f>
         <v>(para)foveal</v>
       </c>
       <c r="W21" t="str">
@@ -3265,7 +4145,7 @@
       </c>
       <c r="C22">
         <f t="shared" ref="C22:AQ22" si="51">SUM(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)/COUNT(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)</f>
-        <v>0.9</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="V22">
         <f t="shared" si="51"/>
@@ -3277,11 +4157,11 @@
       </c>
       <c r="AP22">
         <f t="shared" si="51"/>
-        <v>1</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="AQ22">
         <f t="shared" si="51"/>
-        <v>0.5</v>
+        <v>0.43333333333333335</v>
       </c>
     </row>
     <row r="28" spans="1:43">
@@ -3313,7 +4193,7 @@
       </c>
       <c r="D29">
         <f>AP22</f>
-        <v>1</v>
+        <v>0.96666666666666667</v>
       </c>
     </row>
     <row r="30" spans="1:43">
@@ -3323,7 +4203,7 @@
       </c>
       <c r="B30">
         <f>C22</f>
-        <v>0.9</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="C30">
         <f>W22</f>
@@ -3331,7 +4211,7 @@
       </c>
       <c r="D30">
         <f>AQ22</f>
-        <v>0.5</v>
+        <v>0.43333333333333335</v>
       </c>
     </row>
   </sheetData>
@@ -3344,8 +4224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="P52" sqref="P52"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="U64" sqref="U64:V64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4523,13 +5403,373 @@
     <row r="6" spans="1:61">
       <c r="A6">
         <f>error!A6</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1265</v>
+      </c>
+      <c r="C6">
+        <v>2416</v>
+      </c>
+      <c r="D6">
+        <v>815</v>
+      </c>
+      <c r="E6">
+        <v>1049</v>
+      </c>
+      <c r="F6">
+        <v>965</v>
+      </c>
+      <c r="G6">
+        <v>1182</v>
+      </c>
+      <c r="H6">
+        <v>1315</v>
+      </c>
+      <c r="I6">
+        <v>2129</v>
+      </c>
+      <c r="J6">
+        <v>665</v>
+      </c>
+      <c r="K6">
+        <v>782</v>
+      </c>
+      <c r="L6">
+        <v>1786</v>
+      </c>
+      <c r="M6">
+        <v>1836</v>
+      </c>
+      <c r="N6">
+        <v>1399</v>
+      </c>
+      <c r="O6">
+        <v>1382</v>
+      </c>
+      <c r="P6">
+        <v>1015</v>
+      </c>
+      <c r="Q6">
+        <v>1115</v>
+      </c>
+      <c r="R6">
+        <v>1069</v>
+      </c>
+      <c r="S6">
+        <v>752</v>
+      </c>
+      <c r="T6">
+        <v>1365</v>
+      </c>
+      <c r="U6">
+        <v>1679</v>
+      </c>
+      <c r="V6">
+        <v>1496</v>
+      </c>
+      <c r="W6">
+        <v>928</v>
+      </c>
+      <c r="X6">
+        <v>832</v>
+      </c>
+      <c r="Y6">
+        <v>1283</v>
+      </c>
+      <c r="Z6">
+        <v>962</v>
+      </c>
+      <c r="AA6">
+        <v>1046</v>
+      </c>
+      <c r="AB6">
+        <v>842</v>
+      </c>
+      <c r="AC6">
+        <v>1701</v>
+      </c>
+      <c r="AD6">
+        <v>812</v>
+      </c>
+      <c r="AE6">
+        <v>1213</v>
+      </c>
+      <c r="AF6">
+        <v>828</v>
+      </c>
+      <c r="AG6">
+        <v>1325</v>
+      </c>
+      <c r="AH6">
+        <v>850</v>
+      </c>
+      <c r="AI6">
+        <v>1079</v>
+      </c>
+      <c r="AJ6">
+        <v>595</v>
+      </c>
+      <c r="AK6">
+        <v>1429</v>
+      </c>
+      <c r="AL6">
+        <v>846</v>
+      </c>
+      <c r="AM6">
+        <v>1496</v>
+      </c>
+      <c r="AN6">
+        <v>1108</v>
+      </c>
+      <c r="AO6">
+        <v>829</v>
+      </c>
+      <c r="AP6">
+        <v>4334</v>
+      </c>
+      <c r="AQ6">
+        <v>5005</v>
+      </c>
+      <c r="AR6">
+        <v>697</v>
+      </c>
+      <c r="AS6">
+        <v>5001</v>
+      </c>
+      <c r="AT6">
+        <v>1131</v>
+      </c>
+      <c r="AU6">
+        <v>5001</v>
+      </c>
+      <c r="AV6">
+        <v>1815</v>
+      </c>
+      <c r="AW6">
+        <v>2516</v>
+      </c>
+      <c r="AX6">
+        <v>798</v>
+      </c>
+      <c r="AY6">
+        <v>5001</v>
+      </c>
+      <c r="AZ6">
+        <v>931</v>
+      </c>
+      <c r="BA6">
+        <v>885</v>
+      </c>
+      <c r="BB6">
+        <v>931</v>
+      </c>
+      <c r="BC6">
+        <v>5018</v>
+      </c>
+      <c r="BD6">
+        <v>730</v>
+      </c>
+      <c r="BE6">
+        <v>5001</v>
+      </c>
+      <c r="BF6">
+        <v>1198</v>
+      </c>
+      <c r="BG6">
+        <v>5001</v>
+      </c>
+      <c r="BH6">
+        <v>761</v>
+      </c>
+      <c r="BI6">
+        <v>5001</v>
       </c>
     </row>
     <row r="7" spans="1:61">
       <c r="A7">
         <f>error!A7</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>998</v>
+      </c>
+      <c r="C7">
+        <v>1215</v>
+      </c>
+      <c r="D7">
+        <v>1449</v>
+      </c>
+      <c r="E7">
+        <v>5002</v>
+      </c>
+      <c r="F7">
+        <v>1265</v>
+      </c>
+      <c r="G7">
+        <v>2099</v>
+      </c>
+      <c r="H7">
+        <v>1299</v>
+      </c>
+      <c r="I7">
+        <v>3121</v>
+      </c>
+      <c r="J7">
+        <v>2316</v>
+      </c>
+      <c r="K7">
+        <v>1152</v>
+      </c>
+      <c r="L7">
+        <v>1119</v>
+      </c>
+      <c r="M7">
+        <v>1165</v>
+      </c>
+      <c r="N7">
+        <v>1065</v>
+      </c>
+      <c r="O7">
+        <v>2433</v>
+      </c>
+      <c r="P7">
+        <v>1182</v>
+      </c>
+      <c r="Q7">
+        <v>1069</v>
+      </c>
+      <c r="R7">
+        <v>1065</v>
+      </c>
+      <c r="S7">
+        <v>1799</v>
+      </c>
+      <c r="T7">
+        <v>2253</v>
+      </c>
+      <c r="U7">
+        <v>4138</v>
+      </c>
+      <c r="V7">
+        <v>2647</v>
+      </c>
+      <c r="W7">
+        <v>928</v>
+      </c>
+      <c r="X7">
+        <v>946</v>
+      </c>
+      <c r="Y7">
+        <v>1780</v>
+      </c>
+      <c r="Z7">
+        <v>1226</v>
+      </c>
+      <c r="AA7">
+        <v>1730</v>
+      </c>
+      <c r="AB7">
+        <v>1646</v>
+      </c>
+      <c r="AC7">
+        <v>1429</v>
+      </c>
+      <c r="AD7">
+        <v>1730</v>
+      </c>
+      <c r="AE7">
+        <v>946</v>
+      </c>
+      <c r="AF7">
+        <v>1813</v>
+      </c>
+      <c r="AG7">
+        <v>662</v>
+      </c>
+      <c r="AH7">
+        <v>1179</v>
+      </c>
+      <c r="AI7">
+        <v>1196</v>
+      </c>
+      <c r="AJ7">
+        <v>1630</v>
+      </c>
+      <c r="AK7">
+        <v>1463</v>
+      </c>
+      <c r="AL7">
+        <v>846</v>
+      </c>
+      <c r="AM7">
+        <v>1429</v>
+      </c>
+      <c r="AN7">
+        <v>1580</v>
+      </c>
+      <c r="AO7">
+        <v>1216</v>
+      </c>
+      <c r="AP7">
+        <v>651</v>
+      </c>
+      <c r="AQ7">
+        <v>869</v>
+      </c>
+      <c r="AR7">
+        <v>935</v>
+      </c>
+      <c r="AS7">
+        <v>5001</v>
+      </c>
+      <c r="AT7">
+        <v>1348</v>
+      </c>
+      <c r="AU7">
+        <v>2616</v>
+      </c>
+      <c r="AV7">
+        <v>264</v>
+      </c>
+      <c r="AW7">
+        <v>5000</v>
+      </c>
+      <c r="AX7">
+        <v>1198</v>
+      </c>
+      <c r="AY7">
+        <v>5001</v>
+      </c>
+      <c r="AZ7">
+        <v>881</v>
+      </c>
+      <c r="BA7">
+        <v>5001</v>
+      </c>
+      <c r="BB7">
+        <v>4147</v>
+      </c>
+      <c r="BC7">
+        <v>977</v>
+      </c>
+      <c r="BD7">
+        <v>764</v>
+      </c>
+      <c r="BE7">
+        <v>781</v>
+      </c>
+      <c r="BF7">
+        <v>1398</v>
+      </c>
+      <c r="BG7">
+        <v>5006</v>
+      </c>
+      <c r="BH7">
+        <v>814</v>
+      </c>
+      <c r="BI7">
+        <v>1631</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -4803,7 +6043,7 @@
     </row>
     <row r="28" spans="1:61">
       <c r="A28">
-        <f t="shared" ref="A28:F30" si="1">A2</f>
+        <f t="shared" ref="A28:A29" si="1">A2</f>
         <v>0</v>
       </c>
       <c r="B28" t="str">
@@ -5542,50 +6782,2216 @@
     <row r="31" spans="1:61">
       <c r="A31">
         <f t="shared" ref="A31:A36" si="4">A6</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <f>IF(error!B6=1,time!B6,"")</f>
+        <v>1265</v>
+      </c>
+      <c r="C31">
+        <f>IF(error!C6=1,time!C6,"")</f>
+        <v>2416</v>
+      </c>
+      <c r="D31">
+        <f>IF(error!D6=1,time!D6,"")</f>
+        <v>815</v>
+      </c>
+      <c r="E31">
+        <f>IF(error!E6=1,time!E6,"")</f>
+        <v>1049</v>
+      </c>
+      <c r="F31">
+        <f>IF(error!F6=1,time!F6,"")</f>
+        <v>965</v>
+      </c>
+      <c r="G31">
+        <f>IF(error!G6=1,time!G6,"")</f>
+        <v>1182</v>
+      </c>
+      <c r="H31">
+        <f>IF(error!H6=1,time!H6,"")</f>
+        <v>1315</v>
+      </c>
+      <c r="I31">
+        <f>IF(error!I6=1,time!I6,"")</f>
+        <v>2129</v>
+      </c>
+      <c r="J31">
+        <f>IF(error!J6=1,time!J6,"")</f>
+        <v>665</v>
+      </c>
+      <c r="K31">
+        <f>IF(error!K6=1,time!K6,"")</f>
+        <v>782</v>
+      </c>
+      <c r="L31">
+        <f>IF(error!L6=1,time!L6,"")</f>
+        <v>1786</v>
+      </c>
+      <c r="M31">
+        <f>IF(error!M6=1,time!M6,"")</f>
+        <v>1836</v>
+      </c>
+      <c r="N31">
+        <f>IF(error!N6=1,time!N6,"")</f>
+        <v>1399</v>
+      </c>
+      <c r="O31">
+        <f>IF(error!O6=1,time!O6,"")</f>
+        <v>1382</v>
+      </c>
+      <c r="P31">
+        <f>IF(error!P6=1,time!P6,"")</f>
+        <v>1015</v>
+      </c>
+      <c r="Q31">
+        <f>IF(error!Q6=1,time!Q6,"")</f>
+        <v>1115</v>
+      </c>
+      <c r="R31">
+        <f>IF(error!R6=1,time!R6,"")</f>
+        <v>1069</v>
+      </c>
+      <c r="S31">
+        <f>IF(error!S6=1,time!S6,"")</f>
+        <v>752</v>
+      </c>
+      <c r="T31">
+        <f>IF(error!T6=1,time!T6,"")</f>
+        <v>1365</v>
+      </c>
+      <c r="U31">
+        <f>IF(error!U6=1,time!U6,"")</f>
+        <v>1679</v>
+      </c>
+      <c r="V31">
+        <f>IF(error!V6=1,time!V6,"")</f>
+        <v>1496</v>
+      </c>
+      <c r="W31">
+        <f>IF(error!W6=1,time!W6,"")</f>
+        <v>928</v>
+      </c>
+      <c r="X31">
+        <f>IF(error!X6=1,time!X6,"")</f>
+        <v>832</v>
+      </c>
+      <c r="Y31">
+        <f>IF(error!Y6=1,time!Y6,"")</f>
+        <v>1283</v>
+      </c>
+      <c r="Z31">
+        <f>IF(error!Z6=1,time!Z6,"")</f>
+        <v>962</v>
+      </c>
+      <c r="AA31">
+        <f>IF(error!AA6=1,time!AA6,"")</f>
+        <v>1046</v>
+      </c>
+      <c r="AB31">
+        <f>IF(error!AB6=1,time!AB6,"")</f>
+        <v>842</v>
+      </c>
+      <c r="AC31">
+        <f>IF(error!AC6=1,time!AC6,"")</f>
+        <v>1701</v>
+      </c>
+      <c r="AD31">
+        <f>IF(error!AD6=1,time!AD6,"")</f>
+        <v>812</v>
+      </c>
+      <c r="AE31">
+        <f>IF(error!AE6=1,time!AE6,"")</f>
+        <v>1213</v>
+      </c>
+      <c r="AF31">
+        <f>IF(error!AF6=1,time!AF6,"")</f>
+        <v>828</v>
+      </c>
+      <c r="AG31">
+        <f>IF(error!AG6=1,time!AG6,"")</f>
+        <v>1325</v>
+      </c>
+      <c r="AH31">
+        <f>IF(error!AH6=1,time!AH6,"")</f>
+        <v>850</v>
+      </c>
+      <c r="AI31">
+        <f>IF(error!AI6=1,time!AI6,"")</f>
+        <v>1079</v>
+      </c>
+      <c r="AJ31">
+        <f>IF(error!AJ6=1,time!AJ6,"")</f>
+        <v>595</v>
+      </c>
+      <c r="AK31">
+        <f>IF(error!AK6=1,time!AK6,"")</f>
+        <v>1429</v>
+      </c>
+      <c r="AL31">
+        <f>IF(error!AL6=1,time!AL6,"")</f>
+        <v>846</v>
+      </c>
+      <c r="AM31">
+        <f>IF(error!AM6=1,time!AM6,"")</f>
+        <v>1496</v>
+      </c>
+      <c r="AN31">
+        <f>IF(error!AN6=1,time!AN6,"")</f>
+        <v>1108</v>
+      </c>
+      <c r="AO31">
+        <f>IF(error!AO6=1,time!AO6,"")</f>
+        <v>829</v>
+      </c>
+      <c r="AP31">
+        <f>IF(error!AP6=1,time!AP6,"")</f>
+        <v>4334</v>
+      </c>
+      <c r="AQ31" t="str">
+        <f>IF(error!AQ6=1,time!AQ6,"")</f>
+        <v/>
+      </c>
+      <c r="AR31">
+        <f>IF(error!AR6=1,time!AR6,"")</f>
+        <v>697</v>
+      </c>
+      <c r="AS31" t="str">
+        <f>IF(error!AS6=1,time!AS6,"")</f>
+        <v/>
+      </c>
+      <c r="AT31">
+        <f>IF(error!AT6=1,time!AT6,"")</f>
+        <v>1131</v>
+      </c>
+      <c r="AU31" t="str">
+        <f>IF(error!AU6=1,time!AU6,"")</f>
+        <v/>
+      </c>
+      <c r="AV31">
+        <f>IF(error!AV6=1,time!AV6,"")</f>
+        <v>1815</v>
+      </c>
+      <c r="AW31">
+        <f>IF(error!AW6=1,time!AW6,"")</f>
+        <v>2516</v>
+      </c>
+      <c r="AX31">
+        <f>IF(error!AX6=1,time!AX6,"")</f>
+        <v>798</v>
+      </c>
+      <c r="AY31" t="str">
+        <f>IF(error!AY6=1,time!AY6,"")</f>
+        <v/>
+      </c>
+      <c r="AZ31">
+        <f>IF(error!AZ6=1,time!AZ6,"")</f>
+        <v>931</v>
+      </c>
+      <c r="BA31">
+        <f>IF(error!BA6=1,time!BA6,"")</f>
+        <v>885</v>
+      </c>
+      <c r="BB31">
+        <f>IF(error!BB6=1,time!BB6,"")</f>
+        <v>931</v>
+      </c>
+      <c r="BC31" t="str">
+        <f>IF(error!BC6=1,time!BC6,"")</f>
+        <v/>
+      </c>
+      <c r="BD31">
+        <f>IF(error!BD6=1,time!BD6,"")</f>
+        <v>730</v>
+      </c>
+      <c r="BE31" t="str">
+        <f>IF(error!BE6=1,time!BE6,"")</f>
+        <v/>
+      </c>
+      <c r="BF31">
+        <f>IF(error!BF6=1,time!BF6,"")</f>
+        <v>1198</v>
+      </c>
+      <c r="BG31" t="str">
+        <f>IF(error!BG6=1,time!BG6,"")</f>
+        <v/>
+      </c>
+      <c r="BH31">
+        <f>IF(error!BH6=1,time!BH6,"")</f>
+        <v>761</v>
+      </c>
+      <c r="BI31" t="str">
+        <f>IF(error!BI6=1,time!BI6,"")</f>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:61">
       <c r="A32">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <f>IF(error!B7=1,time!B7,"")</f>
+        <v>998</v>
+      </c>
+      <c r="C32">
+        <f>IF(error!C7=1,time!C7,"")</f>
+        <v>1215</v>
+      </c>
+      <c r="D32">
+        <f>IF(error!D7=1,time!D7,"")</f>
+        <v>1449</v>
+      </c>
+      <c r="E32" t="str">
+        <f>IF(error!E7=1,time!E7,"")</f>
+        <v/>
+      </c>
+      <c r="F32">
+        <f>IF(error!F7=1,time!F7,"")</f>
+        <v>1265</v>
+      </c>
+      <c r="G32">
+        <f>IF(error!G7=1,time!G7,"")</f>
+        <v>2099</v>
+      </c>
+      <c r="H32">
+        <f>IF(error!H7=1,time!H7,"")</f>
+        <v>1299</v>
+      </c>
+      <c r="I32">
+        <f>IF(error!I7=1,time!I7,"")</f>
+        <v>3121</v>
+      </c>
+      <c r="J32">
+        <f>IF(error!J7=1,time!J7,"")</f>
+        <v>2316</v>
+      </c>
+      <c r="K32">
+        <f>IF(error!K7=1,time!K7,"")</f>
+        <v>1152</v>
+      </c>
+      <c r="L32">
+        <f>IF(error!L7=1,time!L7,"")</f>
+        <v>1119</v>
+      </c>
+      <c r="M32">
+        <f>IF(error!M7=1,time!M7,"")</f>
+        <v>1165</v>
+      </c>
+      <c r="N32">
+        <f>IF(error!N7=1,time!N7,"")</f>
+        <v>1065</v>
+      </c>
+      <c r="O32">
+        <f>IF(error!O7=1,time!O7,"")</f>
+        <v>2433</v>
+      </c>
+      <c r="P32">
+        <f>IF(error!P7=1,time!P7,"")</f>
+        <v>1182</v>
+      </c>
+      <c r="Q32">
+        <f>IF(error!Q7=1,time!Q7,"")</f>
+        <v>1069</v>
+      </c>
+      <c r="R32">
+        <f>IF(error!R7=1,time!R7,"")</f>
+        <v>1065</v>
+      </c>
+      <c r="S32">
+        <f>IF(error!S7=1,time!S7,"")</f>
+        <v>1799</v>
+      </c>
+      <c r="T32">
+        <f>IF(error!T7=1,time!T7,"")</f>
+        <v>2253</v>
+      </c>
+      <c r="U32">
+        <f>IF(error!U7=1,time!U7,"")</f>
+        <v>4138</v>
+      </c>
+      <c r="V32">
+        <f>IF(error!V7=1,time!V7,"")</f>
+        <v>2647</v>
+      </c>
+      <c r="W32" t="str">
+        <f>IF(error!W7=1,time!W7,"")</f>
+        <v/>
+      </c>
+      <c r="X32">
+        <f>IF(error!X7=1,time!X7,"")</f>
+        <v>946</v>
+      </c>
+      <c r="Y32">
+        <f>IF(error!Y7=1,time!Y7,"")</f>
+        <v>1780</v>
+      </c>
+      <c r="Z32">
+        <f>IF(error!Z7=1,time!Z7,"")</f>
+        <v>1226</v>
+      </c>
+      <c r="AA32">
+        <f>IF(error!AA7=1,time!AA7,"")</f>
+        <v>1730</v>
+      </c>
+      <c r="AB32">
+        <f>IF(error!AB7=1,time!AB7,"")</f>
+        <v>1646</v>
+      </c>
+      <c r="AC32">
+        <f>IF(error!AC7=1,time!AC7,"")</f>
+        <v>1429</v>
+      </c>
+      <c r="AD32">
+        <f>IF(error!AD7=1,time!AD7,"")</f>
+        <v>1730</v>
+      </c>
+      <c r="AE32">
+        <f>IF(error!AE7=1,time!AE7,"")</f>
+        <v>946</v>
+      </c>
+      <c r="AF32">
+        <f>IF(error!AF7=1,time!AF7,"")</f>
+        <v>1813</v>
+      </c>
+      <c r="AG32" t="str">
+        <f>IF(error!AG7=1,time!AG7,"")</f>
+        <v/>
+      </c>
+      <c r="AH32">
+        <f>IF(error!AH7=1,time!AH7,"")</f>
+        <v>1179</v>
+      </c>
+      <c r="AI32">
+        <f>IF(error!AI7=1,time!AI7,"")</f>
+        <v>1196</v>
+      </c>
+      <c r="AJ32">
+        <f>IF(error!AJ7=1,time!AJ7,"")</f>
+        <v>1630</v>
+      </c>
+      <c r="AK32">
+        <f>IF(error!AK7=1,time!AK7,"")</f>
+        <v>1463</v>
+      </c>
+      <c r="AL32">
+        <f>IF(error!AL7=1,time!AL7,"")</f>
+        <v>846</v>
+      </c>
+      <c r="AM32">
+        <f>IF(error!AM7=1,time!AM7,"")</f>
+        <v>1429</v>
+      </c>
+      <c r="AN32">
+        <f>IF(error!AN7=1,time!AN7,"")</f>
+        <v>1580</v>
+      </c>
+      <c r="AO32">
+        <f>IF(error!AO7=1,time!AO7,"")</f>
+        <v>1216</v>
+      </c>
+      <c r="AP32">
+        <f>IF(error!AP7=1,time!AP7,"")</f>
+        <v>651</v>
+      </c>
+      <c r="AQ32">
+        <f>IF(error!AQ7=1,time!AQ7,"")</f>
+        <v>869</v>
+      </c>
+      <c r="AR32">
+        <f>IF(error!AR7=1,time!AR7,"")</f>
+        <v>935</v>
+      </c>
+      <c r="AS32" t="str">
+        <f>IF(error!AS7=1,time!AS7,"")</f>
+        <v/>
+      </c>
+      <c r="AT32">
+        <f>IF(error!AT7=1,time!AT7,"")</f>
+        <v>1348</v>
+      </c>
+      <c r="AU32">
+        <f>IF(error!AU7=1,time!AU7,"")</f>
+        <v>2616</v>
+      </c>
+      <c r="AV32" t="str">
+        <f>IF(error!AV7=1,time!AV7,"")</f>
+        <v/>
+      </c>
+      <c r="AW32" t="str">
+        <f>IF(error!AW7=1,time!AW7,"")</f>
+        <v/>
+      </c>
+      <c r="AX32">
+        <f>IF(error!AX7=1,time!AX7,"")</f>
+        <v>1198</v>
+      </c>
+      <c r="AY32" t="str">
+        <f>IF(error!AY7=1,time!AY7,"")</f>
+        <v/>
+      </c>
+      <c r="AZ32">
+        <f>IF(error!AZ7=1,time!AZ7,"")</f>
+        <v>881</v>
+      </c>
+      <c r="BA32" t="str">
+        <f>IF(error!BA7=1,time!BA7,"")</f>
+        <v/>
+      </c>
+      <c r="BB32">
+        <f>IF(error!BB7=1,time!BB7,"")</f>
+        <v>4147</v>
+      </c>
+      <c r="BC32">
+        <f>IF(error!BC7=1,time!BC7,"")</f>
+        <v>977</v>
+      </c>
+      <c r="BD32">
+        <f>IF(error!BD7=1,time!BD7,"")</f>
+        <v>764</v>
+      </c>
+      <c r="BE32">
+        <f>IF(error!BE7=1,time!BE7,"")</f>
+        <v>781</v>
+      </c>
+      <c r="BF32">
+        <f>IF(error!BF7=1,time!BF7,"")</f>
+        <v>1398</v>
+      </c>
+      <c r="BG32">
+        <f>IF(error!BG7=1,time!BG7,"")</f>
+        <v>5006</v>
+      </c>
+      <c r="BH32">
+        <f>IF(error!BH7=1,time!BH7,"")</f>
+        <v>814</v>
+      </c>
+      <c r="BI32">
+        <f>IF(error!BI7=1,time!BI7,"")</f>
+        <v>1631</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:61">
       <c r="A33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="B33" t="str">
+        <f>IF(error!B8=1,time!B8,"")</f>
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <f>IF(error!C8=1,time!C8,"")</f>
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <f>IF(error!D8=1,time!D8,"")</f>
+        <v/>
+      </c>
+      <c r="E33" t="str">
+        <f>IF(error!E8=1,time!E8,"")</f>
+        <v/>
+      </c>
+      <c r="F33" t="str">
+        <f>IF(error!F8=1,time!F8,"")</f>
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <f>IF(error!G8=1,time!G8,"")</f>
+        <v/>
+      </c>
+      <c r="H33" t="str">
+        <f>IF(error!H8=1,time!H8,"")</f>
+        <v/>
+      </c>
+      <c r="I33" t="str">
+        <f>IF(error!I8=1,time!I8,"")</f>
+        <v/>
+      </c>
+      <c r="J33" t="str">
+        <f>IF(error!J8=1,time!J8,"")</f>
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <f>IF(error!K8=1,time!K8,"")</f>
+        <v/>
+      </c>
+      <c r="L33" t="str">
+        <f>IF(error!L8=1,time!L8,"")</f>
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <f>IF(error!M8=1,time!M8,"")</f>
+        <v/>
+      </c>
+      <c r="N33" t="str">
+        <f>IF(error!N8=1,time!N8,"")</f>
+        <v/>
+      </c>
+      <c r="O33" t="str">
+        <f>IF(error!O8=1,time!O8,"")</f>
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <f>IF(error!P8=1,time!P8,"")</f>
+        <v/>
+      </c>
+      <c r="Q33" t="str">
+        <f>IF(error!Q8=1,time!Q8,"")</f>
+        <v/>
+      </c>
+      <c r="R33" t="str">
+        <f>IF(error!R8=1,time!R8,"")</f>
+        <v/>
+      </c>
+      <c r="S33" t="str">
+        <f>IF(error!S8=1,time!S8,"")</f>
+        <v/>
+      </c>
+      <c r="T33" t="str">
+        <f>IF(error!T8=1,time!T8,"")</f>
+        <v/>
+      </c>
+      <c r="U33" t="str">
+        <f>IF(error!U8=1,time!U8,"")</f>
+        <v/>
+      </c>
+      <c r="V33" t="str">
+        <f>IF(error!V8=1,time!V8,"")</f>
+        <v/>
+      </c>
+      <c r="W33" t="str">
+        <f>IF(error!W8=1,time!W8,"")</f>
+        <v/>
+      </c>
+      <c r="X33" t="str">
+        <f>IF(error!X8=1,time!X8,"")</f>
+        <v/>
+      </c>
+      <c r="Y33" t="str">
+        <f>IF(error!Y8=1,time!Y8,"")</f>
+        <v/>
+      </c>
+      <c r="Z33" t="str">
+        <f>IF(error!Z8=1,time!Z8,"")</f>
+        <v/>
+      </c>
+      <c r="AA33" t="str">
+        <f>IF(error!AA8=1,time!AA8,"")</f>
+        <v/>
+      </c>
+      <c r="AB33" t="str">
+        <f>IF(error!AB8=1,time!AB8,"")</f>
+        <v/>
+      </c>
+      <c r="AC33" t="str">
+        <f>IF(error!AC8=1,time!AC8,"")</f>
+        <v/>
+      </c>
+      <c r="AD33" t="str">
+        <f>IF(error!AD8=1,time!AD8,"")</f>
+        <v/>
+      </c>
+      <c r="AE33" t="str">
+        <f>IF(error!AE8=1,time!AE8,"")</f>
+        <v/>
+      </c>
+      <c r="AF33" t="str">
+        <f>IF(error!AF8=1,time!AF8,"")</f>
+        <v/>
+      </c>
+      <c r="AG33" t="str">
+        <f>IF(error!AG8=1,time!AG8,"")</f>
+        <v/>
+      </c>
+      <c r="AH33" t="str">
+        <f>IF(error!AH8=1,time!AH8,"")</f>
+        <v/>
+      </c>
+      <c r="AI33" t="str">
+        <f>IF(error!AI8=1,time!AI8,"")</f>
+        <v/>
+      </c>
+      <c r="AJ33" t="str">
+        <f>IF(error!AJ8=1,time!AJ8,"")</f>
+        <v/>
+      </c>
+      <c r="AK33" t="str">
+        <f>IF(error!AK8=1,time!AK8,"")</f>
+        <v/>
+      </c>
+      <c r="AL33" t="str">
+        <f>IF(error!AL8=1,time!AL8,"")</f>
+        <v/>
+      </c>
+      <c r="AM33" t="str">
+        <f>IF(error!AM8=1,time!AM8,"")</f>
+        <v/>
+      </c>
+      <c r="AN33" t="str">
+        <f>IF(error!AN8=1,time!AN8,"")</f>
+        <v/>
+      </c>
+      <c r="AO33" t="str">
+        <f>IF(error!AO8=1,time!AO8,"")</f>
+        <v/>
+      </c>
+      <c r="AP33" t="str">
+        <f>IF(error!AP8=1,time!AP8,"")</f>
+        <v/>
+      </c>
+      <c r="AQ33" t="str">
+        <f>IF(error!AQ8=1,time!AQ8,"")</f>
+        <v/>
+      </c>
+      <c r="AR33" t="str">
+        <f>IF(error!AR8=1,time!AR8,"")</f>
+        <v/>
+      </c>
+      <c r="AS33" t="str">
+        <f>IF(error!AS8=1,time!AS8,"")</f>
+        <v/>
+      </c>
+      <c r="AT33" t="str">
+        <f>IF(error!AT8=1,time!AT8,"")</f>
+        <v/>
+      </c>
+      <c r="AU33" t="str">
+        <f>IF(error!AU8=1,time!AU8,"")</f>
+        <v/>
+      </c>
+      <c r="AV33" t="str">
+        <f>IF(error!AV8=1,time!AV8,"")</f>
+        <v/>
+      </c>
+      <c r="AW33" t="str">
+        <f>IF(error!AW8=1,time!AW8,"")</f>
+        <v/>
+      </c>
+      <c r="AX33" t="str">
+        <f>IF(error!AX8=1,time!AX8,"")</f>
+        <v/>
+      </c>
+      <c r="AY33" t="str">
+        <f>IF(error!AY8=1,time!AY8,"")</f>
+        <v/>
+      </c>
+      <c r="AZ33" t="str">
+        <f>IF(error!AZ8=1,time!AZ8,"")</f>
+        <v/>
+      </c>
+      <c r="BA33" t="str">
+        <f>IF(error!BA8=1,time!BA8,"")</f>
+        <v/>
+      </c>
+      <c r="BB33" t="str">
+        <f>IF(error!BB8=1,time!BB8,"")</f>
+        <v/>
+      </c>
+      <c r="BC33" t="str">
+        <f>IF(error!BC8=1,time!BC8,"")</f>
+        <v/>
+      </c>
+      <c r="BD33" t="str">
+        <f>IF(error!BD8=1,time!BD8,"")</f>
+        <v/>
+      </c>
+      <c r="BE33" t="str">
+        <f>IF(error!BE8=1,time!BE8,"")</f>
+        <v/>
+      </c>
+      <c r="BF33" t="str">
+        <f>IF(error!BF8=1,time!BF8,"")</f>
+        <v/>
+      </c>
+      <c r="BG33" t="str">
+        <f>IF(error!BG8=1,time!BG8,"")</f>
+        <v/>
+      </c>
+      <c r="BH33" t="str">
+        <f>IF(error!BH8=1,time!BH8,"")</f>
+        <v/>
+      </c>
+      <c r="BI33" t="str">
+        <f>IF(error!BI8=1,time!BI8,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:61">
       <c r="A34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="B34" t="str">
+        <f>IF(error!B9=1,time!B9,"")</f>
+        <v/>
+      </c>
+      <c r="C34" t="str">
+        <f>IF(error!C9=1,time!C9,"")</f>
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <f>IF(error!D9=1,time!D9,"")</f>
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <f>IF(error!E9=1,time!E9,"")</f>
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <f>IF(error!F9=1,time!F9,"")</f>
+        <v/>
+      </c>
+      <c r="G34" t="str">
+        <f>IF(error!G9=1,time!G9,"")</f>
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <f>IF(error!H9=1,time!H9,"")</f>
+        <v/>
+      </c>
+      <c r="I34" t="str">
+        <f>IF(error!I9=1,time!I9,"")</f>
+        <v/>
+      </c>
+      <c r="J34" t="str">
+        <f>IF(error!J9=1,time!J9,"")</f>
+        <v/>
+      </c>
+      <c r="K34" t="str">
+        <f>IF(error!K9=1,time!K9,"")</f>
+        <v/>
+      </c>
+      <c r="L34" t="str">
+        <f>IF(error!L9=1,time!L9,"")</f>
+        <v/>
+      </c>
+      <c r="M34" t="str">
+        <f>IF(error!M9=1,time!M9,"")</f>
+        <v/>
+      </c>
+      <c r="N34" t="str">
+        <f>IF(error!N9=1,time!N9,"")</f>
+        <v/>
+      </c>
+      <c r="O34" t="str">
+        <f>IF(error!O9=1,time!O9,"")</f>
+        <v/>
+      </c>
+      <c r="P34" t="str">
+        <f>IF(error!P9=1,time!P9,"")</f>
+        <v/>
+      </c>
+      <c r="Q34" t="str">
+        <f>IF(error!Q9=1,time!Q9,"")</f>
+        <v/>
+      </c>
+      <c r="R34" t="str">
+        <f>IF(error!R9=1,time!R9,"")</f>
+        <v/>
+      </c>
+      <c r="S34" t="str">
+        <f>IF(error!S9=1,time!S9,"")</f>
+        <v/>
+      </c>
+      <c r="T34" t="str">
+        <f>IF(error!T9=1,time!T9,"")</f>
+        <v/>
+      </c>
+      <c r="U34" t="str">
+        <f>IF(error!U9=1,time!U9,"")</f>
+        <v/>
+      </c>
+      <c r="V34" t="str">
+        <f>IF(error!V9=1,time!V9,"")</f>
+        <v/>
+      </c>
+      <c r="W34" t="str">
+        <f>IF(error!W9=1,time!W9,"")</f>
+        <v/>
+      </c>
+      <c r="X34" t="str">
+        <f>IF(error!X9=1,time!X9,"")</f>
+        <v/>
+      </c>
+      <c r="Y34" t="str">
+        <f>IF(error!Y9=1,time!Y9,"")</f>
+        <v/>
+      </c>
+      <c r="Z34" t="str">
+        <f>IF(error!Z9=1,time!Z9,"")</f>
+        <v/>
+      </c>
+      <c r="AA34" t="str">
+        <f>IF(error!AA9=1,time!AA9,"")</f>
+        <v/>
+      </c>
+      <c r="AB34" t="str">
+        <f>IF(error!AB9=1,time!AB9,"")</f>
+        <v/>
+      </c>
+      <c r="AC34" t="str">
+        <f>IF(error!AC9=1,time!AC9,"")</f>
+        <v/>
+      </c>
+      <c r="AD34" t="str">
+        <f>IF(error!AD9=1,time!AD9,"")</f>
+        <v/>
+      </c>
+      <c r="AE34" t="str">
+        <f>IF(error!AE9=1,time!AE9,"")</f>
+        <v/>
+      </c>
+      <c r="AF34" t="str">
+        <f>IF(error!AF9=1,time!AF9,"")</f>
+        <v/>
+      </c>
+      <c r="AG34" t="str">
+        <f>IF(error!AG9=1,time!AG9,"")</f>
+        <v/>
+      </c>
+      <c r="AH34" t="str">
+        <f>IF(error!AH9=1,time!AH9,"")</f>
+        <v/>
+      </c>
+      <c r="AI34" t="str">
+        <f>IF(error!AI9=1,time!AI9,"")</f>
+        <v/>
+      </c>
+      <c r="AJ34" t="str">
+        <f>IF(error!AJ9=1,time!AJ9,"")</f>
+        <v/>
+      </c>
+      <c r="AK34" t="str">
+        <f>IF(error!AK9=1,time!AK9,"")</f>
+        <v/>
+      </c>
+      <c r="AL34" t="str">
+        <f>IF(error!AL9=1,time!AL9,"")</f>
+        <v/>
+      </c>
+      <c r="AM34" t="str">
+        <f>IF(error!AM9=1,time!AM9,"")</f>
+        <v/>
+      </c>
+      <c r="AN34" t="str">
+        <f>IF(error!AN9=1,time!AN9,"")</f>
+        <v/>
+      </c>
+      <c r="AO34" t="str">
+        <f>IF(error!AO9=1,time!AO9,"")</f>
+        <v/>
+      </c>
+      <c r="AP34" t="str">
+        <f>IF(error!AP9=1,time!AP9,"")</f>
+        <v/>
+      </c>
+      <c r="AQ34" t="str">
+        <f>IF(error!AQ9=1,time!AQ9,"")</f>
+        <v/>
+      </c>
+      <c r="AR34" t="str">
+        <f>IF(error!AR9=1,time!AR9,"")</f>
+        <v/>
+      </c>
+      <c r="AS34" t="str">
+        <f>IF(error!AS9=1,time!AS9,"")</f>
+        <v/>
+      </c>
+      <c r="AT34" t="str">
+        <f>IF(error!AT9=1,time!AT9,"")</f>
+        <v/>
+      </c>
+      <c r="AU34" t="str">
+        <f>IF(error!AU9=1,time!AU9,"")</f>
+        <v/>
+      </c>
+      <c r="AV34" t="str">
+        <f>IF(error!AV9=1,time!AV9,"")</f>
+        <v/>
+      </c>
+      <c r="AW34" t="str">
+        <f>IF(error!AW9=1,time!AW9,"")</f>
+        <v/>
+      </c>
+      <c r="AX34" t="str">
+        <f>IF(error!AX9=1,time!AX9,"")</f>
+        <v/>
+      </c>
+      <c r="AY34" t="str">
+        <f>IF(error!AY9=1,time!AY9,"")</f>
+        <v/>
+      </c>
+      <c r="AZ34" t="str">
+        <f>IF(error!AZ9=1,time!AZ9,"")</f>
+        <v/>
+      </c>
+      <c r="BA34" t="str">
+        <f>IF(error!BA9=1,time!BA9,"")</f>
+        <v/>
+      </c>
+      <c r="BB34" t="str">
+        <f>IF(error!BB9=1,time!BB9,"")</f>
+        <v/>
+      </c>
+      <c r="BC34" t="str">
+        <f>IF(error!BC9=1,time!BC9,"")</f>
+        <v/>
+      </c>
+      <c r="BD34" t="str">
+        <f>IF(error!BD9=1,time!BD9,"")</f>
+        <v/>
+      </c>
+      <c r="BE34" t="str">
+        <f>IF(error!BE9=1,time!BE9,"")</f>
+        <v/>
+      </c>
+      <c r="BF34" t="str">
+        <f>IF(error!BF9=1,time!BF9,"")</f>
+        <v/>
+      </c>
+      <c r="BG34" t="str">
+        <f>IF(error!BG9=1,time!BG9,"")</f>
+        <v/>
+      </c>
+      <c r="BH34" t="str">
+        <f>IF(error!BH9=1,time!BH9,"")</f>
+        <v/>
+      </c>
+      <c r="BI34" t="str">
+        <f>IF(error!BI9=1,time!BI9,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:61">
       <c r="A35">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="B35" t="str">
+        <f>IF(error!B10=1,time!B10,"")</f>
+        <v/>
+      </c>
+      <c r="C35" t="str">
+        <f>IF(error!C10=1,time!C10,"")</f>
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(error!D10=1,time!D10,"")</f>
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <f>IF(error!E10=1,time!E10,"")</f>
+        <v/>
+      </c>
+      <c r="F35" t="str">
+        <f>IF(error!F10=1,time!F10,"")</f>
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <f>IF(error!G10=1,time!G10,"")</f>
+        <v/>
+      </c>
+      <c r="H35" t="str">
+        <f>IF(error!H10=1,time!H10,"")</f>
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <f>IF(error!I10=1,time!I10,"")</f>
+        <v/>
+      </c>
+      <c r="J35" t="str">
+        <f>IF(error!J10=1,time!J10,"")</f>
+        <v/>
+      </c>
+      <c r="K35" t="str">
+        <f>IF(error!K10=1,time!K10,"")</f>
+        <v/>
+      </c>
+      <c r="L35" t="str">
+        <f>IF(error!L10=1,time!L10,"")</f>
+        <v/>
+      </c>
+      <c r="M35" t="str">
+        <f>IF(error!M10=1,time!M10,"")</f>
+        <v/>
+      </c>
+      <c r="N35" t="str">
+        <f>IF(error!N10=1,time!N10,"")</f>
+        <v/>
+      </c>
+      <c r="O35" t="str">
+        <f>IF(error!O10=1,time!O10,"")</f>
+        <v/>
+      </c>
+      <c r="P35" t="str">
+        <f>IF(error!P10=1,time!P10,"")</f>
+        <v/>
+      </c>
+      <c r="Q35" t="str">
+        <f>IF(error!Q10=1,time!Q10,"")</f>
+        <v/>
+      </c>
+      <c r="R35" t="str">
+        <f>IF(error!R10=1,time!R10,"")</f>
+        <v/>
+      </c>
+      <c r="S35" t="str">
+        <f>IF(error!S10=1,time!S10,"")</f>
+        <v/>
+      </c>
+      <c r="T35" t="str">
+        <f>IF(error!T10=1,time!T10,"")</f>
+        <v/>
+      </c>
+      <c r="U35" t="str">
+        <f>IF(error!U10=1,time!U10,"")</f>
+        <v/>
+      </c>
+      <c r="V35" t="str">
+        <f>IF(error!V10=1,time!V10,"")</f>
+        <v/>
+      </c>
+      <c r="W35" t="str">
+        <f>IF(error!W10=1,time!W10,"")</f>
+        <v/>
+      </c>
+      <c r="X35" t="str">
+        <f>IF(error!X10=1,time!X10,"")</f>
+        <v/>
+      </c>
+      <c r="Y35" t="str">
+        <f>IF(error!Y10=1,time!Y10,"")</f>
+        <v/>
+      </c>
+      <c r="Z35" t="str">
+        <f>IF(error!Z10=1,time!Z10,"")</f>
+        <v/>
+      </c>
+      <c r="AA35" t="str">
+        <f>IF(error!AA10=1,time!AA10,"")</f>
+        <v/>
+      </c>
+      <c r="AB35" t="str">
+        <f>IF(error!AB10=1,time!AB10,"")</f>
+        <v/>
+      </c>
+      <c r="AC35" t="str">
+        <f>IF(error!AC10=1,time!AC10,"")</f>
+        <v/>
+      </c>
+      <c r="AD35" t="str">
+        <f>IF(error!AD10=1,time!AD10,"")</f>
+        <v/>
+      </c>
+      <c r="AE35" t="str">
+        <f>IF(error!AE10=1,time!AE10,"")</f>
+        <v/>
+      </c>
+      <c r="AF35" t="str">
+        <f>IF(error!AF10=1,time!AF10,"")</f>
+        <v/>
+      </c>
+      <c r="AG35" t="str">
+        <f>IF(error!AG10=1,time!AG10,"")</f>
+        <v/>
+      </c>
+      <c r="AH35" t="str">
+        <f>IF(error!AH10=1,time!AH10,"")</f>
+        <v/>
+      </c>
+      <c r="AI35" t="str">
+        <f>IF(error!AI10=1,time!AI10,"")</f>
+        <v/>
+      </c>
+      <c r="AJ35" t="str">
+        <f>IF(error!AJ10=1,time!AJ10,"")</f>
+        <v/>
+      </c>
+      <c r="AK35" t="str">
+        <f>IF(error!AK10=1,time!AK10,"")</f>
+        <v/>
+      </c>
+      <c r="AL35" t="str">
+        <f>IF(error!AL10=1,time!AL10,"")</f>
+        <v/>
+      </c>
+      <c r="AM35" t="str">
+        <f>IF(error!AM10=1,time!AM10,"")</f>
+        <v/>
+      </c>
+      <c r="AN35" t="str">
+        <f>IF(error!AN10=1,time!AN10,"")</f>
+        <v/>
+      </c>
+      <c r="AO35" t="str">
+        <f>IF(error!AO10=1,time!AO10,"")</f>
+        <v/>
+      </c>
+      <c r="AP35" t="str">
+        <f>IF(error!AP10=1,time!AP10,"")</f>
+        <v/>
+      </c>
+      <c r="AQ35" t="str">
+        <f>IF(error!AQ10=1,time!AQ10,"")</f>
+        <v/>
+      </c>
+      <c r="AR35" t="str">
+        <f>IF(error!AR10=1,time!AR10,"")</f>
+        <v/>
+      </c>
+      <c r="AS35" t="str">
+        <f>IF(error!AS10=1,time!AS10,"")</f>
+        <v/>
+      </c>
+      <c r="AT35" t="str">
+        <f>IF(error!AT10=1,time!AT10,"")</f>
+        <v/>
+      </c>
+      <c r="AU35" t="str">
+        <f>IF(error!AU10=1,time!AU10,"")</f>
+        <v/>
+      </c>
+      <c r="AV35" t="str">
+        <f>IF(error!AV10=1,time!AV10,"")</f>
+        <v/>
+      </c>
+      <c r="AW35" t="str">
+        <f>IF(error!AW10=1,time!AW10,"")</f>
+        <v/>
+      </c>
+      <c r="AX35" t="str">
+        <f>IF(error!AX10=1,time!AX10,"")</f>
+        <v/>
+      </c>
+      <c r="AY35" t="str">
+        <f>IF(error!AY10=1,time!AY10,"")</f>
+        <v/>
+      </c>
+      <c r="AZ35" t="str">
+        <f>IF(error!AZ10=1,time!AZ10,"")</f>
+        <v/>
+      </c>
+      <c r="BA35" t="str">
+        <f>IF(error!BA10=1,time!BA10,"")</f>
+        <v/>
+      </c>
+      <c r="BB35" t="str">
+        <f>IF(error!BB10=1,time!BB10,"")</f>
+        <v/>
+      </c>
+      <c r="BC35" t="str">
+        <f>IF(error!BC10=1,time!BC10,"")</f>
+        <v/>
+      </c>
+      <c r="BD35" t="str">
+        <f>IF(error!BD10=1,time!BD10,"")</f>
+        <v/>
+      </c>
+      <c r="BE35" t="str">
+        <f>IF(error!BE10=1,time!BE10,"")</f>
+        <v/>
+      </c>
+      <c r="BF35" t="str">
+        <f>IF(error!BF10=1,time!BF10,"")</f>
+        <v/>
+      </c>
+      <c r="BG35" t="str">
+        <f>IF(error!BG10=1,time!BG10,"")</f>
+        <v/>
+      </c>
+      <c r="BH35" t="str">
+        <f>IF(error!BH10=1,time!BH10,"")</f>
+        <v/>
+      </c>
+      <c r="BI35" t="str">
+        <f>IF(error!BI10=1,time!BI10,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:61">
       <c r="A36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="B36" t="str">
+        <f>IF(error!B11=1,time!B11,"")</f>
+        <v/>
+      </c>
+      <c r="C36" t="str">
+        <f>IF(error!C11=1,time!C11,"")</f>
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <f>IF(error!D11=1,time!D11,"")</f>
+        <v/>
+      </c>
+      <c r="E36" t="str">
+        <f>IF(error!E11=1,time!E11,"")</f>
+        <v/>
+      </c>
+      <c r="F36" t="str">
+        <f>IF(error!F11=1,time!F11,"")</f>
+        <v/>
+      </c>
+      <c r="G36" t="str">
+        <f>IF(error!G11=1,time!G11,"")</f>
+        <v/>
+      </c>
+      <c r="H36" t="str">
+        <f>IF(error!H11=1,time!H11,"")</f>
+        <v/>
+      </c>
+      <c r="I36" t="str">
+        <f>IF(error!I11=1,time!I11,"")</f>
+        <v/>
+      </c>
+      <c r="J36" t="str">
+        <f>IF(error!J11=1,time!J11,"")</f>
+        <v/>
+      </c>
+      <c r="K36" t="str">
+        <f>IF(error!K11=1,time!K11,"")</f>
+        <v/>
+      </c>
+      <c r="L36" t="str">
+        <f>IF(error!L11=1,time!L11,"")</f>
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <f>IF(error!M11=1,time!M11,"")</f>
+        <v/>
+      </c>
+      <c r="N36" t="str">
+        <f>IF(error!N11=1,time!N11,"")</f>
+        <v/>
+      </c>
+      <c r="O36" t="str">
+        <f>IF(error!O11=1,time!O11,"")</f>
+        <v/>
+      </c>
+      <c r="P36" t="str">
+        <f>IF(error!P11=1,time!P11,"")</f>
+        <v/>
+      </c>
+      <c r="Q36" t="str">
+        <f>IF(error!Q11=1,time!Q11,"")</f>
+        <v/>
+      </c>
+      <c r="R36" t="str">
+        <f>IF(error!R11=1,time!R11,"")</f>
+        <v/>
+      </c>
+      <c r="S36" t="str">
+        <f>IF(error!S11=1,time!S11,"")</f>
+        <v/>
+      </c>
+      <c r="T36" t="str">
+        <f>IF(error!T11=1,time!T11,"")</f>
+        <v/>
+      </c>
+      <c r="U36" t="str">
+        <f>IF(error!U11=1,time!U11,"")</f>
+        <v/>
+      </c>
+      <c r="V36" t="str">
+        <f>IF(error!V11=1,time!V11,"")</f>
+        <v/>
+      </c>
+      <c r="W36" t="str">
+        <f>IF(error!W11=1,time!W11,"")</f>
+        <v/>
+      </c>
+      <c r="X36" t="str">
+        <f>IF(error!X11=1,time!X11,"")</f>
+        <v/>
+      </c>
+      <c r="Y36" t="str">
+        <f>IF(error!Y11=1,time!Y11,"")</f>
+        <v/>
+      </c>
+      <c r="Z36" t="str">
+        <f>IF(error!Z11=1,time!Z11,"")</f>
+        <v/>
+      </c>
+      <c r="AA36" t="str">
+        <f>IF(error!AA11=1,time!AA11,"")</f>
+        <v/>
+      </c>
+      <c r="AB36" t="str">
+        <f>IF(error!AB11=1,time!AB11,"")</f>
+        <v/>
+      </c>
+      <c r="AC36" t="str">
+        <f>IF(error!AC11=1,time!AC11,"")</f>
+        <v/>
+      </c>
+      <c r="AD36" t="str">
+        <f>IF(error!AD11=1,time!AD11,"")</f>
+        <v/>
+      </c>
+      <c r="AE36" t="str">
+        <f>IF(error!AE11=1,time!AE11,"")</f>
+        <v/>
+      </c>
+      <c r="AF36" t="str">
+        <f>IF(error!AF11=1,time!AF11,"")</f>
+        <v/>
+      </c>
+      <c r="AG36" t="str">
+        <f>IF(error!AG11=1,time!AG11,"")</f>
+        <v/>
+      </c>
+      <c r="AH36" t="str">
+        <f>IF(error!AH11=1,time!AH11,"")</f>
+        <v/>
+      </c>
+      <c r="AI36" t="str">
+        <f>IF(error!AI11=1,time!AI11,"")</f>
+        <v/>
+      </c>
+      <c r="AJ36" t="str">
+        <f>IF(error!AJ11=1,time!AJ11,"")</f>
+        <v/>
+      </c>
+      <c r="AK36" t="str">
+        <f>IF(error!AK11=1,time!AK11,"")</f>
+        <v/>
+      </c>
+      <c r="AL36" t="str">
+        <f>IF(error!AL11=1,time!AL11,"")</f>
+        <v/>
+      </c>
+      <c r="AM36" t="str">
+        <f>IF(error!AM11=1,time!AM11,"")</f>
+        <v/>
+      </c>
+      <c r="AN36" t="str">
+        <f>IF(error!AN11=1,time!AN11,"")</f>
+        <v/>
+      </c>
+      <c r="AO36" t="str">
+        <f>IF(error!AO11=1,time!AO11,"")</f>
+        <v/>
+      </c>
+      <c r="AP36" t="str">
+        <f>IF(error!AP11=1,time!AP11,"")</f>
+        <v/>
+      </c>
+      <c r="AQ36" t="str">
+        <f>IF(error!AQ11=1,time!AQ11,"")</f>
+        <v/>
+      </c>
+      <c r="AR36" t="str">
+        <f>IF(error!AR11=1,time!AR11,"")</f>
+        <v/>
+      </c>
+      <c r="AS36" t="str">
+        <f>IF(error!AS11=1,time!AS11,"")</f>
+        <v/>
+      </c>
+      <c r="AT36" t="str">
+        <f>IF(error!AT11=1,time!AT11,"")</f>
+        <v/>
+      </c>
+      <c r="AU36" t="str">
+        <f>IF(error!AU11=1,time!AU11,"")</f>
+        <v/>
+      </c>
+      <c r="AV36" t="str">
+        <f>IF(error!AV11=1,time!AV11,"")</f>
+        <v/>
+      </c>
+      <c r="AW36" t="str">
+        <f>IF(error!AW11=1,time!AW11,"")</f>
+        <v/>
+      </c>
+      <c r="AX36" t="str">
+        <f>IF(error!AX11=1,time!AX11,"")</f>
+        <v/>
+      </c>
+      <c r="AY36" t="str">
+        <f>IF(error!AY11=1,time!AY11,"")</f>
+        <v/>
+      </c>
+      <c r="AZ36" t="str">
+        <f>IF(error!AZ11=1,time!AZ11,"")</f>
+        <v/>
+      </c>
+      <c r="BA36" t="str">
+        <f>IF(error!BA11=1,time!BA11,"")</f>
+        <v/>
+      </c>
+      <c r="BB36" t="str">
+        <f>IF(error!BB11=1,time!BB11,"")</f>
+        <v/>
+      </c>
+      <c r="BC36" t="str">
+        <f>IF(error!BC11=1,time!BC11,"")</f>
+        <v/>
+      </c>
+      <c r="BD36" t="str">
+        <f>IF(error!BD11=1,time!BD11,"")</f>
+        <v/>
+      </c>
+      <c r="BE36" t="str">
+        <f>IF(error!BE11=1,time!BE11,"")</f>
+        <v/>
+      </c>
+      <c r="BF36" t="str">
+        <f>IF(error!BF11=1,time!BF11,"")</f>
+        <v/>
+      </c>
+      <c r="BG36" t="str">
+        <f>IF(error!BG11=1,time!BG11,"")</f>
+        <v/>
+      </c>
+      <c r="BH36" t="str">
+        <f>IF(error!BH11=1,time!BH11,"")</f>
+        <v/>
+      </c>
+      <c r="BI36" t="str">
+        <f>IF(error!BI11=1,time!BI11,"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="45" spans="1:43">
+    <row r="37" spans="1:61">
+      <c r="B37" t="str">
+        <f>IF(error!B12=1,time!B12,"")</f>
+        <v/>
+      </c>
+      <c r="C37" t="str">
+        <f>IF(error!C12=1,time!C12,"")</f>
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <f>IF(error!D12=1,time!D12,"")</f>
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <f>IF(error!E12=1,time!E12,"")</f>
+        <v/>
+      </c>
+      <c r="F37" t="str">
+        <f>IF(error!F12=1,time!F12,"")</f>
+        <v/>
+      </c>
+      <c r="G37" t="str">
+        <f>IF(error!G12=1,time!G12,"")</f>
+        <v/>
+      </c>
+      <c r="H37" t="str">
+        <f>IF(error!H12=1,time!H12,"")</f>
+        <v/>
+      </c>
+      <c r="I37" t="str">
+        <f>IF(error!I12=1,time!I12,"")</f>
+        <v/>
+      </c>
+      <c r="J37" t="str">
+        <f>IF(error!J12=1,time!J12,"")</f>
+        <v/>
+      </c>
+      <c r="K37" t="str">
+        <f>IF(error!K12=1,time!K12,"")</f>
+        <v/>
+      </c>
+      <c r="L37" t="str">
+        <f>IF(error!L12=1,time!L12,"")</f>
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <f>IF(error!M12=1,time!M12,"")</f>
+        <v/>
+      </c>
+      <c r="N37" t="str">
+        <f>IF(error!N12=1,time!N12,"")</f>
+        <v/>
+      </c>
+      <c r="O37" t="str">
+        <f>IF(error!O12=1,time!O12,"")</f>
+        <v/>
+      </c>
+      <c r="P37" t="str">
+        <f>IF(error!P12=1,time!P12,"")</f>
+        <v/>
+      </c>
+      <c r="Q37" t="str">
+        <f>IF(error!Q12=1,time!Q12,"")</f>
+        <v/>
+      </c>
+      <c r="R37" t="str">
+        <f>IF(error!R12=1,time!R12,"")</f>
+        <v/>
+      </c>
+      <c r="S37" t="str">
+        <f>IF(error!S12=1,time!S12,"")</f>
+        <v/>
+      </c>
+      <c r="T37" t="str">
+        <f>IF(error!T12=1,time!T12,"")</f>
+        <v/>
+      </c>
+      <c r="U37" t="str">
+        <f>IF(error!U12=1,time!U12,"")</f>
+        <v/>
+      </c>
+      <c r="V37" t="str">
+        <f>IF(error!V12=1,time!V12,"")</f>
+        <v/>
+      </c>
+      <c r="W37" t="str">
+        <f>IF(error!W12=1,time!W12,"")</f>
+        <v/>
+      </c>
+      <c r="X37" t="str">
+        <f>IF(error!X12=1,time!X12,"")</f>
+        <v/>
+      </c>
+      <c r="Y37" t="str">
+        <f>IF(error!Y12=1,time!Y12,"")</f>
+        <v/>
+      </c>
+      <c r="Z37" t="str">
+        <f>IF(error!Z12=1,time!Z12,"")</f>
+        <v/>
+      </c>
+      <c r="AA37" t="str">
+        <f>IF(error!AA12=1,time!AA12,"")</f>
+        <v/>
+      </c>
+      <c r="AB37" t="str">
+        <f>IF(error!AB12=1,time!AB12,"")</f>
+        <v/>
+      </c>
+      <c r="AC37" t="str">
+        <f>IF(error!AC12=1,time!AC12,"")</f>
+        <v/>
+      </c>
+      <c r="AD37" t="str">
+        <f>IF(error!AD12=1,time!AD12,"")</f>
+        <v/>
+      </c>
+      <c r="AE37" t="str">
+        <f>IF(error!AE12=1,time!AE12,"")</f>
+        <v/>
+      </c>
+      <c r="AF37" t="str">
+        <f>IF(error!AF12=1,time!AF12,"")</f>
+        <v/>
+      </c>
+      <c r="AG37" t="str">
+        <f>IF(error!AG12=1,time!AG12,"")</f>
+        <v/>
+      </c>
+      <c r="AH37" t="str">
+        <f>IF(error!AH12=1,time!AH12,"")</f>
+        <v/>
+      </c>
+      <c r="AI37" t="str">
+        <f>IF(error!AI12=1,time!AI12,"")</f>
+        <v/>
+      </c>
+      <c r="AJ37" t="str">
+        <f>IF(error!AJ12=1,time!AJ12,"")</f>
+        <v/>
+      </c>
+      <c r="AK37" t="str">
+        <f>IF(error!AK12=1,time!AK12,"")</f>
+        <v/>
+      </c>
+      <c r="AL37" t="str">
+        <f>IF(error!AL12=1,time!AL12,"")</f>
+        <v/>
+      </c>
+      <c r="AM37" t="str">
+        <f>IF(error!AM12=1,time!AM12,"")</f>
+        <v/>
+      </c>
+      <c r="AN37" t="str">
+        <f>IF(error!AN12=1,time!AN12,"")</f>
+        <v/>
+      </c>
+      <c r="AO37" t="str">
+        <f>IF(error!AO12=1,time!AO12,"")</f>
+        <v/>
+      </c>
+      <c r="AP37" t="str">
+        <f>IF(error!AP12=1,time!AP12,"")</f>
+        <v/>
+      </c>
+      <c r="AQ37" t="str">
+        <f>IF(error!AQ12=1,time!AQ12,"")</f>
+        <v/>
+      </c>
+      <c r="AR37" t="str">
+        <f>IF(error!AR12=1,time!AR12,"")</f>
+        <v/>
+      </c>
+      <c r="AS37" t="str">
+        <f>IF(error!AS12=1,time!AS12,"")</f>
+        <v/>
+      </c>
+      <c r="AT37" t="str">
+        <f>IF(error!AT12=1,time!AT12,"")</f>
+        <v/>
+      </c>
+      <c r="AU37" t="str">
+        <f>IF(error!AU12=1,time!AU12,"")</f>
+        <v/>
+      </c>
+      <c r="AV37" t="str">
+        <f>IF(error!AV12=1,time!AV12,"")</f>
+        <v/>
+      </c>
+      <c r="AW37" t="str">
+        <f>IF(error!AW12=1,time!AW12,"")</f>
+        <v/>
+      </c>
+      <c r="AX37" t="str">
+        <f>IF(error!AX12=1,time!AX12,"")</f>
+        <v/>
+      </c>
+      <c r="AY37" t="str">
+        <f>IF(error!AY12=1,time!AY12,"")</f>
+        <v/>
+      </c>
+      <c r="AZ37" t="str">
+        <f>IF(error!AZ12=1,time!AZ12,"")</f>
+        <v/>
+      </c>
+      <c r="BA37" t="str">
+        <f>IF(error!BA12=1,time!BA12,"")</f>
+        <v/>
+      </c>
+      <c r="BB37" t="str">
+        <f>IF(error!BB12=1,time!BB12,"")</f>
+        <v/>
+      </c>
+      <c r="BC37" t="str">
+        <f>IF(error!BC12=1,time!BC12,"")</f>
+        <v/>
+      </c>
+      <c r="BD37" t="str">
+        <f>IF(error!BD12=1,time!BD12,"")</f>
+        <v/>
+      </c>
+      <c r="BE37" t="str">
+        <f>IF(error!BE12=1,time!BE12,"")</f>
+        <v/>
+      </c>
+      <c r="BF37" t="str">
+        <f>IF(error!BF12=1,time!BF12,"")</f>
+        <v/>
+      </c>
+      <c r="BG37" t="str">
+        <f>IF(error!BG12=1,time!BG12,"")</f>
+        <v/>
+      </c>
+      <c r="BH37" t="str">
+        <f>IF(error!BH12=1,time!BH12,"")</f>
+        <v/>
+      </c>
+      <c r="BI37" t="str">
+        <f>IF(error!BI12=1,time!BI12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:61">
+      <c r="B38" t="str">
+        <f>IF(error!B13=1,time!B13,"")</f>
+        <v/>
+      </c>
+      <c r="C38" t="str">
+        <f>IF(error!C13=1,time!C13,"")</f>
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <f>IF(error!D13=1,time!D13,"")</f>
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <f>IF(error!E13=1,time!E13,"")</f>
+        <v/>
+      </c>
+      <c r="F38" t="str">
+        <f>IF(error!F13=1,time!F13,"")</f>
+        <v/>
+      </c>
+      <c r="G38" t="str">
+        <f>IF(error!G13=1,time!G13,"")</f>
+        <v/>
+      </c>
+      <c r="H38" t="str">
+        <f>IF(error!H13=1,time!H13,"")</f>
+        <v/>
+      </c>
+      <c r="I38" t="str">
+        <f>IF(error!I13=1,time!I13,"")</f>
+        <v/>
+      </c>
+      <c r="J38" t="str">
+        <f>IF(error!J13=1,time!J13,"")</f>
+        <v/>
+      </c>
+      <c r="K38" t="str">
+        <f>IF(error!K13=1,time!K13,"")</f>
+        <v/>
+      </c>
+      <c r="L38" t="str">
+        <f>IF(error!L13=1,time!L13,"")</f>
+        <v/>
+      </c>
+      <c r="M38" t="str">
+        <f>IF(error!M13=1,time!M13,"")</f>
+        <v/>
+      </c>
+      <c r="N38" t="str">
+        <f>IF(error!N13=1,time!N13,"")</f>
+        <v/>
+      </c>
+      <c r="O38" t="str">
+        <f>IF(error!O13=1,time!O13,"")</f>
+        <v/>
+      </c>
+      <c r="P38" t="str">
+        <f>IF(error!P13=1,time!P13,"")</f>
+        <v/>
+      </c>
+      <c r="Q38" t="str">
+        <f>IF(error!Q13=1,time!Q13,"")</f>
+        <v/>
+      </c>
+      <c r="R38" t="str">
+        <f>IF(error!R13=1,time!R13,"")</f>
+        <v/>
+      </c>
+      <c r="S38" t="str">
+        <f>IF(error!S13=1,time!S13,"")</f>
+        <v/>
+      </c>
+      <c r="T38" t="str">
+        <f>IF(error!T13=1,time!T13,"")</f>
+        <v/>
+      </c>
+      <c r="U38" t="str">
+        <f>IF(error!U13=1,time!U13,"")</f>
+        <v/>
+      </c>
+      <c r="V38" t="str">
+        <f>IF(error!V13=1,time!V13,"")</f>
+        <v/>
+      </c>
+      <c r="W38" t="str">
+        <f>IF(error!W13=1,time!W13,"")</f>
+        <v/>
+      </c>
+      <c r="X38" t="str">
+        <f>IF(error!X13=1,time!X13,"")</f>
+        <v/>
+      </c>
+      <c r="Y38" t="str">
+        <f>IF(error!Y13=1,time!Y13,"")</f>
+        <v/>
+      </c>
+      <c r="Z38" t="str">
+        <f>IF(error!Z13=1,time!Z13,"")</f>
+        <v/>
+      </c>
+      <c r="AA38" t="str">
+        <f>IF(error!AA13=1,time!AA13,"")</f>
+        <v/>
+      </c>
+      <c r="AB38" t="str">
+        <f>IF(error!AB13=1,time!AB13,"")</f>
+        <v/>
+      </c>
+      <c r="AC38" t="str">
+        <f>IF(error!AC13=1,time!AC13,"")</f>
+        <v/>
+      </c>
+      <c r="AD38" t="str">
+        <f>IF(error!AD13=1,time!AD13,"")</f>
+        <v/>
+      </c>
+      <c r="AE38" t="str">
+        <f>IF(error!AE13=1,time!AE13,"")</f>
+        <v/>
+      </c>
+      <c r="AF38" t="str">
+        <f>IF(error!AF13=1,time!AF13,"")</f>
+        <v/>
+      </c>
+      <c r="AG38" t="str">
+        <f>IF(error!AG13=1,time!AG13,"")</f>
+        <v/>
+      </c>
+      <c r="AH38" t="str">
+        <f>IF(error!AH13=1,time!AH13,"")</f>
+        <v/>
+      </c>
+      <c r="AI38" t="str">
+        <f>IF(error!AI13=1,time!AI13,"")</f>
+        <v/>
+      </c>
+      <c r="AJ38" t="str">
+        <f>IF(error!AJ13=1,time!AJ13,"")</f>
+        <v/>
+      </c>
+      <c r="AK38" t="str">
+        <f>IF(error!AK13=1,time!AK13,"")</f>
+        <v/>
+      </c>
+      <c r="AL38" t="str">
+        <f>IF(error!AL13=1,time!AL13,"")</f>
+        <v/>
+      </c>
+      <c r="AM38" t="str">
+        <f>IF(error!AM13=1,time!AM13,"")</f>
+        <v/>
+      </c>
+      <c r="AN38" t="str">
+        <f>IF(error!AN13=1,time!AN13,"")</f>
+        <v/>
+      </c>
+      <c r="AO38" t="str">
+        <f>IF(error!AO13=1,time!AO13,"")</f>
+        <v/>
+      </c>
+      <c r="AP38" t="str">
+        <f>IF(error!AP13=1,time!AP13,"")</f>
+        <v/>
+      </c>
+      <c r="AQ38" t="str">
+        <f>IF(error!AQ13=1,time!AQ13,"")</f>
+        <v/>
+      </c>
+      <c r="AR38" t="str">
+        <f>IF(error!AR13=1,time!AR13,"")</f>
+        <v/>
+      </c>
+      <c r="AS38" t="str">
+        <f>IF(error!AS13=1,time!AS13,"")</f>
+        <v/>
+      </c>
+      <c r="AT38" t="str">
+        <f>IF(error!AT13=1,time!AT13,"")</f>
+        <v/>
+      </c>
+      <c r="AU38" t="str">
+        <f>IF(error!AU13=1,time!AU13,"")</f>
+        <v/>
+      </c>
+      <c r="AV38" t="str">
+        <f>IF(error!AV13=1,time!AV13,"")</f>
+        <v/>
+      </c>
+      <c r="AW38" t="str">
+        <f>IF(error!AW13=1,time!AW13,"")</f>
+        <v/>
+      </c>
+      <c r="AX38" t="str">
+        <f>IF(error!AX13=1,time!AX13,"")</f>
+        <v/>
+      </c>
+      <c r="AY38" t="str">
+        <f>IF(error!AY13=1,time!AY13,"")</f>
+        <v/>
+      </c>
+      <c r="AZ38" t="str">
+        <f>IF(error!AZ13=1,time!AZ13,"")</f>
+        <v/>
+      </c>
+      <c r="BA38" t="str">
+        <f>IF(error!BA13=1,time!BA13,"")</f>
+        <v/>
+      </c>
+      <c r="BB38" t="str">
+        <f>IF(error!BB13=1,time!BB13,"")</f>
+        <v/>
+      </c>
+      <c r="BC38" t="str">
+        <f>IF(error!BC13=1,time!BC13,"")</f>
+        <v/>
+      </c>
+      <c r="BD38" t="str">
+        <f>IF(error!BD13=1,time!BD13,"")</f>
+        <v/>
+      </c>
+      <c r="BE38" t="str">
+        <f>IF(error!BE13=1,time!BE13,"")</f>
+        <v/>
+      </c>
+      <c r="BF38" t="str">
+        <f>IF(error!BF13=1,time!BF13,"")</f>
+        <v/>
+      </c>
+      <c r="BG38" t="str">
+        <f>IF(error!BG13=1,time!BG13,"")</f>
+        <v/>
+      </c>
+      <c r="BH38" t="str">
+        <f>IF(error!BH13=1,time!BH13,"")</f>
+        <v/>
+      </c>
+      <c r="BI38" t="str">
+        <f>IF(error!BI13=1,time!BI13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:61">
+      <c r="B39" t="str">
+        <f>IF(error!B14=1,time!B14,"")</f>
+        <v/>
+      </c>
+      <c r="C39" t="str">
+        <f>IF(error!C14=1,time!C14,"")</f>
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <f>IF(error!D14=1,time!D14,"")</f>
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <f>IF(error!E14=1,time!E14,"")</f>
+        <v/>
+      </c>
+      <c r="F39" t="str">
+        <f>IF(error!F14=1,time!F14,"")</f>
+        <v/>
+      </c>
+      <c r="G39" t="str">
+        <f>IF(error!G14=1,time!G14,"")</f>
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <f>IF(error!H14=1,time!H14,"")</f>
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <f>IF(error!I14=1,time!I14,"")</f>
+        <v/>
+      </c>
+      <c r="J39" t="str">
+        <f>IF(error!J14=1,time!J14,"")</f>
+        <v/>
+      </c>
+      <c r="K39" t="str">
+        <f>IF(error!K14=1,time!K14,"")</f>
+        <v/>
+      </c>
+      <c r="L39" t="str">
+        <f>IF(error!L14=1,time!L14,"")</f>
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <f>IF(error!M14=1,time!M14,"")</f>
+        <v/>
+      </c>
+      <c r="N39" t="str">
+        <f>IF(error!N14=1,time!N14,"")</f>
+        <v/>
+      </c>
+      <c r="O39" t="str">
+        <f>IF(error!O14=1,time!O14,"")</f>
+        <v/>
+      </c>
+      <c r="P39" t="str">
+        <f>IF(error!P14=1,time!P14,"")</f>
+        <v/>
+      </c>
+      <c r="Q39" t="str">
+        <f>IF(error!Q14=1,time!Q14,"")</f>
+        <v/>
+      </c>
+      <c r="R39" t="str">
+        <f>IF(error!R14=1,time!R14,"")</f>
+        <v/>
+      </c>
+      <c r="S39" t="str">
+        <f>IF(error!S14=1,time!S14,"")</f>
+        <v/>
+      </c>
+      <c r="T39" t="str">
+        <f>IF(error!T14=1,time!T14,"")</f>
+        <v/>
+      </c>
+      <c r="U39" t="str">
+        <f>IF(error!U14=1,time!U14,"")</f>
+        <v/>
+      </c>
+      <c r="V39" t="str">
+        <f>IF(error!V14=1,time!V14,"")</f>
+        <v/>
+      </c>
+      <c r="W39" t="str">
+        <f>IF(error!W14=1,time!W14,"")</f>
+        <v/>
+      </c>
+      <c r="X39" t="str">
+        <f>IF(error!X14=1,time!X14,"")</f>
+        <v/>
+      </c>
+      <c r="Y39" t="str">
+        <f>IF(error!Y14=1,time!Y14,"")</f>
+        <v/>
+      </c>
+      <c r="Z39" t="str">
+        <f>IF(error!Z14=1,time!Z14,"")</f>
+        <v/>
+      </c>
+      <c r="AA39" t="str">
+        <f>IF(error!AA14=1,time!AA14,"")</f>
+        <v/>
+      </c>
+      <c r="AB39" t="str">
+        <f>IF(error!AB14=1,time!AB14,"")</f>
+        <v/>
+      </c>
+      <c r="AC39" t="str">
+        <f>IF(error!AC14=1,time!AC14,"")</f>
+        <v/>
+      </c>
+      <c r="AD39" t="str">
+        <f>IF(error!AD14=1,time!AD14,"")</f>
+        <v/>
+      </c>
+      <c r="AE39" t="str">
+        <f>IF(error!AE14=1,time!AE14,"")</f>
+        <v/>
+      </c>
+      <c r="AF39" t="str">
+        <f>IF(error!AF14=1,time!AF14,"")</f>
+        <v/>
+      </c>
+      <c r="AG39" t="str">
+        <f>IF(error!AG14=1,time!AG14,"")</f>
+        <v/>
+      </c>
+      <c r="AH39" t="str">
+        <f>IF(error!AH14=1,time!AH14,"")</f>
+        <v/>
+      </c>
+      <c r="AI39" t="str">
+        <f>IF(error!AI14=1,time!AI14,"")</f>
+        <v/>
+      </c>
+      <c r="AJ39" t="str">
+        <f>IF(error!AJ14=1,time!AJ14,"")</f>
+        <v/>
+      </c>
+      <c r="AK39" t="str">
+        <f>IF(error!AK14=1,time!AK14,"")</f>
+        <v/>
+      </c>
+      <c r="AL39" t="str">
+        <f>IF(error!AL14=1,time!AL14,"")</f>
+        <v/>
+      </c>
+      <c r="AM39" t="str">
+        <f>IF(error!AM14=1,time!AM14,"")</f>
+        <v/>
+      </c>
+      <c r="AN39" t="str">
+        <f>IF(error!AN14=1,time!AN14,"")</f>
+        <v/>
+      </c>
+      <c r="AO39" t="str">
+        <f>IF(error!AO14=1,time!AO14,"")</f>
+        <v/>
+      </c>
+      <c r="AP39" t="str">
+        <f>IF(error!AP14=1,time!AP14,"")</f>
+        <v/>
+      </c>
+      <c r="AQ39" t="str">
+        <f>IF(error!AQ14=1,time!AQ14,"")</f>
+        <v/>
+      </c>
+      <c r="AR39" t="str">
+        <f>IF(error!AR14=1,time!AR14,"")</f>
+        <v/>
+      </c>
+      <c r="AS39" t="str">
+        <f>IF(error!AS14=1,time!AS14,"")</f>
+        <v/>
+      </c>
+      <c r="AT39" t="str">
+        <f>IF(error!AT14=1,time!AT14,"")</f>
+        <v/>
+      </c>
+      <c r="AU39" t="str">
+        <f>IF(error!AU14=1,time!AU14,"")</f>
+        <v/>
+      </c>
+      <c r="AV39" t="str">
+        <f>IF(error!AV14=1,time!AV14,"")</f>
+        <v/>
+      </c>
+      <c r="AW39" t="str">
+        <f>IF(error!AW14=1,time!AW14,"")</f>
+        <v/>
+      </c>
+      <c r="AX39" t="str">
+        <f>IF(error!AX14=1,time!AX14,"")</f>
+        <v/>
+      </c>
+      <c r="AY39" t="str">
+        <f>IF(error!AY14=1,time!AY14,"")</f>
+        <v/>
+      </c>
+      <c r="AZ39" t="str">
+        <f>IF(error!AZ14=1,time!AZ14,"")</f>
+        <v/>
+      </c>
+      <c r="BA39" t="str">
+        <f>IF(error!BA14=1,time!BA14,"")</f>
+        <v/>
+      </c>
+      <c r="BB39" t="str">
+        <f>IF(error!BB14=1,time!BB14,"")</f>
+        <v/>
+      </c>
+      <c r="BC39" t="str">
+        <f>IF(error!BC14=1,time!BC14,"")</f>
+        <v/>
+      </c>
+      <c r="BD39" t="str">
+        <f>IF(error!BD14=1,time!BD14,"")</f>
+        <v/>
+      </c>
+      <c r="BE39" t="str">
+        <f>IF(error!BE14=1,time!BE14,"")</f>
+        <v/>
+      </c>
+      <c r="BF39" t="str">
+        <f>IF(error!BF14=1,time!BF14,"")</f>
+        <v/>
+      </c>
+      <c r="BG39" t="str">
+        <f>IF(error!BG14=1,time!BG14,"")</f>
+        <v/>
+      </c>
+      <c r="BH39" t="str">
+        <f>IF(error!BH14=1,time!BH14,"")</f>
+        <v/>
+      </c>
+      <c r="BI39" t="str">
+        <f>IF(error!BI14=1,time!BI14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:61">
       <c r="B45" t="str">
         <f>B27</f>
         <v>AF</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" ref="C45:E45" si="5">C27</f>
+        <f t="shared" ref="C45" si="5">C27</f>
         <v>AF</v>
       </c>
       <c r="V45" t="str">
-        <f t="shared" ref="F45:W45" si="6">V27</f>
+        <f t="shared" ref="V45:W45" si="6">V27</f>
         <v>SL</v>
       </c>
       <c r="W45" t="str">
@@ -5593,7 +8999,7 @@
         <v>SL</v>
       </c>
       <c r="AP45" t="str">
-        <f t="shared" ref="X45:AQ45" si="7">AP27</f>
+        <f t="shared" ref="AP45:AQ45" si="7">AP27</f>
         <v>H</v>
       </c>
       <c r="AQ45" t="str">
@@ -5601,17 +9007,17 @@
         <v>H</v>
       </c>
     </row>
-    <row r="46" spans="1:43">
+    <row r="46" spans="1:61">
       <c r="B46" t="str">
         <f>B29</f>
         <v>(para)foveal</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" ref="C46:E46" si="8">C29</f>
+        <f t="shared" ref="C46" si="8">C29</f>
         <v>peripheral</v>
       </c>
       <c r="V46" t="str">
-        <f t="shared" ref="F46:W46" si="9">V29</f>
+        <f t="shared" ref="V46:W46" si="9">V29</f>
         <v>(para)foveal</v>
       </c>
       <c r="W46" t="str">
@@ -5619,7 +9025,7 @@
         <v>peripheral</v>
       </c>
       <c r="AP46" t="str">
-        <f t="shared" ref="X46:AQ46" si="10">AP29</f>
+        <f t="shared" ref="AP46:AQ46" si="10">AP29</f>
         <v>(para)foveal</v>
       </c>
       <c r="AQ46" t="str">
@@ -5627,62 +9033,62 @@
         <v>peripheral</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:61">
       <c r="A47" t="s">
         <v>36</v>
       </c>
       <c r="B47">
         <f>AVERAGE(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42)</f>
-        <v>1179.3</v>
+        <v>1248.7666666666667</v>
       </c>
       <c r="C47">
         <f>AVERAGE(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42)</f>
-        <v>1765.5555555555557</v>
+        <v>1728.6785714285713</v>
       </c>
       <c r="V47">
-        <f t="shared" ref="D47:AQ47" si="11">AVERAGE(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42)</f>
-        <v>1084.0999999999999</v>
+        <f t="shared" ref="V47:AQ47" si="11">AVERAGE(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42)</f>
+        <v>1175.1666666666667</v>
       </c>
       <c r="W47">
         <f t="shared" si="11"/>
-        <v>1198.0999999999999</v>
+        <v>1267.8214285714287</v>
       </c>
       <c r="AP47">
         <f t="shared" si="11"/>
-        <v>1216.7</v>
+        <v>1297.5517241379309</v>
       </c>
       <c r="AQ47">
         <f t="shared" si="11"/>
-        <v>2028.8</v>
+        <v>1955.7692307692307</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:61">
       <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48">
         <f>STDEV((B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))/SQRT(COUNT(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))</f>
-        <v>46.948446903669378</v>
+        <v>64.455967030398014</v>
       </c>
       <c r="C48">
         <f>STDEV((C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))/SQRT(COUNT(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))</f>
-        <v>415.02998924813693</v>
+        <v>185.09066885523671</v>
       </c>
       <c r="V48">
         <f>STDEV((V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))/SQRT(COUNT(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))</f>
-        <v>166.61855638953705</v>
+        <v>92.245974068252778</v>
       </c>
       <c r="W48">
         <f>STDEV((W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))/SQRT(COUNT(W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))</f>
-        <v>87.498120614737289</v>
+        <v>52.45479418250202</v>
       </c>
       <c r="AP48">
         <f>STDEV((AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))/SQRT(COUNT(AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))</f>
-        <v>248.39645953819692</v>
+        <v>178.99620621104802</v>
       </c>
       <c r="AQ48">
         <f>STDEV((AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))/SQRT(COUNT(AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))</f>
-        <v>631.19683142423958</v>
+        <v>382.46575435512898</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5706,15 +9112,15 @@
       </c>
       <c r="B54">
         <f>B47</f>
-        <v>1179.3</v>
+        <v>1248.7666666666667</v>
       </c>
       <c r="C54">
         <f>V47</f>
-        <v>1084.0999999999999</v>
+        <v>1175.1666666666667</v>
       </c>
       <c r="D54">
         <f>AP47</f>
-        <v>1216.7</v>
+        <v>1297.5517241379309</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -5724,15 +9130,15 @@
       </c>
       <c r="B55">
         <f>C47</f>
-        <v>1765.5555555555557</v>
+        <v>1728.6785714285713</v>
       </c>
       <c r="C55">
         <f>W47</f>
-        <v>1198.0999999999999</v>
+        <v>1267.8214285714287</v>
       </c>
       <c r="D55">
         <f>AQ47</f>
-        <v>2028.8</v>
+        <v>1955.7692307692307</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -5756,15 +9162,15 @@
       </c>
       <c r="B60">
         <f>B48</f>
-        <v>46.948446903669378</v>
+        <v>64.455967030398014</v>
       </c>
       <c r="C60">
         <f>V48</f>
-        <v>166.61855638953705</v>
+        <v>92.245974068252778</v>
       </c>
       <c r="D60">
         <f>AP48</f>
-        <v>248.39645953819692</v>
+        <v>178.99620621104802</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -5774,15 +9180,15 @@
       </c>
       <c r="B61">
         <f>C48</f>
-        <v>415.02998924813693</v>
+        <v>185.09066885523671</v>
       </c>
       <c r="C61">
         <f>W48</f>
-        <v>87.498120614737289</v>
+        <v>52.45479418250202</v>
       </c>
       <c r="D61">
         <f>AQ48</f>
-        <v>631.19683142423958</v>
+        <v>382.46575435512898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pilot 3 - user 5.
</commit_message>
<xml_diff>
--- a/UnityProject/results.xlsx
+++ b/UnityProject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="330" windowWidth="113955" windowHeight="16890" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="330" windowWidth="113955" windowHeight="16890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -259,7 +259,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96666666666666667</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -303,36 +303,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.93333333333333335</c:v>
+                  <c:v>0.92500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.92105263157894735</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.43333333333333335</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="131977984"/>
-        <c:axId val="131979520"/>
+        <c:axId val="127402752"/>
+        <c:axId val="127404288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131977984"/>
+        <c:axId val="127402752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131979520"/>
+        <c:crossAx val="127404288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131979520"/>
+        <c:axId val="127404288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -340,7 +340,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131977984"/>
+        <c:crossAx val="127402752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -353,7 +353,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -392,13 +392,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>64.455967030398014</c:v>
+                    <c:v>53.13369310474021</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>92.245974068252778</c:v>
+                    <c:v>72.080952421031981</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>178.99620621104802</c:v>
+                    <c:v>149.78243186705706</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -410,13 +410,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>64.455967030398014</c:v>
+                    <c:v>53.13369310474021</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>92.245974068252778</c:v>
+                    <c:v>72.080952421031981</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>178.99620621104802</c:v>
+                    <c:v>149.78243186705706</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -446,13 +446,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1248.7666666666667</c:v>
+                  <c:v>1197.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1175.1666666666667</c:v>
+                  <c:v>1108.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1297.5517241379309</c:v>
+                  <c:v>1346.2105263157894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,13 +482,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>185.09066885523671</c:v>
+                    <c:v>177.77273320646992</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>52.45479418250202</c:v>
+                    <c:v>47.900214908028254</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>382.46575435512898</c:v>
+                    <c:v>294.15221038744045</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -500,13 +500,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>185.09066885523671</c:v>
+                    <c:v>177.77273320646992</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>52.45479418250202</c:v>
+                    <c:v>47.900214908028254</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>382.46575435512898</c:v>
+                    <c:v>294.15221038744045</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -536,36 +536,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1728.6785714285713</c:v>
+                  <c:v>1689.3783783783783</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1267.8214285714287</c:v>
+                  <c:v>1215.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1955.7692307692307</c:v>
+                  <c:v>1947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="133740416"/>
-        <c:axId val="133741952"/>
+        <c:axId val="129017728"/>
+        <c:axId val="129019264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133740416"/>
+        <c:axId val="129017728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133741952"/>
+        <c:crossAx val="129019264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133741952"/>
+        <c:axId val="129019264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,7 +573,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133740416"/>
+        <c:crossAx val="129017728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -586,7 +586,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -950,7 +950,7 @@
   <dimension ref="A1:BI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+      <selection activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2493,8 +2493,187 @@
     </row>
     <row r="8" spans="1:61">
       <c r="A8" s="1">
-        <f>error!A8</f>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>174</v>
+      </c>
+      <c r="H8">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>14</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>11</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>12</v>
+      </c>
+      <c r="S8">
+        <v>11</v>
+      </c>
+      <c r="T8">
+        <v>9</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <v>9</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
+        <v>11</v>
+      </c>
+      <c r="Y8">
+        <v>14</v>
+      </c>
+      <c r="Z8">
+        <v>11</v>
+      </c>
+      <c r="AA8">
+        <v>126</v>
+      </c>
+      <c r="AB8">
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <v>11</v>
+      </c>
+      <c r="AD8">
+        <v>16</v>
+      </c>
+      <c r="AE8">
+        <v>9</v>
+      </c>
+      <c r="AF8">
+        <v>15</v>
+      </c>
+      <c r="AG8">
+        <v>19</v>
+      </c>
+      <c r="AH8">
+        <v>20</v>
+      </c>
+      <c r="AI8">
+        <v>62</v>
+      </c>
+      <c r="AJ8">
+        <v>12</v>
+      </c>
+      <c r="AK8">
+        <v>53</v>
+      </c>
+      <c r="AL8">
+        <v>16</v>
+      </c>
+      <c r="AM8">
+        <v>130</v>
+      </c>
+      <c r="AN8">
+        <v>7</v>
+      </c>
+      <c r="AO8">
+        <v>123</v>
+      </c>
+      <c r="AP8">
+        <v>14</v>
+      </c>
+      <c r="AQ8">
+        <v>12</v>
+      </c>
+      <c r="AR8">
+        <v>10</v>
+      </c>
+      <c r="AS8">
+        <v>-1</v>
+      </c>
+      <c r="AT8">
+        <v>13</v>
+      </c>
+      <c r="AU8">
+        <v>-1</v>
+      </c>
+      <c r="AV8">
+        <v>4</v>
+      </c>
+      <c r="AW8">
+        <v>-1</v>
+      </c>
+      <c r="AX8">
+        <v>6</v>
+      </c>
+      <c r="AY8">
+        <v>12</v>
+      </c>
+      <c r="AZ8">
+        <v>-1</v>
+      </c>
+      <c r="BA8">
+        <v>-1</v>
+      </c>
+      <c r="BB8">
+        <v>9</v>
+      </c>
+      <c r="BC8">
+        <v>6</v>
+      </c>
+      <c r="BD8">
+        <v>9</v>
+      </c>
+      <c r="BE8">
+        <v>-1</v>
+      </c>
+      <c r="BF8">
+        <v>9</v>
+      </c>
+      <c r="BG8">
+        <v>6</v>
+      </c>
+      <c r="BH8">
+        <v>9</v>
+      </c>
+      <c r="BI8">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -2560,8 +2739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4060,7 +4239,249 @@
       </c>
     </row>
     <row r="8" spans="1:61">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f>IF(AND(distance!B8&lt;80,distance!B8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>IF(AND(distance!C8&lt;80,distance!C8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f>IF(AND(distance!D8&lt;80,distance!D8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>IF(AND(distance!E8&lt;80,distance!E8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>IF(AND(distance!F8&lt;80,distance!F8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f>IF(AND(distance!G8&lt;80,distance!G8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>IF(AND(distance!H8&lt;80,distance!H8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>IF(AND(distance!I8&lt;80,distance!I8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>IF(AND(distance!J8&lt;80,distance!J8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f>IF(AND(distance!K8&lt;80,distance!K8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f>IF(AND(distance!L8&lt;80,distance!L8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f>IF(AND(distance!M8&lt;80,distance!M8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <f>IF(AND(distance!N8&lt;80,distance!N8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f>IF(AND(distance!O8&lt;80,distance!O8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <f>IF(AND(distance!P8&lt;80,distance!P8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <f>IF(AND(distance!Q8&lt;80,distance!Q8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f>IF(AND(distance!R8&lt;80,distance!R8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f>IF(AND(distance!S8&lt;80,distance!S8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <f>IF(AND(distance!T8&lt;80,distance!T8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <f>IF(AND(distance!U8&lt;80,distance!U8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <f>IF(AND(distance!V8&lt;80,distance!V8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <f>IF(AND(distance!W8&lt;80,distance!W8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <f>IF(AND(distance!X8&lt;80,distance!X8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <f>IF(AND(distance!Y8&lt;80,distance!Y8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <f>IF(AND(distance!Z8&lt;80,distance!Z8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <f>IF(AND(distance!AA8&lt;80,distance!AA8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <f>IF(AND(distance!AB8&lt;80,distance!AB8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <f>IF(AND(distance!AC8&lt;80,distance!AC8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <f>IF(AND(distance!AD8&lt;80,distance!AD8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <f>IF(AND(distance!AE8&lt;80,distance!AE8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <f>IF(AND(distance!AF8&lt;80,distance!AF8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <f>IF(AND(distance!AG8&lt;80,distance!AG8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <f>IF(AND(distance!AH8&lt;80,distance!AH8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <f>IF(AND(distance!AI8&lt;80,distance!AI8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <f>IF(AND(distance!AJ8&lt;80,distance!AJ8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <f>IF(AND(distance!AK8&lt;80,distance!AK8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <f>IF(AND(distance!AL8&lt;80,distance!AL8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <f>IF(AND(distance!AM8&lt;80,distance!AM8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <f>IF(AND(distance!AN8&lt;80,distance!AN8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <f>IF(AND(distance!AO8&lt;80,distance!AO8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <f>IF(AND(distance!AP8&lt;80,distance!AP8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ8">
+        <f>IF(AND(distance!AQ8&lt;80,distance!AQ8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AR8">
+        <f>IF(AND(distance!AR8&lt;80,distance!AR8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AS8">
+        <f>IF(AND(distance!AS8&lt;80,distance!AS8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <f>IF(AND(distance!AT8&lt;80,distance!AT8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU8">
+        <f>IF(AND(distance!AU8&lt;80,distance!AU8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <f>IF(AND(distance!AV8&lt;80,distance!AV8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AW8">
+        <f>IF(AND(distance!AW8&lt;80,distance!AW8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <f>IF(AND(distance!AX8&lt;80,distance!AX8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY8">
+        <f>IF(AND(distance!AY8&lt;80,distance!AY8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ8">
+        <f>IF(AND(distance!AZ8&lt;80,distance!AZ8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <f>IF(AND(distance!BA8&lt;80,distance!BA8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <f>IF(AND(distance!BB8&lt;80,distance!BB8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC8">
+        <f>IF(AND(distance!BC8&lt;80,distance!BC8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BD8">
+        <f>IF(AND(distance!BD8&lt;80,distance!BD8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE8">
+        <f>IF(AND(distance!BE8&lt;80,distance!BE8&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF8">
+        <f>IF(AND(distance!BF8&lt;80,distance!BF8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG8">
+        <f>IF(AND(distance!BG8&lt;80,distance!BG8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BH8">
+        <f>IF(AND(distance!BH8&lt;80,distance!BH8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI8">
+        <f>IF(AND(distance!BI8&lt;80,distance!BI8&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:61">
       <c r="A9" s="1"/>
@@ -4145,7 +4566,7 @@
       </c>
       <c r="C22">
         <f t="shared" ref="C22:AQ22" si="51">SUM(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)/COUNT(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)</f>
-        <v>0.93333333333333335</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="V22">
         <f t="shared" si="51"/>
@@ -4153,15 +4574,15 @@
       </c>
       <c r="W22">
         <f t="shared" si="51"/>
-        <v>1</v>
+        <v>0.92105263157894735</v>
       </c>
       <c r="AP22">
         <f t="shared" si="51"/>
-        <v>0.96666666666666667</v>
+        <v>0.95</v>
       </c>
       <c r="AQ22">
         <f t="shared" si="51"/>
-        <v>0.43333333333333335</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="28" spans="1:43">
@@ -4193,7 +4614,7 @@
       </c>
       <c r="D29">
         <f>AP22</f>
-        <v>0.96666666666666667</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="30" spans="1:43">
@@ -4203,15 +4624,15 @@
       </c>
       <c r="B30">
         <f>C22</f>
-        <v>0.93333333333333335</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="C30">
         <f>W22</f>
-        <v>1</v>
+        <v>0.92105263157894735</v>
       </c>
       <c r="D30">
         <f>AQ22</f>
-        <v>0.43333333333333335</v>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>
@@ -4224,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="U64" sqref="U64:V64"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5775,7 +6196,187 @@
     <row r="8" spans="1:61">
       <c r="A8">
         <f>error!A8</f>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1015</v>
+      </c>
+      <c r="C8">
+        <v>978</v>
+      </c>
+      <c r="D8">
+        <v>911</v>
+      </c>
+      <c r="E8">
+        <v>932</v>
+      </c>
+      <c r="F8">
+        <v>915</v>
+      </c>
+      <c r="G8">
+        <v>1382</v>
+      </c>
+      <c r="H8">
+        <v>948</v>
+      </c>
+      <c r="I8">
+        <v>4719</v>
+      </c>
+      <c r="J8">
+        <v>1599</v>
+      </c>
+      <c r="K8">
+        <v>865</v>
+      </c>
+      <c r="L8">
+        <v>949</v>
+      </c>
+      <c r="M8">
+        <v>661</v>
+      </c>
+      <c r="N8">
+        <v>849</v>
+      </c>
+      <c r="O8">
+        <v>999</v>
+      </c>
+      <c r="P8">
+        <v>882</v>
+      </c>
+      <c r="Q8">
+        <v>685</v>
+      </c>
+      <c r="R8">
+        <v>1249</v>
+      </c>
+      <c r="S8">
+        <v>1065</v>
+      </c>
+      <c r="T8">
+        <v>1115</v>
+      </c>
+      <c r="U8">
+        <v>3200</v>
+      </c>
+      <c r="V8">
+        <v>913</v>
+      </c>
+      <c r="W8">
+        <v>946</v>
+      </c>
+      <c r="X8">
+        <v>979</v>
+      </c>
+      <c r="Y8">
+        <v>845</v>
+      </c>
+      <c r="Z8">
+        <v>796</v>
+      </c>
+      <c r="AA8">
+        <v>695</v>
+      </c>
+      <c r="AB8">
+        <v>829</v>
+      </c>
+      <c r="AC8">
+        <v>1413</v>
+      </c>
+      <c r="AD8">
+        <v>829</v>
+      </c>
+      <c r="AE8">
+        <v>1012</v>
+      </c>
+      <c r="AF8">
+        <v>1213</v>
+      </c>
+      <c r="AG8">
+        <v>1100</v>
+      </c>
+      <c r="AH8">
+        <v>812</v>
+      </c>
+      <c r="AI8">
+        <v>762</v>
+      </c>
+      <c r="AJ8">
+        <v>861</v>
+      </c>
+      <c r="AK8">
+        <v>962</v>
+      </c>
+      <c r="AL8">
+        <v>1062</v>
+      </c>
+      <c r="AM8">
+        <v>745</v>
+      </c>
+      <c r="AN8">
+        <v>796</v>
+      </c>
+      <c r="AO8">
+        <v>1229</v>
+      </c>
+      <c r="AP8">
+        <v>814</v>
+      </c>
+      <c r="AQ8">
+        <v>2582</v>
+      </c>
+      <c r="AR8">
+        <v>964</v>
+      </c>
+      <c r="AS8">
+        <v>5018</v>
+      </c>
+      <c r="AT8">
+        <v>764</v>
+      </c>
+      <c r="AU8">
+        <v>5001</v>
+      </c>
+      <c r="AV8">
+        <v>1998</v>
+      </c>
+      <c r="AW8">
+        <v>5001</v>
+      </c>
+      <c r="AX8">
+        <v>1277</v>
+      </c>
+      <c r="AY8">
+        <v>1014</v>
+      </c>
+      <c r="AZ8">
+        <v>5001</v>
+      </c>
+      <c r="BA8">
+        <v>5001</v>
+      </c>
+      <c r="BB8">
+        <v>1331</v>
+      </c>
+      <c r="BC8">
+        <v>877</v>
+      </c>
+      <c r="BD8">
+        <v>1048</v>
+      </c>
+      <c r="BE8">
+        <v>5001</v>
+      </c>
+      <c r="BF8">
+        <v>3253</v>
+      </c>
+      <c r="BG8">
+        <v>2099</v>
+      </c>
+      <c r="BH8">
+        <v>2078</v>
+      </c>
+      <c r="BI8">
+        <v>3049</v>
       </c>
     </row>
     <row r="9" spans="1:61">
@@ -7274,207 +7875,207 @@
     <row r="33" spans="1:61">
       <c r="A33">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B33" t="str">
+        <v>5</v>
+      </c>
+      <c r="B33">
         <f>IF(error!B8=1,time!B8,"")</f>
-        <v/>
-      </c>
-      <c r="C33" t="str">
+        <v>1015</v>
+      </c>
+      <c r="C33">
         <f>IF(error!C8=1,time!C8,"")</f>
-        <v/>
-      </c>
-      <c r="D33" t="str">
+        <v>978</v>
+      </c>
+      <c r="D33">
         <f>IF(error!D8=1,time!D8,"")</f>
-        <v/>
-      </c>
-      <c r="E33" t="str">
+        <v>911</v>
+      </c>
+      <c r="E33">
         <f>IF(error!E8=1,time!E8,"")</f>
-        <v/>
-      </c>
-      <c r="F33" t="str">
+        <v>932</v>
+      </c>
+      <c r="F33">
         <f>IF(error!F8=1,time!F8,"")</f>
-        <v/>
+        <v>915</v>
       </c>
       <c r="G33" t="str">
         <f>IF(error!G8=1,time!G8,"")</f>
         <v/>
       </c>
-      <c r="H33" t="str">
+      <c r="H33">
         <f>IF(error!H8=1,time!H8,"")</f>
-        <v/>
-      </c>
-      <c r="I33" t="str">
+        <v>948</v>
+      </c>
+      <c r="I33">
         <f>IF(error!I8=1,time!I8,"")</f>
-        <v/>
-      </c>
-      <c r="J33" t="str">
+        <v>4719</v>
+      </c>
+      <c r="J33">
         <f>IF(error!J8=1,time!J8,"")</f>
-        <v/>
-      </c>
-      <c r="K33" t="str">
+        <v>1599</v>
+      </c>
+      <c r="K33">
         <f>IF(error!K8=1,time!K8,"")</f>
-        <v/>
-      </c>
-      <c r="L33" t="str">
+        <v>865</v>
+      </c>
+      <c r="L33">
         <f>IF(error!L8=1,time!L8,"")</f>
-        <v/>
-      </c>
-      <c r="M33" t="str">
+        <v>949</v>
+      </c>
+      <c r="M33">
         <f>IF(error!M8=1,time!M8,"")</f>
-        <v/>
-      </c>
-      <c r="N33" t="str">
+        <v>661</v>
+      </c>
+      <c r="N33">
         <f>IF(error!N8=1,time!N8,"")</f>
-        <v/>
-      </c>
-      <c r="O33" t="str">
+        <v>849</v>
+      </c>
+      <c r="O33">
         <f>IF(error!O8=1,time!O8,"")</f>
-        <v/>
-      </c>
-      <c r="P33" t="str">
+        <v>999</v>
+      </c>
+      <c r="P33">
         <f>IF(error!P8=1,time!P8,"")</f>
-        <v/>
-      </c>
-      <c r="Q33" t="str">
+        <v>882</v>
+      </c>
+      <c r="Q33">
         <f>IF(error!Q8=1,time!Q8,"")</f>
-        <v/>
-      </c>
-      <c r="R33" t="str">
+        <v>685</v>
+      </c>
+      <c r="R33">
         <f>IF(error!R8=1,time!R8,"")</f>
-        <v/>
-      </c>
-      <c r="S33" t="str">
+        <v>1249</v>
+      </c>
+      <c r="S33">
         <f>IF(error!S8=1,time!S8,"")</f>
-        <v/>
-      </c>
-      <c r="T33" t="str">
+        <v>1065</v>
+      </c>
+      <c r="T33">
         <f>IF(error!T8=1,time!T8,"")</f>
-        <v/>
-      </c>
-      <c r="U33" t="str">
+        <v>1115</v>
+      </c>
+      <c r="U33">
         <f>IF(error!U8=1,time!U8,"")</f>
-        <v/>
-      </c>
-      <c r="V33" t="str">
+        <v>3200</v>
+      </c>
+      <c r="V33">
         <f>IF(error!V8=1,time!V8,"")</f>
-        <v/>
-      </c>
-      <c r="W33" t="str">
+        <v>913</v>
+      </c>
+      <c r="W33">
         <f>IF(error!W8=1,time!W8,"")</f>
-        <v/>
-      </c>
-      <c r="X33" t="str">
+        <v>946</v>
+      </c>
+      <c r="X33">
         <f>IF(error!X8=1,time!X8,"")</f>
-        <v/>
-      </c>
-      <c r="Y33" t="str">
+        <v>979</v>
+      </c>
+      <c r="Y33">
         <f>IF(error!Y8=1,time!Y8,"")</f>
-        <v/>
-      </c>
-      <c r="Z33" t="str">
+        <v>845</v>
+      </c>
+      <c r="Z33">
         <f>IF(error!Z8=1,time!Z8,"")</f>
-        <v/>
+        <v>796</v>
       </c>
       <c r="AA33" t="str">
         <f>IF(error!AA8=1,time!AA8,"")</f>
         <v/>
       </c>
-      <c r="AB33" t="str">
+      <c r="AB33">
         <f>IF(error!AB8=1,time!AB8,"")</f>
-        <v/>
-      </c>
-      <c r="AC33" t="str">
+        <v>829</v>
+      </c>
+      <c r="AC33">
         <f>IF(error!AC8=1,time!AC8,"")</f>
-        <v/>
-      </c>
-      <c r="AD33" t="str">
+        <v>1413</v>
+      </c>
+      <c r="AD33">
         <f>IF(error!AD8=1,time!AD8,"")</f>
-        <v/>
-      </c>
-      <c r="AE33" t="str">
+        <v>829</v>
+      </c>
+      <c r="AE33">
         <f>IF(error!AE8=1,time!AE8,"")</f>
-        <v/>
-      </c>
-      <c r="AF33" t="str">
+        <v>1012</v>
+      </c>
+      <c r="AF33">
         <f>IF(error!AF8=1,time!AF8,"")</f>
-        <v/>
-      </c>
-      <c r="AG33" t="str">
+        <v>1213</v>
+      </c>
+      <c r="AG33">
         <f>IF(error!AG8=1,time!AG8,"")</f>
-        <v/>
-      </c>
-      <c r="AH33" t="str">
+        <v>1100</v>
+      </c>
+      <c r="AH33">
         <f>IF(error!AH8=1,time!AH8,"")</f>
-        <v/>
-      </c>
-      <c r="AI33" t="str">
+        <v>812</v>
+      </c>
+      <c r="AI33">
         <f>IF(error!AI8=1,time!AI8,"")</f>
-        <v/>
-      </c>
-      <c r="AJ33" t="str">
+        <v>762</v>
+      </c>
+      <c r="AJ33">
         <f>IF(error!AJ8=1,time!AJ8,"")</f>
-        <v/>
-      </c>
-      <c r="AK33" t="str">
+        <v>861</v>
+      </c>
+      <c r="AK33">
         <f>IF(error!AK8=1,time!AK8,"")</f>
-        <v/>
-      </c>
-      <c r="AL33" t="str">
+        <v>962</v>
+      </c>
+      <c r="AL33">
         <f>IF(error!AL8=1,time!AL8,"")</f>
-        <v/>
+        <v>1062</v>
       </c>
       <c r="AM33" t="str">
         <f>IF(error!AM8=1,time!AM8,"")</f>
         <v/>
       </c>
-      <c r="AN33" t="str">
+      <c r="AN33">
         <f>IF(error!AN8=1,time!AN8,"")</f>
-        <v/>
+        <v>796</v>
       </c>
       <c r="AO33" t="str">
         <f>IF(error!AO8=1,time!AO8,"")</f>
         <v/>
       </c>
-      <c r="AP33" t="str">
+      <c r="AP33">
         <f>IF(error!AP8=1,time!AP8,"")</f>
-        <v/>
-      </c>
-      <c r="AQ33" t="str">
+        <v>814</v>
+      </c>
+      <c r="AQ33">
         <f>IF(error!AQ8=1,time!AQ8,"")</f>
-        <v/>
-      </c>
-      <c r="AR33" t="str">
+        <v>2582</v>
+      </c>
+      <c r="AR33">
         <f>IF(error!AR8=1,time!AR8,"")</f>
-        <v/>
+        <v>964</v>
       </c>
       <c r="AS33" t="str">
         <f>IF(error!AS8=1,time!AS8,"")</f>
         <v/>
       </c>
-      <c r="AT33" t="str">
+      <c r="AT33">
         <f>IF(error!AT8=1,time!AT8,"")</f>
-        <v/>
+        <v>764</v>
       </c>
       <c r="AU33" t="str">
         <f>IF(error!AU8=1,time!AU8,"")</f>
         <v/>
       </c>
-      <c r="AV33" t="str">
+      <c r="AV33">
         <f>IF(error!AV8=1,time!AV8,"")</f>
-        <v/>
+        <v>1998</v>
       </c>
       <c r="AW33" t="str">
         <f>IF(error!AW8=1,time!AW8,"")</f>
         <v/>
       </c>
-      <c r="AX33" t="str">
+      <c r="AX33">
         <f>IF(error!AX8=1,time!AX8,"")</f>
-        <v/>
-      </c>
-      <c r="AY33" t="str">
+        <v>1277</v>
+      </c>
+      <c r="AY33">
         <f>IF(error!AY8=1,time!AY8,"")</f>
-        <v/>
+        <v>1014</v>
       </c>
       <c r="AZ33" t="str">
         <f>IF(error!AZ8=1,time!AZ8,"")</f>
@@ -7484,37 +8085,37 @@
         <f>IF(error!BA8=1,time!BA8,"")</f>
         <v/>
       </c>
-      <c r="BB33" t="str">
+      <c r="BB33">
         <f>IF(error!BB8=1,time!BB8,"")</f>
-        <v/>
-      </c>
-      <c r="BC33" t="str">
+        <v>1331</v>
+      </c>
+      <c r="BC33">
         <f>IF(error!BC8=1,time!BC8,"")</f>
-        <v/>
-      </c>
-      <c r="BD33" t="str">
+        <v>877</v>
+      </c>
+      <c r="BD33">
         <f>IF(error!BD8=1,time!BD8,"")</f>
-        <v/>
+        <v>1048</v>
       </c>
       <c r="BE33" t="str">
         <f>IF(error!BE8=1,time!BE8,"")</f>
         <v/>
       </c>
-      <c r="BF33" t="str">
+      <c r="BF33">
         <f>IF(error!BF8=1,time!BF8,"")</f>
-        <v/>
-      </c>
-      <c r="BG33" t="str">
+        <v>3253</v>
+      </c>
+      <c r="BG33">
         <f>IF(error!BG8=1,time!BG8,"")</f>
-        <v/>
-      </c>
-      <c r="BH33" t="str">
+        <v>2099</v>
+      </c>
+      <c r="BH33">
         <f>IF(error!BH8=1,time!BH8,"")</f>
-        <v/>
-      </c>
-      <c r="BI33" t="str">
+        <v>2078</v>
+      </c>
+      <c r="BI33">
         <f>IF(error!BI8=1,time!BI8,"")</f>
-        <v/>
+        <v>3049</v>
       </c>
     </row>
     <row r="34" spans="1:61">
@@ -9039,27 +9640,27 @@
       </c>
       <c r="B47">
         <f>AVERAGE(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42)</f>
-        <v>1248.7666666666667</v>
+        <v>1197.375</v>
       </c>
       <c r="C47">
         <f>AVERAGE(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42)</f>
-        <v>1728.6785714285713</v>
+        <v>1689.3783783783783</v>
       </c>
       <c r="V47">
         <f t="shared" ref="V47:AQ47" si="11">AVERAGE(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42)</f>
-        <v>1175.1666666666667</v>
+        <v>1108.625</v>
       </c>
       <c r="W47">
         <f t="shared" si="11"/>
-        <v>1267.8214285714287</v>
+        <v>1215.4000000000001</v>
       </c>
       <c r="AP47">
         <f t="shared" si="11"/>
-        <v>1297.5517241379309</v>
+        <v>1346.2105263157894</v>
       </c>
       <c r="AQ47">
         <f t="shared" si="11"/>
-        <v>1955.7692307692307</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="48" spans="1:61">
@@ -9068,27 +9669,27 @@
       </c>
       <c r="B48">
         <f>STDEV((B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))/SQRT(COUNT(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))</f>
-        <v>64.455967030398014</v>
+        <v>53.13369310474021</v>
       </c>
       <c r="C48">
         <f>STDEV((C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))/SQRT(COUNT(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))</f>
-        <v>185.09066885523671</v>
+        <v>177.77273320646992</v>
       </c>
       <c r="V48">
         <f>STDEV((V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))/SQRT(COUNT(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))</f>
-        <v>92.245974068252778</v>
+        <v>72.080952421031981</v>
       </c>
       <c r="W48">
         <f>STDEV((W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))/SQRT(COUNT(W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))</f>
-        <v>52.45479418250202</v>
+        <v>47.900214908028254</v>
       </c>
       <c r="AP48">
         <f>STDEV((AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))/SQRT(COUNT(AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))</f>
-        <v>178.99620621104802</v>
+        <v>149.78243186705706</v>
       </c>
       <c r="AQ48">
         <f>STDEV((AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))/SQRT(COUNT(AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))</f>
-        <v>382.46575435512898</v>
+        <v>294.15221038744045</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -9112,15 +9713,15 @@
       </c>
       <c r="B54">
         <f>B47</f>
-        <v>1248.7666666666667</v>
+        <v>1197.375</v>
       </c>
       <c r="C54">
         <f>V47</f>
-        <v>1175.1666666666667</v>
+        <v>1108.625</v>
       </c>
       <c r="D54">
         <f>AP47</f>
-        <v>1297.5517241379309</v>
+        <v>1346.2105263157894</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -9130,15 +9731,15 @@
       </c>
       <c r="B55">
         <f>C47</f>
-        <v>1728.6785714285713</v>
+        <v>1689.3783783783783</v>
       </c>
       <c r="C55">
         <f>W47</f>
-        <v>1267.8214285714287</v>
+        <v>1215.4000000000001</v>
       </c>
       <c r="D55">
         <f>AQ47</f>
-        <v>1955.7692307692307</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -9162,15 +9763,15 @@
       </c>
       <c r="B60">
         <f>B48</f>
-        <v>64.455967030398014</v>
+        <v>53.13369310474021</v>
       </c>
       <c r="C60">
         <f>V48</f>
-        <v>92.245974068252778</v>
+        <v>72.080952421031981</v>
       </c>
       <c r="D60">
         <f>AP48</f>
-        <v>178.99620621104802</v>
+        <v>149.78243186705706</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -9180,15 +9781,15 @@
       </c>
       <c r="B61">
         <f>C48</f>
-        <v>185.09066885523671</v>
+        <v>177.77273320646992</v>
       </c>
       <c r="C61">
         <f>W48</f>
-        <v>52.45479418250202</v>
+        <v>47.900214908028254</v>
       </c>
       <c r="D61">
         <f>AQ48</f>
-        <v>382.46575435512898</v>
+        <v>294.15221038744045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pilot 3 - updated results with first 6 participants.
</commit_message>
<xml_diff>
--- a/UnityProject/results.xlsx
+++ b/UnityProject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="330" windowWidth="113955" windowHeight="16890" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="330" windowWidth="113955" windowHeight="16890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="distance" sheetId="2" r:id="rId1"/>
@@ -259,7 +259,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95</c:v>
+                  <c:v>0.91666666666666663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -303,44 +303,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.92500000000000004</c:v>
+                  <c:v>0.94915254237288138</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92105263157894735</c:v>
+                  <c:v>0.94827586206896552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="127402752"/>
-        <c:axId val="127404288"/>
+        <c:axId val="128856832"/>
+        <c:axId val="128858368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127402752"/>
+        <c:axId val="128856832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127404288"/>
+        <c:crossAx val="128858368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127404288"/>
+        <c:axId val="128858368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127402752"/>
+        <c:crossAx val="128856832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -353,7 +355,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -392,13 +394,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>53.13369310474021</c:v>
+                    <c:v>39.91407738438064</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>72.080952421031981</c:v>
+                    <c:v>53.301559170264127</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>149.78243186705706</c:v>
+                    <c:v>128.42403563699798</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -410,13 +412,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>53.13369310474021</c:v>
+                    <c:v>39.91407738438064</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>72.080952421031981</c:v>
+                    <c:v>53.301559170264127</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>149.78243186705706</c:v>
+                    <c:v>128.42403563699798</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -446,13 +448,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1197.375</c:v>
+                  <c:v>1145.55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1108.625</c:v>
+                  <c:v>997.48333333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1346.2105263157894</c:v>
+                  <c:v>1319.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,13 +484,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>177.77273320646992</c:v>
+                    <c:v>123.19226490122465</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>47.900214908028254</c:v>
+                    <c:v>38.912240188481483</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>294.15221038744045</c:v>
+                    <c:v>243.48871850385046</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -500,13 +502,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>177.77273320646992</c:v>
+                    <c:v>123.19226490122465</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>47.900214908028254</c:v>
+                    <c:v>38.912240188481483</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>294.15221038744045</c:v>
+                    <c:v>243.48871850385046</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -536,36 +538,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1689.3783783783783</c:v>
+                  <c:v>1610.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1215.4000000000001</c:v>
+                  <c:v>1129.2545454545455</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1947</c:v>
+                  <c:v>1896.1666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="129017728"/>
-        <c:axId val="129019264"/>
+        <c:axId val="130340736"/>
+        <c:axId val="130342272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129017728"/>
+        <c:axId val="130340736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129019264"/>
+        <c:crossAx val="130342272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129019264"/>
+        <c:axId val="130342272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,7 +575,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129017728"/>
+        <c:crossAx val="130340736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -586,7 +588,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -950,7 +952,7 @@
   <dimension ref="A1:BI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1941,7 +1943,6 @@
     </row>
     <row r="5" spans="1:61">
       <c r="A5" s="1">
-        <f>error!A5</f>
         <v>2</v>
       </c>
       <c r="B5">
@@ -2678,57 +2679,392 @@
     </row>
     <row r="9" spans="1:61">
       <c r="A9" s="1">
-        <f>error!A9</f>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>11</v>
+      </c>
+      <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <v>15</v>
+      </c>
+      <c r="V9">
+        <v>7</v>
+      </c>
+      <c r="W9">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>5</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+      <c r="AA9">
+        <v>10</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>13</v>
+      </c>
+      <c r="AD9">
+        <v>5</v>
+      </c>
+      <c r="AE9">
+        <v>12</v>
+      </c>
+      <c r="AF9">
+        <v>7</v>
+      </c>
+      <c r="AG9">
+        <v>8</v>
+      </c>
+      <c r="AH9">
+        <v>7</v>
+      </c>
+      <c r="AI9">
+        <v>9</v>
+      </c>
+      <c r="AJ9">
+        <v>3</v>
+      </c>
+      <c r="AK9">
+        <v>10</v>
+      </c>
+      <c r="AL9">
+        <v>7</v>
+      </c>
+      <c r="AM9">
+        <v>9</v>
+      </c>
+      <c r="AN9">
+        <v>9</v>
+      </c>
+      <c r="AO9">
+        <v>2</v>
+      </c>
+      <c r="AP9">
+        <v>6</v>
+      </c>
+      <c r="AQ9">
+        <v>-1</v>
+      </c>
+      <c r="AR9">
+        <v>9</v>
+      </c>
+      <c r="AS9">
+        <v>-1</v>
+      </c>
+      <c r="AT9">
+        <v>13</v>
+      </c>
+      <c r="AU9">
+        <v>-1</v>
+      </c>
+      <c r="AV9">
+        <v>10</v>
+      </c>
+      <c r="AW9">
+        <v>8</v>
+      </c>
+      <c r="AX9">
+        <v>8</v>
+      </c>
+      <c r="AY9">
+        <v>-1</v>
+      </c>
+      <c r="AZ9">
+        <v>5</v>
+      </c>
+      <c r="BA9">
+        <v>12</v>
+      </c>
+      <c r="BB9">
+        <v>8</v>
+      </c>
+      <c r="BC9">
+        <v>16</v>
+      </c>
+      <c r="BD9">
+        <v>9</v>
+      </c>
+      <c r="BE9">
+        <v>-1</v>
+      </c>
+      <c r="BF9">
+        <v>14</v>
+      </c>
+      <c r="BG9">
+        <v>9</v>
+      </c>
+      <c r="BH9">
+        <v>5</v>
+      </c>
+      <c r="BI9">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:61">
       <c r="A10" s="1">
-        <f>error!A10</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10">
+        <v>18</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>6</v>
+      </c>
+      <c r="U10">
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <v>4</v>
+      </c>
+      <c r="X10">
+        <v>7</v>
+      </c>
+      <c r="Y10">
+        <v>8</v>
+      </c>
+      <c r="Z10">
+        <v>14</v>
+      </c>
+      <c r="AA10">
+        <v>7</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>7</v>
+      </c>
+      <c r="AD10">
+        <v>6</v>
+      </c>
+      <c r="AE10">
+        <v>3</v>
+      </c>
+      <c r="AF10">
+        <v>6</v>
+      </c>
+      <c r="AG10">
+        <v>7</v>
+      </c>
+      <c r="AH10">
+        <v>13</v>
+      </c>
+      <c r="AI10">
+        <v>68</v>
+      </c>
+      <c r="AJ10">
+        <v>8</v>
+      </c>
+      <c r="AK10">
+        <v>7</v>
+      </c>
+      <c r="AL10">
+        <v>13</v>
+      </c>
+      <c r="AM10">
+        <v>2</v>
+      </c>
+      <c r="AN10">
+        <v>2</v>
+      </c>
+      <c r="AO10">
+        <v>3</v>
+      </c>
+      <c r="AP10">
+        <v>-1</v>
+      </c>
+      <c r="AQ10">
+        <v>-1</v>
+      </c>
+      <c r="AR10">
+        <v>-1</v>
+      </c>
+      <c r="AS10">
+        <v>-1</v>
+      </c>
+      <c r="AT10">
+        <v>-1</v>
+      </c>
+      <c r="AU10">
+        <v>-1</v>
+      </c>
+      <c r="AV10">
+        <v>7</v>
+      </c>
+      <c r="AW10">
+        <v>-1</v>
+      </c>
+      <c r="AX10">
+        <v>14</v>
+      </c>
+      <c r="AY10">
+        <v>-1</v>
+      </c>
+      <c r="AZ10">
+        <v>5</v>
+      </c>
+      <c r="BA10">
+        <v>-1</v>
+      </c>
+      <c r="BB10">
+        <v>5</v>
+      </c>
+      <c r="BC10">
+        <v>-1</v>
+      </c>
+      <c r="BD10">
+        <v>7</v>
+      </c>
+      <c r="BE10">
+        <v>-1</v>
+      </c>
+      <c r="BF10">
+        <v>6</v>
+      </c>
+      <c r="BG10">
+        <v>4</v>
+      </c>
+      <c r="BH10">
+        <v>5</v>
+      </c>
+      <c r="BI10">
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:61">
-      <c r="A11" s="1">
-        <f>error!A11</f>
-        <v>0</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:61">
-      <c r="A12" s="1">
-        <f>error!A12</f>
-        <v>0</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:61">
-      <c r="A13" s="1">
-        <f>error!A13</f>
-        <v>0</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:61">
-      <c r="A14" s="1">
-        <f>error!A14</f>
-        <v>0</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:61">
-      <c r="A15" s="1">
-        <f>error!A15</f>
-        <v>0</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:61">
-      <c r="A16" s="1">
-        <f>error!A16</f>
-        <v>0</v>
-      </c>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="1">
-        <f>error!A17</f>
-        <v>0</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2739,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3511,6 +3847,7 @@
     </row>
     <row r="5" spans="1:61">
       <c r="A5" s="1">
+        <f>distance!A5</f>
         <v>2</v>
       </c>
       <c r="B5">
@@ -3756,6 +4093,7 @@
     </row>
     <row r="6" spans="1:61">
       <c r="A6" s="1">
+        <f>distance!A6</f>
         <v>3</v>
       </c>
       <c r="B6">
@@ -4001,6 +4339,7 @@
     </row>
     <row r="7" spans="1:61">
       <c r="A7" s="1">
+        <f>distance!A7</f>
         <v>4</v>
       </c>
       <c r="B7">
@@ -4240,6 +4579,7 @@
     </row>
     <row r="8" spans="1:61">
       <c r="A8" s="1">
+        <f>distance!A8</f>
         <v>5</v>
       </c>
       <c r="B8">
@@ -4484,13 +4824,499 @@
       </c>
     </row>
     <row r="9" spans="1:61">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <f>distance!A9</f>
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <f>IF(AND(distance!B9&lt;80,distance!B9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>IF(AND(distance!C9&lt;80,distance!C9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f>IF(AND(distance!D9&lt;80,distance!D9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>IF(AND(distance!E9&lt;80,distance!E9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f>IF(AND(distance!F9&lt;80,distance!F9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>IF(AND(distance!G9&lt;80,distance!G9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>IF(AND(distance!H9&lt;80,distance!H9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f>IF(AND(distance!I9&lt;80,distance!I9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f>IF(AND(distance!J9&lt;80,distance!J9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>IF(AND(distance!K9&lt;80,distance!K9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f>IF(AND(distance!L9&lt;80,distance!L9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f>IF(AND(distance!M9&lt;80,distance!M9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f>IF(AND(distance!N9&lt;80,distance!N9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f>IF(AND(distance!O9&lt;80,distance!O9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <f>IF(AND(distance!P9&lt;80,distance!P9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f>IF(AND(distance!Q9&lt;80,distance!Q9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f>IF(AND(distance!R9&lt;80,distance!R9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f>IF(AND(distance!S9&lt;80,distance!S9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <f>IF(AND(distance!T9&lt;80,distance!T9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <f>IF(AND(distance!U9&lt;80,distance!U9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <f>IF(AND(distance!V9&lt;80,distance!V9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <f>IF(AND(distance!W9&lt;80,distance!W9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <f>IF(AND(distance!X9&lt;80,distance!X9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <f>IF(AND(distance!Y9&lt;80,distance!Y9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <f>IF(AND(distance!Z9&lt;80,distance!Z9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <f>IF(AND(distance!AA9&lt;80,distance!AA9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <f>IF(AND(distance!AB9&lt;80,distance!AB9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <f>IF(AND(distance!AC9&lt;80,distance!AC9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <f>IF(AND(distance!AD9&lt;80,distance!AD9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <f>IF(AND(distance!AE9&lt;80,distance!AE9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <f>IF(AND(distance!AF9&lt;80,distance!AF9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <f>IF(AND(distance!AG9&lt;80,distance!AG9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <f>IF(AND(distance!AH9&lt;80,distance!AH9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <f>IF(AND(distance!AI9&lt;80,distance!AI9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <f>IF(AND(distance!AJ9&lt;80,distance!AJ9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <f>IF(AND(distance!AK9&lt;80,distance!AK9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <f>IF(AND(distance!AL9&lt;80,distance!AL9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <f>IF(AND(distance!AM9&lt;80,distance!AM9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN9">
+        <f>IF(AND(distance!AN9&lt;80,distance!AN9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO9">
+        <f>IF(AND(distance!AO9&lt;80,distance!AO9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AP9">
+        <f>IF(AND(distance!AP9&lt;80,distance!AP9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ9">
+        <f>IF(AND(distance!AQ9&lt;80,distance!AQ9&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <f>IF(AND(distance!AR9&lt;80,distance!AR9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AS9">
+        <f>IF(AND(distance!AS9&lt;80,distance!AS9&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <f>IF(AND(distance!AT9&lt;80,distance!AT9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU9">
+        <f>IF(AND(distance!AU9&lt;80,distance!AU9&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <f>IF(AND(distance!AV9&lt;80,distance!AV9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AW9">
+        <f>IF(AND(distance!AW9&lt;80,distance!AW9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AX9">
+        <f>IF(AND(distance!AX9&lt;80,distance!AX9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY9">
+        <f>IF(AND(distance!AY9&lt;80,distance!AY9&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ9">
+        <f>IF(AND(distance!AZ9&lt;80,distance!AZ9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <f>IF(AND(distance!BA9&lt;80,distance!BA9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BB9">
+        <f>IF(AND(distance!BB9&lt;80,distance!BB9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <f>IF(AND(distance!BC9&lt;80,distance!BC9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BD9">
+        <f>IF(AND(distance!BD9&lt;80,distance!BD9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE9">
+        <f>IF(AND(distance!BE9&lt;80,distance!BE9&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF9">
+        <f>IF(AND(distance!BF9&lt;80,distance!BF9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG9">
+        <f>IF(AND(distance!BG9&lt;80,distance!BG9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BH9">
+        <f>IF(AND(distance!BH9&lt;80,distance!BH9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI9">
+        <f>IF(AND(distance!BI9&lt;80,distance!BI9&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:61">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <f>distance!A10</f>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f>IF(AND(distance!B10&lt;80,distance!B10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>IF(AND(distance!C10&lt;80,distance!C10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>IF(AND(distance!D10&lt;80,distance!D10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>IF(AND(distance!E10&lt;80,distance!E10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>IF(AND(distance!F10&lt;80,distance!F10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f>IF(AND(distance!G10&lt;80,distance!G10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f>IF(AND(distance!H10&lt;80,distance!H10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f>IF(AND(distance!I10&lt;80,distance!I10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f>IF(AND(distance!J10&lt;80,distance!J10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f>IF(AND(distance!K10&lt;80,distance!K10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f>IF(AND(distance!L10&lt;80,distance!L10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f>IF(AND(distance!M10&lt;80,distance!M10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>IF(AND(distance!N10&lt;80,distance!N10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f>IF(AND(distance!O10&lt;80,distance!O10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f>IF(AND(distance!P10&lt;80,distance!P10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10">
+        <f>IF(AND(distance!R10&lt;80,distance!R10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <f>IF(AND(distance!S10&lt;80,distance!S10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <f>IF(AND(distance!T10&lt;80,distance!T10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <f>IF(AND(distance!U10&lt;80,distance!U10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <f>IF(AND(distance!V10&lt;80,distance!V10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <f>IF(AND(distance!W10&lt;80,distance!W10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <f>IF(AND(distance!X10&lt;80,distance!X10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <f>IF(AND(distance!Y10&lt;80,distance!Y10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <f>IF(AND(distance!Z10&lt;80,distance!Z10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <f>IF(AND(distance!AA10&lt;80,distance!AA10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <f>IF(AND(distance!AB10&lt;80,distance!AB10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <f>IF(AND(distance!AC10&lt;80,distance!AC10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <f>IF(AND(distance!AD10&lt;80,distance!AD10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <f>IF(AND(distance!AE10&lt;80,distance!AE10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <f>IF(AND(distance!AF10&lt;80,distance!AF10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <f>IF(AND(distance!AG10&lt;80,distance!AG10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <f>IF(AND(distance!AH10&lt;80,distance!AH10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <f>IF(AND(distance!AI10&lt;80,distance!AI10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <f>IF(AND(distance!AJ10&lt;80,distance!AJ10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <f>IF(AND(distance!AK10&lt;80,distance!AK10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <f>IF(AND(distance!AL10&lt;80,distance!AL10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <f>IF(AND(distance!AM10&lt;80,distance!AM10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <f>IF(AND(distance!AN10&lt;80,distance!AN10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <f>IF(AND(distance!AO10&lt;80,distance!AO10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <f>IF(AND(distance!AP10&lt;80,distance!AP10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <f>IF(AND(distance!AQ10&lt;80,distance!AQ10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <f>IF(AND(distance!AR10&lt;80,distance!AR10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <f>IF(AND(distance!AS10&lt;80,distance!AS10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <f>IF(AND(distance!AT10&lt;80,distance!AT10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <f>IF(AND(distance!AU10&lt;80,distance!AU10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <f>IF(AND(distance!AV10&lt;80,distance!AV10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AW10">
+        <f>IF(AND(distance!AW10&lt;80,distance!AW10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX10">
+        <f>IF(AND(distance!AX10&lt;80,distance!AX10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY10">
+        <f>IF(AND(distance!AY10&lt;80,distance!AY10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <f>IF(AND(distance!AZ10&lt;80,distance!AZ10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BA10">
+        <f>IF(AND(distance!BA10&lt;80,distance!BA10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <f>IF(AND(distance!BB10&lt;80,distance!BB10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC10">
+        <f>IF(AND(distance!BC10&lt;80,distance!BC10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BD10">
+        <f>IF(AND(distance!BD10&lt;80,distance!BD10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE10">
+        <f>IF(AND(distance!BE10&lt;80,distance!BE10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF10">
+        <f>IF(AND(distance!BF10&lt;80,distance!BF10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG10">
+        <f>IF(AND(distance!BG10&lt;80,distance!BG10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BH10">
+        <f>IF(AND(distance!BH10&lt;80,distance!BH10&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI10">
+        <f>IF(AND(distance!BI10&lt;80,distance!BI10&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:61">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <f>distance!A11</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:61">
       <c r="A12" s="1"/>
@@ -4566,7 +5392,7 @@
       </c>
       <c r="C22">
         <f t="shared" ref="C22:AQ22" si="51">SUM(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)/COUNT(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)</f>
-        <v>0.92500000000000004</v>
+        <v>0.94915254237288138</v>
       </c>
       <c r="V22">
         <f t="shared" si="51"/>
@@ -4574,15 +5400,15 @@
       </c>
       <c r="W22">
         <f t="shared" si="51"/>
-        <v>0.92105263157894735</v>
+        <v>0.94827586206896552</v>
       </c>
       <c r="AP22">
         <f t="shared" si="51"/>
-        <v>0.95</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="AQ22">
         <f t="shared" si="51"/>
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="28" spans="1:43">
@@ -4614,7 +5440,7 @@
       </c>
       <c r="D29">
         <f>AP22</f>
-        <v>0.95</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="30" spans="1:43">
@@ -4624,15 +5450,15 @@
       </c>
       <c r="B30">
         <f>C22</f>
-        <v>0.92500000000000004</v>
+        <v>0.94915254237288138</v>
       </c>
       <c r="C30">
         <f>W22</f>
-        <v>0.92105263157894735</v>
+        <v>0.94827586206896552</v>
       </c>
       <c r="D30">
         <f>AQ22</f>
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -4645,8 +5471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6382,13 +7208,373 @@
     <row r="9" spans="1:61">
       <c r="A9">
         <f>error!A9</f>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>698</v>
+      </c>
+      <c r="C9">
+        <v>2683</v>
+      </c>
+      <c r="D9">
+        <v>1132</v>
+      </c>
+      <c r="E9">
+        <v>1065</v>
+      </c>
+      <c r="F9">
+        <v>1336</v>
+      </c>
+      <c r="G9">
+        <v>982</v>
+      </c>
+      <c r="H9">
+        <v>911</v>
+      </c>
+      <c r="I9">
+        <v>1566</v>
+      </c>
+      <c r="J9">
+        <v>965</v>
+      </c>
+      <c r="K9">
+        <v>982</v>
+      </c>
+      <c r="L9">
+        <v>949</v>
+      </c>
+      <c r="M9">
+        <v>2033</v>
+      </c>
+      <c r="N9">
+        <v>882</v>
+      </c>
+      <c r="O9">
+        <v>1578</v>
+      </c>
+      <c r="P9">
+        <v>936</v>
+      </c>
+      <c r="Q9">
+        <v>1212</v>
+      </c>
+      <c r="R9">
+        <v>1015</v>
+      </c>
+      <c r="S9">
+        <v>1465</v>
+      </c>
+      <c r="T9">
+        <v>832</v>
+      </c>
+      <c r="U9">
+        <v>1269</v>
+      </c>
+      <c r="V9">
+        <v>829</v>
+      </c>
+      <c r="W9">
+        <v>679</v>
+      </c>
+      <c r="X9">
+        <v>679</v>
+      </c>
+      <c r="Y9">
+        <v>566</v>
+      </c>
+      <c r="Z9">
+        <v>716</v>
+      </c>
+      <c r="AA9">
+        <v>682</v>
+      </c>
+      <c r="AB9">
+        <v>495</v>
+      </c>
+      <c r="AC9">
+        <v>1142</v>
+      </c>
+      <c r="AD9">
+        <v>717</v>
+      </c>
+      <c r="AE9">
+        <v>1311</v>
+      </c>
+      <c r="AF9">
+        <v>405</v>
+      </c>
+      <c r="AG9">
+        <v>679</v>
+      </c>
+      <c r="AH9">
+        <v>677</v>
+      </c>
+      <c r="AI9">
+        <v>841</v>
+      </c>
+      <c r="AJ9">
+        <v>756</v>
+      </c>
+      <c r="AK9">
+        <v>941</v>
+      </c>
+      <c r="AL9">
+        <v>779</v>
+      </c>
+      <c r="AM9">
+        <v>740</v>
+      </c>
+      <c r="AN9">
+        <v>610</v>
+      </c>
+      <c r="AO9">
+        <v>1187</v>
+      </c>
+      <c r="AP9">
+        <v>1915</v>
+      </c>
+      <c r="AQ9">
+        <v>5005</v>
+      </c>
+      <c r="AR9">
+        <v>1662</v>
+      </c>
+      <c r="AS9">
+        <v>5004</v>
+      </c>
+      <c r="AT9">
+        <v>770</v>
+      </c>
+      <c r="AU9">
+        <v>5000</v>
+      </c>
+      <c r="AV9">
+        <v>543</v>
+      </c>
+      <c r="AW9">
+        <v>1131</v>
+      </c>
+      <c r="AX9">
+        <v>464</v>
+      </c>
+      <c r="AY9">
+        <v>5009</v>
+      </c>
+      <c r="AZ9">
+        <v>799</v>
+      </c>
+      <c r="BA9">
+        <v>3963</v>
+      </c>
+      <c r="BB9">
+        <v>1164</v>
+      </c>
+      <c r="BC9">
+        <v>1217</v>
+      </c>
+      <c r="BD9">
+        <v>831</v>
+      </c>
+      <c r="BE9">
+        <v>5004</v>
+      </c>
+      <c r="BF9">
+        <v>792</v>
+      </c>
+      <c r="BG9">
+        <v>1135</v>
+      </c>
+      <c r="BH9">
+        <v>710</v>
+      </c>
+      <c r="BI9">
+        <v>1551</v>
       </c>
     </row>
     <row r="10" spans="1:61">
       <c r="A10">
         <f>error!A10</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>961</v>
+      </c>
+      <c r="C10">
+        <v>2379</v>
+      </c>
+      <c r="D10">
+        <v>1032</v>
+      </c>
+      <c r="E10">
+        <v>1399</v>
+      </c>
+      <c r="F10">
+        <v>1315</v>
+      </c>
+      <c r="G10">
+        <v>1482</v>
+      </c>
+      <c r="H10">
+        <v>815</v>
+      </c>
+      <c r="I10">
+        <v>1432</v>
+      </c>
+      <c r="J10">
+        <v>1132</v>
+      </c>
+      <c r="K10">
+        <v>1149</v>
+      </c>
+      <c r="L10">
+        <v>1286</v>
+      </c>
+      <c r="M10">
+        <v>1432</v>
+      </c>
+      <c r="N10">
+        <v>1645</v>
+      </c>
+      <c r="O10">
+        <v>1553</v>
+      </c>
+      <c r="P10">
+        <v>982</v>
+      </c>
+      <c r="Q10">
+        <v>965</v>
+      </c>
+      <c r="R10">
+        <v>915</v>
+      </c>
+      <c r="S10">
+        <v>1148</v>
+      </c>
+      <c r="T10">
+        <v>1099</v>
+      </c>
+      <c r="U10">
+        <v>865</v>
+      </c>
+      <c r="V10">
+        <v>762</v>
+      </c>
+      <c r="W10">
+        <v>958</v>
+      </c>
+      <c r="X10">
+        <v>1017</v>
+      </c>
+      <c r="Y10">
+        <v>1163</v>
+      </c>
+      <c r="Z10">
+        <v>825</v>
+      </c>
+      <c r="AA10">
+        <v>1329</v>
+      </c>
+      <c r="AB10">
+        <v>863</v>
+      </c>
+      <c r="AC10">
+        <v>979</v>
+      </c>
+      <c r="AD10">
+        <v>962</v>
+      </c>
+      <c r="AE10">
+        <v>795</v>
+      </c>
+      <c r="AF10">
+        <v>879</v>
+      </c>
+      <c r="AG10">
+        <v>1113</v>
+      </c>
+      <c r="AH10">
+        <v>746</v>
+      </c>
+      <c r="AI10">
+        <v>962</v>
+      </c>
+      <c r="AJ10">
+        <v>983</v>
+      </c>
+      <c r="AK10">
+        <v>1062</v>
+      </c>
+      <c r="AL10">
+        <v>842</v>
+      </c>
+      <c r="AM10">
+        <v>1329</v>
+      </c>
+      <c r="AN10">
+        <v>962</v>
+      </c>
+      <c r="AO10">
+        <v>1112</v>
+      </c>
+      <c r="AP10">
+        <v>5001</v>
+      </c>
+      <c r="AQ10">
+        <v>5001</v>
+      </c>
+      <c r="AR10">
+        <v>5001</v>
+      </c>
+      <c r="AS10">
+        <v>5008</v>
+      </c>
+      <c r="AT10">
+        <v>5018</v>
+      </c>
+      <c r="AU10">
+        <v>5001</v>
+      </c>
+      <c r="AV10">
+        <v>1582</v>
+      </c>
+      <c r="AW10">
+        <v>5005</v>
+      </c>
+      <c r="AX10">
+        <v>944</v>
+      </c>
+      <c r="AY10">
+        <v>5001</v>
+      </c>
+      <c r="AZ10">
+        <v>5001</v>
+      </c>
+      <c r="BA10">
+        <v>5001</v>
+      </c>
+      <c r="BB10">
+        <v>1147</v>
+      </c>
+      <c r="BC10">
+        <v>5001</v>
+      </c>
+      <c r="BD10">
+        <v>797</v>
+      </c>
+      <c r="BE10">
+        <v>5000</v>
+      </c>
+      <c r="BF10">
+        <v>1181</v>
+      </c>
+      <c r="BG10">
+        <v>1465</v>
+      </c>
+      <c r="BH10">
+        <v>1131</v>
+      </c>
+      <c r="BI10">
+        <v>5001</v>
       </c>
     </row>
     <row r="26" spans="1:61">
@@ -8121,413 +9307,413 @@
     <row r="34" spans="1:61">
       <c r="A34">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B34" t="str">
+        <v>6</v>
+      </c>
+      <c r="B34">
         <f>IF(error!B9=1,time!B9,"")</f>
-        <v/>
-      </c>
-      <c r="C34" t="str">
+        <v>698</v>
+      </c>
+      <c r="C34">
         <f>IF(error!C9=1,time!C9,"")</f>
-        <v/>
-      </c>
-      <c r="D34" t="str">
+        <v>2683</v>
+      </c>
+      <c r="D34">
         <f>IF(error!D9=1,time!D9,"")</f>
-        <v/>
-      </c>
-      <c r="E34" t="str">
+        <v>1132</v>
+      </c>
+      <c r="E34">
         <f>IF(error!E9=1,time!E9,"")</f>
-        <v/>
-      </c>
-      <c r="F34" t="str">
+        <v>1065</v>
+      </c>
+      <c r="F34">
         <f>IF(error!F9=1,time!F9,"")</f>
-        <v/>
-      </c>
-      <c r="G34" t="str">
+        <v>1336</v>
+      </c>
+      <c r="G34">
         <f>IF(error!G9=1,time!G9,"")</f>
-        <v/>
-      </c>
-      <c r="H34" t="str">
+        <v>982</v>
+      </c>
+      <c r="H34">
         <f>IF(error!H9=1,time!H9,"")</f>
-        <v/>
-      </c>
-      <c r="I34" t="str">
+        <v>911</v>
+      </c>
+      <c r="I34">
         <f>IF(error!I9=1,time!I9,"")</f>
-        <v/>
-      </c>
-      <c r="J34" t="str">
+        <v>1566</v>
+      </c>
+      <c r="J34">
         <f>IF(error!J9=1,time!J9,"")</f>
-        <v/>
-      </c>
-      <c r="K34" t="str">
+        <v>965</v>
+      </c>
+      <c r="K34">
         <f>IF(error!K9=1,time!K9,"")</f>
-        <v/>
-      </c>
-      <c r="L34" t="str">
+        <v>982</v>
+      </c>
+      <c r="L34">
         <f>IF(error!L9=1,time!L9,"")</f>
-        <v/>
-      </c>
-      <c r="M34" t="str">
+        <v>949</v>
+      </c>
+      <c r="M34">
         <f>IF(error!M9=1,time!M9,"")</f>
-        <v/>
-      </c>
-      <c r="N34" t="str">
+        <v>2033</v>
+      </c>
+      <c r="N34">
         <f>IF(error!N9=1,time!N9,"")</f>
-        <v/>
-      </c>
-      <c r="O34" t="str">
+        <v>882</v>
+      </c>
+      <c r="O34">
         <f>IF(error!O9=1,time!O9,"")</f>
-        <v/>
-      </c>
-      <c r="P34" t="str">
+        <v>1578</v>
+      </c>
+      <c r="P34">
         <f>IF(error!P9=1,time!P9,"")</f>
-        <v/>
-      </c>
-      <c r="Q34" t="str">
+        <v>936</v>
+      </c>
+      <c r="Q34">
         <f>IF(error!Q9=1,time!Q9,"")</f>
-        <v/>
-      </c>
-      <c r="R34" t="str">
+        <v>1212</v>
+      </c>
+      <c r="R34">
         <f>IF(error!R9=1,time!R9,"")</f>
-        <v/>
-      </c>
-      <c r="S34" t="str">
+        <v>1015</v>
+      </c>
+      <c r="S34">
         <f>IF(error!S9=1,time!S9,"")</f>
-        <v/>
-      </c>
-      <c r="T34" t="str">
+        <v>1465</v>
+      </c>
+      <c r="T34">
         <f>IF(error!T9=1,time!T9,"")</f>
-        <v/>
-      </c>
-      <c r="U34" t="str">
+        <v>832</v>
+      </c>
+      <c r="U34">
         <f>IF(error!U9=1,time!U9,"")</f>
-        <v/>
-      </c>
-      <c r="V34" t="str">
+        <v>1269</v>
+      </c>
+      <c r="V34">
         <f>IF(error!V9=1,time!V9,"")</f>
-        <v/>
-      </c>
-      <c r="W34" t="str">
+        <v>829</v>
+      </c>
+      <c r="W34">
         <f>IF(error!W9=1,time!W9,"")</f>
-        <v/>
-      </c>
-      <c r="X34" t="str">
+        <v>679</v>
+      </c>
+      <c r="X34">
         <f>IF(error!X9=1,time!X9,"")</f>
-        <v/>
-      </c>
-      <c r="Y34" t="str">
+        <v>679</v>
+      </c>
+      <c r="Y34">
         <f>IF(error!Y9=1,time!Y9,"")</f>
-        <v/>
-      </c>
-      <c r="Z34" t="str">
+        <v>566</v>
+      </c>
+      <c r="Z34">
         <f>IF(error!Z9=1,time!Z9,"")</f>
-        <v/>
-      </c>
-      <c r="AA34" t="str">
+        <v>716</v>
+      </c>
+      <c r="AA34">
         <f>IF(error!AA9=1,time!AA9,"")</f>
-        <v/>
-      </c>
-      <c r="AB34" t="str">
+        <v>682</v>
+      </c>
+      <c r="AB34">
         <f>IF(error!AB9=1,time!AB9,"")</f>
-        <v/>
-      </c>
-      <c r="AC34" t="str">
+        <v>495</v>
+      </c>
+      <c r="AC34">
         <f>IF(error!AC9=1,time!AC9,"")</f>
-        <v/>
-      </c>
-      <c r="AD34" t="str">
+        <v>1142</v>
+      </c>
+      <c r="AD34">
         <f>IF(error!AD9=1,time!AD9,"")</f>
-        <v/>
-      </c>
-      <c r="AE34" t="str">
+        <v>717</v>
+      </c>
+      <c r="AE34">
         <f>IF(error!AE9=1,time!AE9,"")</f>
-        <v/>
-      </c>
-      <c r="AF34" t="str">
+        <v>1311</v>
+      </c>
+      <c r="AF34">
         <f>IF(error!AF9=1,time!AF9,"")</f>
-        <v/>
-      </c>
-      <c r="AG34" t="str">
+        <v>405</v>
+      </c>
+      <c r="AG34">
         <f>IF(error!AG9=1,time!AG9,"")</f>
-        <v/>
-      </c>
-      <c r="AH34" t="str">
+        <v>679</v>
+      </c>
+      <c r="AH34">
         <f>IF(error!AH9=1,time!AH9,"")</f>
-        <v/>
-      </c>
-      <c r="AI34" t="str">
+        <v>677</v>
+      </c>
+      <c r="AI34">
         <f>IF(error!AI9=1,time!AI9,"")</f>
-        <v/>
-      </c>
-      <c r="AJ34" t="str">
+        <v>841</v>
+      </c>
+      <c r="AJ34">
         <f>IF(error!AJ9=1,time!AJ9,"")</f>
-        <v/>
-      </c>
-      <c r="AK34" t="str">
+        <v>756</v>
+      </c>
+      <c r="AK34">
         <f>IF(error!AK9=1,time!AK9,"")</f>
-        <v/>
-      </c>
-      <c r="AL34" t="str">
+        <v>941</v>
+      </c>
+      <c r="AL34">
         <f>IF(error!AL9=1,time!AL9,"")</f>
-        <v/>
-      </c>
-      <c r="AM34" t="str">
+        <v>779</v>
+      </c>
+      <c r="AM34">
         <f>IF(error!AM9=1,time!AM9,"")</f>
-        <v/>
-      </c>
-      <c r="AN34" t="str">
+        <v>740</v>
+      </c>
+      <c r="AN34">
         <f>IF(error!AN9=1,time!AN9,"")</f>
-        <v/>
-      </c>
-      <c r="AO34" t="str">
+        <v>610</v>
+      </c>
+      <c r="AO34">
         <f>IF(error!AO9=1,time!AO9,"")</f>
-        <v/>
-      </c>
-      <c r="AP34" t="str">
+        <v>1187</v>
+      </c>
+      <c r="AP34">
         <f>IF(error!AP9=1,time!AP9,"")</f>
-        <v/>
+        <v>1915</v>
       </c>
       <c r="AQ34" t="str">
         <f>IF(error!AQ9=1,time!AQ9,"")</f>
         <v/>
       </c>
-      <c r="AR34" t="str">
+      <c r="AR34">
         <f>IF(error!AR9=1,time!AR9,"")</f>
-        <v/>
+        <v>1662</v>
       </c>
       <c r="AS34" t="str">
         <f>IF(error!AS9=1,time!AS9,"")</f>
         <v/>
       </c>
-      <c r="AT34" t="str">
+      <c r="AT34">
         <f>IF(error!AT9=1,time!AT9,"")</f>
-        <v/>
+        <v>770</v>
       </c>
       <c r="AU34" t="str">
         <f>IF(error!AU9=1,time!AU9,"")</f>
         <v/>
       </c>
-      <c r="AV34" t="str">
+      <c r="AV34">
         <f>IF(error!AV9=1,time!AV9,"")</f>
-        <v/>
-      </c>
-      <c r="AW34" t="str">
+        <v>543</v>
+      </c>
+      <c r="AW34">
         <f>IF(error!AW9=1,time!AW9,"")</f>
-        <v/>
-      </c>
-      <c r="AX34" t="str">
+        <v>1131</v>
+      </c>
+      <c r="AX34">
         <f>IF(error!AX9=1,time!AX9,"")</f>
-        <v/>
+        <v>464</v>
       </c>
       <c r="AY34" t="str">
         <f>IF(error!AY9=1,time!AY9,"")</f>
         <v/>
       </c>
-      <c r="AZ34" t="str">
+      <c r="AZ34">
         <f>IF(error!AZ9=1,time!AZ9,"")</f>
-        <v/>
-      </c>
-      <c r="BA34" t="str">
+        <v>799</v>
+      </c>
+      <c r="BA34">
         <f>IF(error!BA9=1,time!BA9,"")</f>
-        <v/>
-      </c>
-      <c r="BB34" t="str">
+        <v>3963</v>
+      </c>
+      <c r="BB34">
         <f>IF(error!BB9=1,time!BB9,"")</f>
-        <v/>
-      </c>
-      <c r="BC34" t="str">
+        <v>1164</v>
+      </c>
+      <c r="BC34">
         <f>IF(error!BC9=1,time!BC9,"")</f>
-        <v/>
-      </c>
-      <c r="BD34" t="str">
+        <v>1217</v>
+      </c>
+      <c r="BD34">
         <f>IF(error!BD9=1,time!BD9,"")</f>
-        <v/>
+        <v>831</v>
       </c>
       <c r="BE34" t="str">
         <f>IF(error!BE9=1,time!BE9,"")</f>
         <v/>
       </c>
-      <c r="BF34" t="str">
+      <c r="BF34">
         <f>IF(error!BF9=1,time!BF9,"")</f>
-        <v/>
-      </c>
-      <c r="BG34" t="str">
+        <v>792</v>
+      </c>
+      <c r="BG34">
         <f>IF(error!BG9=1,time!BG9,"")</f>
-        <v/>
-      </c>
-      <c r="BH34" t="str">
+        <v>1135</v>
+      </c>
+      <c r="BH34">
         <f>IF(error!BH9=1,time!BH9,"")</f>
-        <v/>
-      </c>
-      <c r="BI34" t="str">
+        <v>710</v>
+      </c>
+      <c r="BI34">
         <f>IF(error!BI9=1,time!BI9,"")</f>
-        <v/>
+        <v>1551</v>
       </c>
     </row>
     <row r="35" spans="1:61">
       <c r="A35">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="B35" t="str">
+        <v>7</v>
+      </c>
+      <c r="B35">
         <f>IF(error!B10=1,time!B10,"")</f>
-        <v/>
-      </c>
-      <c r="C35" t="str">
+        <v>961</v>
+      </c>
+      <c r="C35">
         <f>IF(error!C10=1,time!C10,"")</f>
-        <v/>
-      </c>
-      <c r="D35" t="str">
+        <v>2379</v>
+      </c>
+      <c r="D35">
         <f>IF(error!D10=1,time!D10,"")</f>
-        <v/>
-      </c>
-      <c r="E35" t="str">
+        <v>1032</v>
+      </c>
+      <c r="E35">
         <f>IF(error!E10=1,time!E10,"")</f>
-        <v/>
-      </c>
-      <c r="F35" t="str">
+        <v>1399</v>
+      </c>
+      <c r="F35">
         <f>IF(error!F10=1,time!F10,"")</f>
-        <v/>
-      </c>
-      <c r="G35" t="str">
+        <v>1315</v>
+      </c>
+      <c r="G35">
         <f>IF(error!G10=1,time!G10,"")</f>
-        <v/>
-      </c>
-      <c r="H35" t="str">
+        <v>1482</v>
+      </c>
+      <c r="H35">
         <f>IF(error!H10=1,time!H10,"")</f>
-        <v/>
-      </c>
-      <c r="I35" t="str">
+        <v>815</v>
+      </c>
+      <c r="I35">
         <f>IF(error!I10=1,time!I10,"")</f>
-        <v/>
-      </c>
-      <c r="J35" t="str">
+        <v>1432</v>
+      </c>
+      <c r="J35">
         <f>IF(error!J10=1,time!J10,"")</f>
-        <v/>
-      </c>
-      <c r="K35" t="str">
+        <v>1132</v>
+      </c>
+      <c r="K35">
         <f>IF(error!K10=1,time!K10,"")</f>
-        <v/>
-      </c>
-      <c r="L35" t="str">
+        <v>1149</v>
+      </c>
+      <c r="L35">
         <f>IF(error!L10=1,time!L10,"")</f>
-        <v/>
-      </c>
-      <c r="M35" t="str">
+        <v>1286</v>
+      </c>
+      <c r="M35">
         <f>IF(error!M10=1,time!M10,"")</f>
-        <v/>
-      </c>
-      <c r="N35" t="str">
+        <v>1432</v>
+      </c>
+      <c r="N35">
         <f>IF(error!N10=1,time!N10,"")</f>
-        <v/>
-      </c>
-      <c r="O35" t="str">
+        <v>1645</v>
+      </c>
+      <c r="O35">
         <f>IF(error!O10=1,time!O10,"")</f>
-        <v/>
-      </c>
-      <c r="P35" t="str">
+        <v>1553</v>
+      </c>
+      <c r="P35">
         <f>IF(error!P10=1,time!P10,"")</f>
-        <v/>
+        <v>982</v>
       </c>
       <c r="Q35" t="str">
         <f>IF(error!Q10=1,time!Q10,"")</f>
         <v/>
       </c>
-      <c r="R35" t="str">
+      <c r="R35">
         <f>IF(error!R10=1,time!R10,"")</f>
-        <v/>
-      </c>
-      <c r="S35" t="str">
+        <v>915</v>
+      </c>
+      <c r="S35">
         <f>IF(error!S10=1,time!S10,"")</f>
-        <v/>
-      </c>
-      <c r="T35" t="str">
+        <v>1148</v>
+      </c>
+      <c r="T35">
         <f>IF(error!T10=1,time!T10,"")</f>
-        <v/>
-      </c>
-      <c r="U35" t="str">
+        <v>1099</v>
+      </c>
+      <c r="U35">
         <f>IF(error!U10=1,time!U10,"")</f>
-        <v/>
-      </c>
-      <c r="V35" t="str">
+        <v>865</v>
+      </c>
+      <c r="V35">
         <f>IF(error!V10=1,time!V10,"")</f>
-        <v/>
-      </c>
-      <c r="W35" t="str">
+        <v>762</v>
+      </c>
+      <c r="W35">
         <f>IF(error!W10=1,time!W10,"")</f>
-        <v/>
-      </c>
-      <c r="X35" t="str">
+        <v>958</v>
+      </c>
+      <c r="X35">
         <f>IF(error!X10=1,time!X10,"")</f>
-        <v/>
-      </c>
-      <c r="Y35" t="str">
+        <v>1017</v>
+      </c>
+      <c r="Y35">
         <f>IF(error!Y10=1,time!Y10,"")</f>
-        <v/>
-      </c>
-      <c r="Z35" t="str">
+        <v>1163</v>
+      </c>
+      <c r="Z35">
         <f>IF(error!Z10=1,time!Z10,"")</f>
-        <v/>
-      </c>
-      <c r="AA35" t="str">
+        <v>825</v>
+      </c>
+      <c r="AA35">
         <f>IF(error!AA10=1,time!AA10,"")</f>
-        <v/>
-      </c>
-      <c r="AB35" t="str">
+        <v>1329</v>
+      </c>
+      <c r="AB35">
         <f>IF(error!AB10=1,time!AB10,"")</f>
-        <v/>
-      </c>
-      <c r="AC35" t="str">
+        <v>863</v>
+      </c>
+      <c r="AC35">
         <f>IF(error!AC10=1,time!AC10,"")</f>
-        <v/>
-      </c>
-      <c r="AD35" t="str">
+        <v>979</v>
+      </c>
+      <c r="AD35">
         <f>IF(error!AD10=1,time!AD10,"")</f>
-        <v/>
-      </c>
-      <c r="AE35" t="str">
+        <v>962</v>
+      </c>
+      <c r="AE35">
         <f>IF(error!AE10=1,time!AE10,"")</f>
-        <v/>
-      </c>
-      <c r="AF35" t="str">
+        <v>795</v>
+      </c>
+      <c r="AF35">
         <f>IF(error!AF10=1,time!AF10,"")</f>
-        <v/>
-      </c>
-      <c r="AG35" t="str">
+        <v>879</v>
+      </c>
+      <c r="AG35">
         <f>IF(error!AG10=1,time!AG10,"")</f>
-        <v/>
-      </c>
-      <c r="AH35" t="str">
+        <v>1113</v>
+      </c>
+      <c r="AH35">
         <f>IF(error!AH10=1,time!AH10,"")</f>
-        <v/>
-      </c>
-      <c r="AI35" t="str">
+        <v>746</v>
+      </c>
+      <c r="AI35">
         <f>IF(error!AI10=1,time!AI10,"")</f>
-        <v/>
-      </c>
-      <c r="AJ35" t="str">
+        <v>962</v>
+      </c>
+      <c r="AJ35">
         <f>IF(error!AJ10=1,time!AJ10,"")</f>
-        <v/>
-      </c>
-      <c r="AK35" t="str">
+        <v>983</v>
+      </c>
+      <c r="AK35">
         <f>IF(error!AK10=1,time!AK10,"")</f>
-        <v/>
-      </c>
-      <c r="AL35" t="str">
+        <v>1062</v>
+      </c>
+      <c r="AL35">
         <f>IF(error!AL10=1,time!AL10,"")</f>
-        <v/>
-      </c>
-      <c r="AM35" t="str">
+        <v>842</v>
+      </c>
+      <c r="AM35">
         <f>IF(error!AM10=1,time!AM10,"")</f>
-        <v/>
-      </c>
-      <c r="AN35" t="str">
+        <v>1329</v>
+      </c>
+      <c r="AN35">
         <f>IF(error!AN10=1,time!AN10,"")</f>
-        <v/>
-      </c>
-      <c r="AO35" t="str">
+        <v>962</v>
+      </c>
+      <c r="AO35">
         <f>IF(error!AO10=1,time!AO10,"")</f>
-        <v/>
+        <v>1112</v>
       </c>
       <c r="AP35" t="str">
         <f>IF(error!AP10=1,time!AP10,"")</f>
@@ -8553,57 +9739,57 @@
         <f>IF(error!AU10=1,time!AU10,"")</f>
         <v/>
       </c>
-      <c r="AV35" t="str">
+      <c r="AV35">
         <f>IF(error!AV10=1,time!AV10,"")</f>
-        <v/>
+        <v>1582</v>
       </c>
       <c r="AW35" t="str">
         <f>IF(error!AW10=1,time!AW10,"")</f>
         <v/>
       </c>
-      <c r="AX35" t="str">
+      <c r="AX35">
         <f>IF(error!AX10=1,time!AX10,"")</f>
-        <v/>
+        <v>944</v>
       </c>
       <c r="AY35" t="str">
         <f>IF(error!AY10=1,time!AY10,"")</f>
         <v/>
       </c>
-      <c r="AZ35" t="str">
+      <c r="AZ35">
         <f>IF(error!AZ10=1,time!AZ10,"")</f>
-        <v/>
+        <v>5001</v>
       </c>
       <c r="BA35" t="str">
         <f>IF(error!BA10=1,time!BA10,"")</f>
         <v/>
       </c>
-      <c r="BB35" t="str">
+      <c r="BB35">
         <f>IF(error!BB10=1,time!BB10,"")</f>
-        <v/>
+        <v>1147</v>
       </c>
       <c r="BC35" t="str">
         <f>IF(error!BC10=1,time!BC10,"")</f>
         <v/>
       </c>
-      <c r="BD35" t="str">
+      <c r="BD35">
         <f>IF(error!BD10=1,time!BD10,"")</f>
-        <v/>
+        <v>797</v>
       </c>
       <c r="BE35" t="str">
         <f>IF(error!BE10=1,time!BE10,"")</f>
         <v/>
       </c>
-      <c r="BF35" t="str">
+      <c r="BF35">
         <f>IF(error!BF10=1,time!BF10,"")</f>
-        <v/>
-      </c>
-      <c r="BG35" t="str">
+        <v>1181</v>
+      </c>
+      <c r="BG35">
         <f>IF(error!BG10=1,time!BG10,"")</f>
-        <v/>
-      </c>
-      <c r="BH35" t="str">
+        <v>1465</v>
+      </c>
+      <c r="BH35">
         <f>IF(error!BH10=1,time!BH10,"")</f>
-        <v/>
+        <v>1131</v>
       </c>
       <c r="BI35" t="str">
         <f>IF(error!BI10=1,time!BI10,"")</f>
@@ -9640,27 +10826,27 @@
       </c>
       <c r="B47">
         <f>AVERAGE(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42)</f>
-        <v>1197.375</v>
+        <v>1145.55</v>
       </c>
       <c r="C47">
         <f>AVERAGE(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42)</f>
-        <v>1689.3783783783783</v>
+        <v>1610.375</v>
       </c>
       <c r="V47">
         <f t="shared" ref="V47:AQ47" si="11">AVERAGE(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42)</f>
-        <v>1108.625</v>
+        <v>997.48333333333335</v>
       </c>
       <c r="W47">
         <f t="shared" si="11"/>
-        <v>1215.4000000000001</v>
+        <v>1129.2545454545455</v>
       </c>
       <c r="AP47">
         <f t="shared" si="11"/>
-        <v>1346.2105263157894</v>
+        <v>1319.8</v>
       </c>
       <c r="AQ47">
         <f t="shared" si="11"/>
-        <v>1947</v>
+        <v>1896.1666666666667</v>
       </c>
     </row>
     <row r="48" spans="1:61">
@@ -9669,27 +10855,27 @@
       </c>
       <c r="B48">
         <f>STDEV((B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))/SQRT(COUNT(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))</f>
-        <v>53.13369310474021</v>
+        <v>39.91407738438064</v>
       </c>
       <c r="C48">
         <f>STDEV((C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))/SQRT(COUNT(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))</f>
-        <v>177.77273320646992</v>
+        <v>123.19226490122465</v>
       </c>
       <c r="V48">
         <f>STDEV((V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))/SQRT(COUNT(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))</f>
-        <v>72.080952421031981</v>
+        <v>53.301559170264127</v>
       </c>
       <c r="W48">
         <f>STDEV((W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))/SQRT(COUNT(W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))</f>
-        <v>47.900214908028254</v>
+        <v>38.912240188481483</v>
       </c>
       <c r="AP48">
         <f>STDEV((AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))/SQRT(COUNT(AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))</f>
-        <v>149.78243186705706</v>
+        <v>128.42403563699798</v>
       </c>
       <c r="AQ48">
         <f>STDEV((AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))/SQRT(COUNT(AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))</f>
-        <v>294.15221038744045</v>
+        <v>243.48871850385046</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -9713,15 +10899,15 @@
       </c>
       <c r="B54">
         <f>B47</f>
-        <v>1197.375</v>
+        <v>1145.55</v>
       </c>
       <c r="C54">
         <f>V47</f>
-        <v>1108.625</v>
+        <v>997.48333333333335</v>
       </c>
       <c r="D54">
         <f>AP47</f>
-        <v>1346.2105263157894</v>
+        <v>1319.8</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -9731,15 +10917,15 @@
       </c>
       <c r="B55">
         <f>C47</f>
-        <v>1689.3783783783783</v>
+        <v>1610.375</v>
       </c>
       <c r="C55">
         <f>W47</f>
-        <v>1215.4000000000001</v>
+        <v>1129.2545454545455</v>
       </c>
       <c r="D55">
         <f>AQ47</f>
-        <v>1947</v>
+        <v>1896.1666666666667</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -9763,15 +10949,15 @@
       </c>
       <c r="B60">
         <f>B48</f>
-        <v>53.13369310474021</v>
+        <v>39.91407738438064</v>
       </c>
       <c r="C60">
         <f>V48</f>
-        <v>72.080952421031981</v>
+        <v>53.301559170264127</v>
       </c>
       <c r="D60">
         <f>AP48</f>
-        <v>149.78243186705706</v>
+        <v>128.42403563699798</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -9781,15 +10967,15 @@
       </c>
       <c r="B61">
         <f>C48</f>
-        <v>177.77273320646992</v>
+        <v>123.19226490122465</v>
       </c>
       <c r="C61">
         <f>W48</f>
-        <v>47.900214908028254</v>
+        <v>38.912240188481483</v>
       </c>
       <c r="D61">
         <f>AQ48</f>
-        <v>294.15221038744045</v>
+        <v>243.48871850385046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pilot 3 - results sheet updated.
</commit_message>
<xml_diff>
--- a/UnityProject/results.xlsx
+++ b/UnityProject/results.xlsx
@@ -293,7 +293,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9375</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,37 +337,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.96202531645569622</c:v>
+                  <c:v>0.95959595959595956</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94871794871794868</c:v>
+                  <c:v>0.94897959183673475</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38750000000000001</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="127900288"/>
-        <c:axId val="127922560"/>
+        <c:axId val="127261312"/>
+        <c:axId val="127345024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127900288"/>
+        <c:axId val="127261312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127922560"/>
+        <c:crossAx val="127345024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127922560"/>
+        <c:axId val="127345024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -377,7 +376,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127900288"/>
+        <c:crossAx val="127261312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -391,7 +390,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -430,13 +429,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>31.352194798305373</c:v>
+                    <c:v>29.235396354419407</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>44.483416676073965</c:v>
+                    <c:v>39.413350799089905</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>107.70861709165054</c:v>
+                    <c:v>96.094400281935677</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -448,13 +447,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>31.352194798305373</c:v>
+                    <c:v>29.235396354419407</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>44.483416676073965</c:v>
+                    <c:v>39.413350799089905</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>107.70861709165054</c:v>
+                    <c:v>96.094400281935677</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -484,13 +483,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1123.5250000000001</c:v>
+                  <c:v>1139.22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1015.725</c:v>
+                  <c:v>1061.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1315.1866666666667</c:v>
+                  <c:v>1361.3157894736842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,13 +519,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>93.016923270842369</c:v>
+                    <c:v>94.13276573395305</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>63.607603292640107</c:v>
+                    <c:v>54.501606219974747</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>243.31333740581513</c:v>
+                    <c:v>231.95314389233542</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -538,13 +537,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>93.016923270842369</c:v>
+                    <c:v>94.13276573395305</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>63.607603292640107</c:v>
+                    <c:v>54.501606219974747</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>243.31333740581513</c:v>
+                    <c:v>231.95314389233542</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -574,37 +573,36 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1551.3684210526317</c:v>
+                  <c:v>1674.957894736842</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1244.1756756756756</c:v>
+                  <c:v>1278.989247311828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2146.4193548387098</c:v>
+                  <c:v>2478.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="128025344"/>
-        <c:axId val="128026880"/>
+        <c:axId val="133083904"/>
+        <c:axId val="133085440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128025344"/>
+        <c:axId val="133083904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128026880"/>
+        <c:crossAx val="133085440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128026880"/>
+        <c:axId val="133085440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +610,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128025344"/>
+        <c:crossAx val="133083904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -626,7 +624,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -990,7 +988,7 @@
   <dimension ref="A1:BI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AP12" sqref="AP12:BI12"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3454,10 +3452,374 @@
       </c>
     </row>
     <row r="13" spans="1:61">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>133</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="R13">
+        <v>5</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>6</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13">
+        <v>6</v>
+      </c>
+      <c r="W13">
+        <v>2</v>
+      </c>
+      <c r="X13">
+        <v>6</v>
+      </c>
+      <c r="Y13">
+        <v>6</v>
+      </c>
+      <c r="Z13">
+        <v>5</v>
+      </c>
+      <c r="AA13">
+        <v>4</v>
+      </c>
+      <c r="AB13">
+        <v>6</v>
+      </c>
+      <c r="AC13">
+        <v>3</v>
+      </c>
+      <c r="AD13">
+        <v>5</v>
+      </c>
+      <c r="AE13">
+        <v>6</v>
+      </c>
+      <c r="AF13">
+        <v>6</v>
+      </c>
+      <c r="AG13">
+        <v>12</v>
+      </c>
+      <c r="AH13">
+        <v>7</v>
+      </c>
+      <c r="AI13">
+        <v>4</v>
+      </c>
+      <c r="AJ13">
+        <v>3</v>
+      </c>
+      <c r="AK13">
+        <v>4</v>
+      </c>
+      <c r="AL13">
+        <v>8</v>
+      </c>
+      <c r="AM13">
+        <v>4</v>
+      </c>
+      <c r="AN13">
+        <v>7</v>
+      </c>
+      <c r="AO13">
+        <v>9</v>
+      </c>
+      <c r="AP13">
+        <v>2</v>
+      </c>
+      <c r="AQ13">
+        <v>6</v>
+      </c>
+      <c r="AR13">
+        <v>9</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13">
+        <v>2</v>
+      </c>
+      <c r="AU13">
+        <v>-1</v>
+      </c>
+      <c r="AV13">
+        <v>5</v>
+      </c>
+      <c r="AW13">
+        <v>6</v>
+      </c>
+      <c r="AX13">
+        <v>4</v>
+      </c>
+      <c r="AY13">
+        <v>10</v>
+      </c>
+      <c r="AZ13">
+        <v>10</v>
+      </c>
+      <c r="BA13">
+        <v>16</v>
+      </c>
+      <c r="BB13">
+        <v>3</v>
+      </c>
+      <c r="BC13">
+        <v>6</v>
+      </c>
+      <c r="BD13">
+        <v>1</v>
+      </c>
+      <c r="BE13">
+        <v>13</v>
+      </c>
+      <c r="BF13">
+        <v>16</v>
+      </c>
+      <c r="BG13">
+        <v>7</v>
+      </c>
+      <c r="BH13">
+        <v>11</v>
+      </c>
+      <c r="BI13">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14" spans="1:61">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14">
+        <v>7</v>
+      </c>
+      <c r="N14">
+        <v>11</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>11</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>2</v>
+      </c>
+      <c r="X14">
+        <v>7</v>
+      </c>
+      <c r="Y14">
+        <v>6</v>
+      </c>
+      <c r="Z14">
+        <v>7</v>
+      </c>
+      <c r="AA14">
+        <v>9</v>
+      </c>
+      <c r="AB14">
+        <v>4</v>
+      </c>
+      <c r="AC14">
+        <v>15</v>
+      </c>
+      <c r="AD14">
+        <v>17</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>11</v>
+      </c>
+      <c r="AG14">
+        <v>7</v>
+      </c>
+      <c r="AH14">
+        <v>5</v>
+      </c>
+      <c r="AI14">
+        <v>7</v>
+      </c>
+      <c r="AJ14">
+        <v>17</v>
+      </c>
+      <c r="AK14">
+        <v>13</v>
+      </c>
+      <c r="AL14">
+        <v>6</v>
+      </c>
+      <c r="AM14">
+        <v>135</v>
+      </c>
+      <c r="AN14">
+        <v>9</v>
+      </c>
+      <c r="AO14">
+        <v>11</v>
+      </c>
+      <c r="AP14">
+        <v>11</v>
+      </c>
+      <c r="AQ14">
+        <v>-1</v>
+      </c>
+      <c r="AR14">
+        <v>4</v>
+      </c>
+      <c r="AS14">
+        <v>-1</v>
+      </c>
+      <c r="AT14">
+        <v>11</v>
+      </c>
+      <c r="AU14">
+        <v>-1</v>
+      </c>
+      <c r="AV14">
+        <v>15</v>
+      </c>
+      <c r="AW14">
+        <v>-1</v>
+      </c>
+      <c r="AX14">
+        <v>14</v>
+      </c>
+      <c r="AY14">
+        <v>3</v>
+      </c>
+      <c r="AZ14">
+        <v>20</v>
+      </c>
+      <c r="BA14">
+        <v>-1</v>
+      </c>
+      <c r="BB14">
+        <v>9</v>
+      </c>
+      <c r="BC14">
+        <v>-1</v>
+      </c>
+      <c r="BD14">
+        <v>7</v>
+      </c>
+      <c r="BE14">
+        <v>-1</v>
+      </c>
+      <c r="BF14">
+        <v>16</v>
+      </c>
+      <c r="BG14">
+        <v>-1</v>
+      </c>
+      <c r="BH14">
+        <v>14</v>
+      </c>
+      <c r="BI14">
+        <v>-1</v>
+      </c>
     </row>
     <row r="15" spans="1:61">
       <c r="A15" s="1"/>
@@ -3478,7 +3840,7 @@
   <dimension ref="A1:BQ30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6447,10 +6809,544 @@
       </c>
     </row>
     <row r="13" spans="1:69">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <f>distance!A13</f>
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>IF(AND(distance!B13&lt;80,distance!B13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>IF(AND(distance!C13&lt;80,distance!C13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>IF(AND(distance!D13&lt;80,distance!D13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f>IF(AND(distance!E13&lt;80,distance!E13&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>IF(AND(distance!F13&lt;80,distance!F13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>IF(AND(distance!G13&lt;80,distance!G13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f>IF(AND(distance!H13&lt;80,distance!H13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f>IF(AND(distance!I13&lt;80,distance!I13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f>IF(AND(distance!J13&lt;80,distance!J13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f>IF(AND(distance!K13&lt;80,distance!K13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f>IF(AND(distance!L13&lt;80,distance!L13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f>IF(AND(distance!M13&lt;80,distance!M13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f>IF(AND(distance!N13&lt;80,distance!N13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f>IF(AND(distance!O13&lt;80,distance!O13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <f>IF(AND(distance!P13&lt;80,distance!P13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <f>IF(AND(distance!Q13&lt;80,distance!Q13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <f>IF(AND(distance!R13&lt;80,distance!R13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <f>IF(AND(distance!S13&lt;80,distance!S13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <f>IF(AND(distance!T13&lt;80,distance!T13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <f>IF(AND(distance!U13&lt;80,distance!U13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <f>IF(AND(distance!V13&lt;80,distance!V13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <f>IF(AND(distance!W13&lt;80,distance!W13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <f>IF(AND(distance!X13&lt;80,distance!X13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <f>IF(AND(distance!Y13&lt;80,distance!Y13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <f>IF(AND(distance!Z13&lt;80,distance!Z13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <f>IF(AND(distance!AA13&lt;80,distance!AA13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <f>IF(AND(distance!AB13&lt;80,distance!AB13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <f>IF(AND(distance!AC13&lt;80,distance!AC13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD13">
+        <f>IF(AND(distance!AD13&lt;80,distance!AD13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE13">
+        <f>IF(AND(distance!AE13&lt;80,distance!AE13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <f>IF(AND(distance!AF13&lt;80,distance!AF13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <f>IF(AND(distance!AG13&lt;80,distance!AG13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <f>IF(AND(distance!AH13&lt;80,distance!AH13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <f>IF(AND(distance!AI13&lt;80,distance!AI13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ13">
+        <f>IF(AND(distance!AJ13&lt;80,distance!AJ13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK13">
+        <f>IF(AND(distance!AK13&lt;80,distance!AK13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <f>IF(AND(distance!AL13&lt;80,distance!AL13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM13">
+        <f>IF(AND(distance!AM13&lt;80,distance!AM13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN13">
+        <f>IF(AND(distance!AN13&lt;80,distance!AN13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO13">
+        <f>IF(AND(distance!AO13&lt;80,distance!AO13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AP13">
+        <f>IF(AND(distance!AP13&lt;80,distance!AP13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ13">
+        <f>IF(AND(distance!AQ13&lt;80,distance!AQ13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AR13">
+        <f>IF(AND(distance!AR13&lt;80,distance!AR13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AS13">
+        <f>IF(AND(distance!AS13&lt;80,distance!AS13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AT13">
+        <f>IF(AND(distance!AT13&lt;80,distance!AT13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU13">
+        <f>IF(AND(distance!AU13&lt;80,distance!AU13&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV13">
+        <f>IF(AND(distance!AV13&lt;80,distance!AV13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AW13">
+        <f>IF(AND(distance!AW13&lt;80,distance!AW13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AX13">
+        <f>IF(AND(distance!AX13&lt;80,distance!AX13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY13">
+        <f>IF(AND(distance!AY13&lt;80,distance!AY13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ13">
+        <f>IF(AND(distance!AZ13&lt;80,distance!AZ13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BA13">
+        <f>IF(AND(distance!BA13&lt;80,distance!BA13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BB13">
+        <f>IF(AND(distance!BB13&lt;80,distance!BB13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC13">
+        <f>IF(AND(distance!BC13&lt;80,distance!BC13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BD13">
+        <f>IF(AND(distance!BD13&lt;80,distance!BD13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE13">
+        <f>IF(AND(distance!BE13&lt;80,distance!BE13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BF13">
+        <f>IF(AND(distance!BF13&lt;80,distance!BF13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG13">
+        <f>IF(AND(distance!BG13&lt;80,distance!BG13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BH13">
+        <f>IF(AND(distance!BH13&lt;80,distance!BH13&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI13">
+        <f>IF(AND(distance!BI13&lt;80,distance!BI13&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BL13">
+        <f t="shared" ref="BL13:BL14" si="60">SUM(B13,D13,F13,H13,J13,L13,N13,P13,R13,T13)/COUNT(B13,D13,F13,H13,J13,L13,N13,P13,R13,T13)</f>
+        <v>1</v>
+      </c>
+      <c r="BM13">
+        <f t="shared" ref="BM13:BM14" si="61">SUM(C13,E13,G13,I13,K13,M13,O13,Q13,S13,U13)/COUNT(C13,E13,G13,I13,K13,M13,O13,Q13,S13,U13)</f>
+        <v>0.9</v>
+      </c>
+      <c r="BN13">
+        <f t="shared" ref="BN13:BN14" si="62">SUM(V13,X13,Z13,AB13,AD13,AF13,AH13,AJ13,AL13,AN13)/COUNT(V13,X13,Z13,AB13,AD13,AF13,AH13,AJ13,AL13,AN13)</f>
+        <v>1</v>
+      </c>
+      <c r="BO13">
+        <f t="shared" ref="BO13:BO14" si="63">SUM(W13,Y13,AA13,AC13,AE13,AG13,AI13,AK13,AM13,AO13)/COUNT(W13,Y13,AA13,AC13,AE13,AG13,AI13,AK13,AM13,AO13)</f>
+        <v>1</v>
+      </c>
+      <c r="BP13">
+        <f t="shared" ref="BP13:BP14" si="64">SUM(AP13,AR13,AT13,AV13,AX13,AZ13,BB13,BD13,BF13,BH13)/COUNT(AP13,AR13,AT13,AV13,AX13,AZ13,BB13,BD13,BF13,BH13)</f>
+        <v>1</v>
+      </c>
+      <c r="BQ13">
+        <f t="shared" ref="BQ13:BQ14" si="65">SUM(AQ13,AS13,AU13,AW13,AY13,BA13,BC13,BE13,BG13,BI13)/COUNT(AQ13,AS13,AU13,AW13,AY13,BA13,BC13,BE13,BG13,BI13)</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="14" spans="1:69">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <f>distance!A14</f>
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f>IF(AND(distance!B14&lt;80,distance!B14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f>IF(AND(distance!C14&lt;80,distance!C14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>IF(AND(distance!D14&lt;80,distance!D14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f>IF(AND(distance!E14&lt;80,distance!E14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>IF(AND(distance!F14&lt;80,distance!F14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f>IF(AND(distance!G14&lt;80,distance!G14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f>IF(AND(distance!H14&lt;80,distance!H14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f>IF(AND(distance!I14&lt;80,distance!I14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f>IF(AND(distance!J14&lt;80,distance!J14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f>IF(AND(distance!K14&lt;80,distance!K14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f>IF(AND(distance!L14&lt;80,distance!L14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f>IF(AND(distance!M14&lt;80,distance!M14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f>IF(AND(distance!N14&lt;80,distance!N14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <f>IF(AND(distance!O14&lt;80,distance!O14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <f>IF(AND(distance!P14&lt;80,distance!P14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <f>IF(AND(distance!Q14&lt;80,distance!Q14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <f>IF(AND(distance!R14&lt;80,distance!R14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <f>IF(AND(distance!S14&lt;80,distance!S14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <f>IF(AND(distance!T14&lt;80,distance!T14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <f>IF(AND(distance!U14&lt;80,distance!U14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <f>IF(AND(distance!V14&lt;80,distance!V14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <f>IF(AND(distance!W14&lt;80,distance!W14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <f>IF(AND(distance!X14&lt;80,distance!X14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <f>IF(AND(distance!Y14&lt;80,distance!Y14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <f>IF(AND(distance!Z14&lt;80,distance!Z14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <f>IF(AND(distance!AA14&lt;80,distance!AA14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <f>IF(AND(distance!AB14&lt;80,distance!AB14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <f>IF(AND(distance!AC14&lt;80,distance!AC14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <f>IF(AND(distance!AD14&lt;80,distance!AD14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <f>IF(AND(distance!AE14&lt;80,distance!AE14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <f>IF(AND(distance!AF14&lt;80,distance!AF14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <f>IF(AND(distance!AG14&lt;80,distance!AG14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <f>IF(AND(distance!AH14&lt;80,distance!AH14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <f>IF(AND(distance!AI14&lt;80,distance!AI14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ14">
+        <f>IF(AND(distance!AJ14&lt;80,distance!AJ14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AK14">
+        <f>IF(AND(distance!AK14&lt;80,distance!AK14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <f>IF(AND(distance!AL14&lt;80,distance!AL14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AM14">
+        <f>IF(AND(distance!AM14&lt;80,distance!AM14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <f>IF(AND(distance!AN14&lt;80,distance!AN14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO14">
+        <f>IF(AND(distance!AO14&lt;80,distance!AO14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AP14">
+        <f>IF(AND(distance!AP14&lt;80,distance!AP14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ14">
+        <f>IF(AND(distance!AQ14&lt;80,distance!AQ14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <f>IF(AND(distance!AR14&lt;80,distance!AR14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AS14">
+        <f>IF(AND(distance!AS14&lt;80,distance!AS14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <f>IF(AND(distance!AT14&lt;80,distance!AT14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU14">
+        <f>IF(AND(distance!AU14&lt;80,distance!AU14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <f>IF(AND(distance!AV14&lt;80,distance!AV14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AW14">
+        <f>IF(AND(distance!AW14&lt;80,distance!AW14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <f>IF(AND(distance!AX14&lt;80,distance!AX14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AY14">
+        <f>IF(AND(distance!AY14&lt;80,distance!AY14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ14">
+        <f>IF(AND(distance!AZ14&lt;80,distance!AZ14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BA14">
+        <f>IF(AND(distance!BA14&lt;80,distance!BA14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <f>IF(AND(distance!BB14&lt;80,distance!BB14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BC14">
+        <f>IF(AND(distance!BC14&lt;80,distance!BC14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <f>IF(AND(distance!BD14&lt;80,distance!BD14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BE14">
+        <f>IF(AND(distance!BE14&lt;80,distance!BE14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF14">
+        <f>IF(AND(distance!BF14&lt;80,distance!BF14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BG14">
+        <f>IF(AND(distance!BG14&lt;80,distance!BG14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BH14">
+        <f>IF(AND(distance!BH14&lt;80,distance!BH14&gt;=0),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BI14">
+        <f>IF(AND(distance!BI14&lt;80,distance!BI14&gt;=0),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BL14">
+        <f t="shared" si="60"/>
+        <v>1</v>
+      </c>
+      <c r="BM14">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+      <c r="BN14">
+        <f t="shared" si="62"/>
+        <v>1</v>
+      </c>
+      <c r="BO14">
+        <f t="shared" si="63"/>
+        <v>0.9</v>
+      </c>
+      <c r="BP14">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="BQ14">
+        <f t="shared" si="65"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="15" spans="1:69">
       <c r="A15" s="1"/>
@@ -6464,23 +7360,23 @@
         <v>AF</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" ref="C20" si="60">C1</f>
+        <f t="shared" ref="C20" si="66">C1</f>
         <v>AF</v>
       </c>
       <c r="V20" t="str">
-        <f t="shared" ref="V20:AQ20" si="61">V1</f>
+        <f t="shared" ref="V20:AQ20" si="67">V1</f>
         <v>SL</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
         <v>SL</v>
       </c>
       <c r="AP20" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
         <v>H</v>
       </c>
       <c r="AQ20" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
         <v>H</v>
       </c>
     </row>
@@ -6490,23 +7386,23 @@
         <v>(para)foveal</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" ref="C21" si="62">C3</f>
+        <f t="shared" ref="C21" si="68">C3</f>
         <v>peripheral</v>
       </c>
       <c r="V21" t="str">
-        <f t="shared" ref="V21:AQ21" si="63">V3</f>
+        <f t="shared" ref="V21:AQ21" si="69">V3</f>
         <v>(para)foveal</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>peripheral</v>
       </c>
       <c r="AP21" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>(para)foveal</v>
       </c>
       <c r="AQ21" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>peripheral</v>
       </c>
     </row>
@@ -6516,24 +7412,24 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:AQ22" si="64">SUM(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)/COUNT(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)</f>
-        <v>0.96202531645569622</v>
+        <f t="shared" ref="C22:AQ22" si="70">SUM(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)/COUNT(C5:C17,E5:E17,G5:G17,I5:I17,K5:K17,M5:M17,O5:O17,Q5:Q17,S5:S17,U5:U17)</f>
+        <v>0.95959595959595956</v>
       </c>
       <c r="V22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="W22">
-        <f t="shared" si="64"/>
-        <v>0.94871794871794868</v>
+        <f t="shared" si="70"/>
+        <v>0.94897959183673475</v>
       </c>
       <c r="AP22">
-        <f t="shared" si="64"/>
-        <v>0.9375</v>
+        <f t="shared" si="70"/>
+        <v>0.95</v>
       </c>
       <c r="AQ22">
-        <f t="shared" si="64"/>
-        <v>0.38750000000000001</v>
+        <f t="shared" si="70"/>
+        <v>0.4</v>
       </c>
     </row>
     <row r="28" spans="1:43">
@@ -6565,7 +7461,7 @@
       </c>
       <c r="D29">
         <f>AP22</f>
-        <v>0.9375</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="30" spans="1:43">
@@ -6575,15 +7471,15 @@
       </c>
       <c r="B30">
         <f>C22</f>
-        <v>0.96202531645569622</v>
+        <v>0.95959595959595956</v>
       </c>
       <c r="C30">
         <f>W22</f>
-        <v>0.94871794871794868</v>
+        <v>0.94897959183673475</v>
       </c>
       <c r="D30">
         <f>AQ22</f>
-        <v>0.38750000000000001</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -6597,8 +7493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BQ40" sqref="BQ40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9075,6 +9971,378 @@
         <v>782</v>
       </c>
     </row>
+    <row r="13" spans="1:61">
+      <c r="A13">
+        <f>error!A13</f>
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1009</v>
+      </c>
+      <c r="C13">
+        <v>1283</v>
+      </c>
+      <c r="D13">
+        <v>999</v>
+      </c>
+      <c r="E13">
+        <v>821</v>
+      </c>
+      <c r="F13">
+        <v>863</v>
+      </c>
+      <c r="G13">
+        <v>1498</v>
+      </c>
+      <c r="H13">
+        <v>1589</v>
+      </c>
+      <c r="I13">
+        <v>1136</v>
+      </c>
+      <c r="J13">
+        <v>1010</v>
+      </c>
+      <c r="K13">
+        <v>1245</v>
+      </c>
+      <c r="L13">
+        <v>919</v>
+      </c>
+      <c r="M13">
+        <v>2867</v>
+      </c>
+      <c r="N13">
+        <v>1212</v>
+      </c>
+      <c r="O13">
+        <v>1516</v>
+      </c>
+      <c r="P13">
+        <v>801</v>
+      </c>
+      <c r="Q13">
+        <v>944</v>
+      </c>
+      <c r="R13">
+        <v>1184</v>
+      </c>
+      <c r="S13">
+        <v>1295</v>
+      </c>
+      <c r="T13">
+        <v>1454</v>
+      </c>
+      <c r="U13">
+        <v>1389</v>
+      </c>
+      <c r="V13">
+        <v>1113</v>
+      </c>
+      <c r="W13">
+        <v>1396</v>
+      </c>
+      <c r="X13">
+        <v>986</v>
+      </c>
+      <c r="Y13">
+        <v>1335</v>
+      </c>
+      <c r="Z13">
+        <v>1046</v>
+      </c>
+      <c r="AA13">
+        <v>1042</v>
+      </c>
+      <c r="AB13">
+        <v>1529</v>
+      </c>
+      <c r="AC13">
+        <v>1596</v>
+      </c>
+      <c r="AD13">
+        <v>1134</v>
+      </c>
+      <c r="AE13">
+        <v>1508</v>
+      </c>
+      <c r="AF13">
+        <v>824</v>
+      </c>
+      <c r="AG13">
+        <v>1080</v>
+      </c>
+      <c r="AH13">
+        <v>623</v>
+      </c>
+      <c r="AI13">
+        <v>1266</v>
+      </c>
+      <c r="AJ13">
+        <v>986</v>
+      </c>
+      <c r="AK13">
+        <v>1079</v>
+      </c>
+      <c r="AL13">
+        <v>1313</v>
+      </c>
+      <c r="AM13">
+        <v>963</v>
+      </c>
+      <c r="AN13">
+        <v>922</v>
+      </c>
+      <c r="AO13">
+        <v>1171</v>
+      </c>
+      <c r="AP13">
+        <v>721</v>
+      </c>
+      <c r="AQ13">
+        <v>3370</v>
+      </c>
+      <c r="AR13">
+        <v>1930</v>
+      </c>
+      <c r="AS13">
+        <v>3259</v>
+      </c>
+      <c r="AT13">
+        <v>3841</v>
+      </c>
+      <c r="AU13">
+        <v>5012</v>
+      </c>
+      <c r="AV13">
+        <v>1044</v>
+      </c>
+      <c r="AW13">
+        <v>4902</v>
+      </c>
+      <c r="AX13">
+        <v>587</v>
+      </c>
+      <c r="AY13">
+        <v>5018</v>
+      </c>
+      <c r="AZ13">
+        <v>664</v>
+      </c>
+      <c r="BA13">
+        <v>4199</v>
+      </c>
+      <c r="BB13">
+        <v>1051</v>
+      </c>
+      <c r="BC13">
+        <v>1219</v>
+      </c>
+      <c r="BD13">
+        <v>1000</v>
+      </c>
+      <c r="BE13">
+        <v>2266</v>
+      </c>
+      <c r="BF13">
+        <v>614</v>
+      </c>
+      <c r="BG13">
+        <v>3350</v>
+      </c>
+      <c r="BH13">
+        <v>957</v>
+      </c>
+      <c r="BI13">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61">
+      <c r="A14">
+        <f>error!A14</f>
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>828</v>
+      </c>
+      <c r="C14">
+        <v>3267</v>
+      </c>
+      <c r="D14">
+        <v>2203</v>
+      </c>
+      <c r="E14">
+        <v>4685</v>
+      </c>
+      <c r="F14">
+        <v>1328</v>
+      </c>
+      <c r="G14">
+        <v>2550</v>
+      </c>
+      <c r="H14">
+        <v>1399</v>
+      </c>
+      <c r="I14">
+        <v>1432</v>
+      </c>
+      <c r="J14">
+        <v>1161</v>
+      </c>
+      <c r="K14">
+        <v>1166</v>
+      </c>
+      <c r="L14">
+        <v>1286</v>
+      </c>
+      <c r="M14">
+        <v>3831</v>
+      </c>
+      <c r="N14">
+        <v>1199</v>
+      </c>
+      <c r="O14">
+        <v>4301</v>
+      </c>
+      <c r="P14">
+        <v>1599</v>
+      </c>
+      <c r="Q14">
+        <v>2433</v>
+      </c>
+      <c r="R14">
+        <v>898</v>
+      </c>
+      <c r="S14">
+        <v>1712</v>
+      </c>
+      <c r="T14">
+        <v>1099</v>
+      </c>
+      <c r="U14">
+        <v>2667</v>
+      </c>
+      <c r="V14">
+        <v>1196</v>
+      </c>
+      <c r="W14">
+        <v>998</v>
+      </c>
+      <c r="X14">
+        <v>1417</v>
+      </c>
+      <c r="Y14">
+        <v>2011</v>
+      </c>
+      <c r="Z14">
+        <v>1446</v>
+      </c>
+      <c r="AA14">
+        <v>2247</v>
+      </c>
+      <c r="AB14">
+        <v>1417</v>
+      </c>
+      <c r="AC14">
+        <v>1213</v>
+      </c>
+      <c r="AD14">
+        <v>1814</v>
+      </c>
+      <c r="AE14">
+        <v>1219</v>
+      </c>
+      <c r="AF14">
+        <v>1296</v>
+      </c>
+      <c r="AG14">
+        <v>1980</v>
+      </c>
+      <c r="AH14">
+        <v>1559</v>
+      </c>
+      <c r="AI14">
+        <v>2147</v>
+      </c>
+      <c r="AJ14">
+        <v>1780</v>
+      </c>
+      <c r="AK14">
+        <v>963</v>
+      </c>
+      <c r="AL14">
+        <v>1596</v>
+      </c>
+      <c r="AM14">
+        <v>729</v>
+      </c>
+      <c r="AN14">
+        <v>846</v>
+      </c>
+      <c r="AO14">
+        <v>1663</v>
+      </c>
+      <c r="AP14">
+        <v>3403</v>
+      </c>
+      <c r="AQ14">
+        <v>5018</v>
+      </c>
+      <c r="AR14">
+        <v>2215</v>
+      </c>
+      <c r="AS14">
+        <v>5001</v>
+      </c>
+      <c r="AT14">
+        <v>1251</v>
+      </c>
+      <c r="AU14">
+        <v>5001</v>
+      </c>
+      <c r="AV14">
+        <v>831</v>
+      </c>
+      <c r="AW14">
+        <v>5001</v>
+      </c>
+      <c r="AX14">
+        <v>1882</v>
+      </c>
+      <c r="AY14">
+        <v>5004</v>
+      </c>
+      <c r="AZ14">
+        <v>2569</v>
+      </c>
+      <c r="BA14">
+        <v>5001</v>
+      </c>
+      <c r="BB14">
+        <v>1198</v>
+      </c>
+      <c r="BC14">
+        <v>5002</v>
+      </c>
+      <c r="BD14">
+        <v>911</v>
+      </c>
+      <c r="BE14">
+        <v>5005</v>
+      </c>
+      <c r="BF14">
+        <v>1334</v>
+      </c>
+      <c r="BG14">
+        <v>5001</v>
+      </c>
+      <c r="BH14">
+        <v>2683</v>
+      </c>
+      <c r="BI14">
+        <v>5005</v>
+      </c>
+    </row>
     <row r="26" spans="1:69">
       <c r="A26" t="s">
         <v>35</v>
@@ -10138,7 +11406,7 @@
     </row>
     <row r="31" spans="1:69">
       <c r="A31">
-        <f t="shared" ref="A31:A37" si="7">A6</f>
+        <f t="shared" ref="A31:A39" si="7">A6</f>
         <v>3</v>
       </c>
       <c r="B31">
@@ -11732,27 +13000,27 @@
         <v/>
       </c>
       <c r="BL36">
-        <f t="shared" ref="BL36:BL38" si="14">AVERAGE(B36,D36,F36,H36,J36,L36,N36,P36,R36,T36)</f>
+        <f t="shared" ref="BL36:BL37" si="14">AVERAGE(B36,D36,F36,H36,J36,L36,N36,P36,R36,T36)</f>
         <v>1146.8</v>
       </c>
       <c r="BM36">
-        <f t="shared" ref="BM36:BM38" si="15">AVERAGE(C36,E36,G36,I36,K36,M36,O36,Q36,S36,U36)</f>
+        <f t="shared" ref="BM36:BM37" si="15">AVERAGE(C36,E36,G36,I36,K36,M36,O36,Q36,S36,U36)</f>
         <v>1370.2</v>
       </c>
       <c r="BN36">
-        <f t="shared" ref="BN36:BN38" si="16">AVERAGE(V36,X36,Z36,AB36,AD36,AF36,AH36,AJ36,AL36,AN36)</f>
+        <f t="shared" ref="BN36:BN37" si="16">AVERAGE(V36,X36,Z36,AB36,AD36,AF36,AH36,AJ36,AL36,AN36)</f>
         <v>1168.9000000000001</v>
       </c>
       <c r="BO36">
-        <f t="shared" ref="BO36:BO38" si="17">AVERAGE(W36,Y36,AA36,AC36,AE36,AG36,AI36,AK36,AM36,AO36)</f>
+        <f t="shared" ref="BO36:BO37" si="17">AVERAGE(W36,Y36,AA36,AC36,AE36,AG36,AI36,AK36,AM36,AO36)</f>
         <v>1520.2</v>
       </c>
       <c r="BP36">
-        <f t="shared" ref="BP36:BP38" si="18">AVERAGE(AP36,AR36,AT36,AV36,AX36,AZ36,BB36,BD36,BF36,BH36)</f>
+        <f t="shared" ref="BP36:BP37" si="18">AVERAGE(AP36,AR36,AT36,AV36,AX36,AZ36,BB36,BD36,BF36,BH36)</f>
         <v>1142.4000000000001</v>
       </c>
       <c r="BQ36">
-        <f t="shared" ref="BQ36:BQ38" si="19">AVERAGE(AQ36,AS36,AU36,AW36,AY36,BA36,BC36,BE36,BG36,BI36)</f>
+        <f t="shared" ref="BQ36:BQ37" si="19">AVERAGE(AQ36,AS36,AU36,AW36,AY36,BA36,BC36,BE36,BG36,BI36)</f>
         <v>1282</v>
       </c>
     </row>
@@ -12027,241 +13295,245 @@
       </c>
     </row>
     <row r="38" spans="1:69">
-      <c r="B38" t="str">
+      <c r="A38">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="B38">
         <f>IF(error!B13=1,time!B13,"")</f>
-        <v/>
-      </c>
-      <c r="C38" t="str">
+        <v>1009</v>
+      </c>
+      <c r="C38">
         <f>IF(error!C13=1,time!C13,"")</f>
-        <v/>
-      </c>
-      <c r="D38" t="str">
+        <v>1283</v>
+      </c>
+      <c r="D38">
         <f>IF(error!D13=1,time!D13,"")</f>
-        <v/>
+        <v>999</v>
       </c>
       <c r="E38" t="str">
         <f>IF(error!E13=1,time!E13,"")</f>
         <v/>
       </c>
-      <c r="F38" t="str">
+      <c r="F38">
         <f>IF(error!F13=1,time!F13,"")</f>
-        <v/>
-      </c>
-      <c r="G38" t="str">
+        <v>863</v>
+      </c>
+      <c r="G38">
         <f>IF(error!G13=1,time!G13,"")</f>
-        <v/>
-      </c>
-      <c r="H38" t="str">
+        <v>1498</v>
+      </c>
+      <c r="H38">
         <f>IF(error!H13=1,time!H13,"")</f>
-        <v/>
-      </c>
-      <c r="I38" t="str">
+        <v>1589</v>
+      </c>
+      <c r="I38">
         <f>IF(error!I13=1,time!I13,"")</f>
-        <v/>
-      </c>
-      <c r="J38" t="str">
+        <v>1136</v>
+      </c>
+      <c r="J38">
         <f>IF(error!J13=1,time!J13,"")</f>
-        <v/>
-      </c>
-      <c r="K38" t="str">
+        <v>1010</v>
+      </c>
+      <c r="K38">
         <f>IF(error!K13=1,time!K13,"")</f>
-        <v/>
-      </c>
-      <c r="L38" t="str">
+        <v>1245</v>
+      </c>
+      <c r="L38">
         <f>IF(error!L13=1,time!L13,"")</f>
-        <v/>
-      </c>
-      <c r="M38" t="str">
+        <v>919</v>
+      </c>
+      <c r="M38">
         <f>IF(error!M13=1,time!M13,"")</f>
-        <v/>
-      </c>
-      <c r="N38" t="str">
+        <v>2867</v>
+      </c>
+      <c r="N38">
         <f>IF(error!N13=1,time!N13,"")</f>
-        <v/>
-      </c>
-      <c r="O38" t="str">
+        <v>1212</v>
+      </c>
+      <c r="O38">
         <f>IF(error!O13=1,time!O13,"")</f>
-        <v/>
-      </c>
-      <c r="P38" t="str">
+        <v>1516</v>
+      </c>
+      <c r="P38">
         <f>IF(error!P13=1,time!P13,"")</f>
-        <v/>
-      </c>
-      <c r="Q38" t="str">
+        <v>801</v>
+      </c>
+      <c r="Q38">
         <f>IF(error!Q13=1,time!Q13,"")</f>
-        <v/>
-      </c>
-      <c r="R38" t="str">
+        <v>944</v>
+      </c>
+      <c r="R38">
         <f>IF(error!R13=1,time!R13,"")</f>
-        <v/>
-      </c>
-      <c r="S38" t="str">
+        <v>1184</v>
+      </c>
+      <c r="S38">
         <f>IF(error!S13=1,time!S13,"")</f>
-        <v/>
-      </c>
-      <c r="T38" t="str">
+        <v>1295</v>
+      </c>
+      <c r="T38">
         <f>IF(error!T13=1,time!T13,"")</f>
-        <v/>
-      </c>
-      <c r="U38" t="str">
+        <v>1454</v>
+      </c>
+      <c r="U38">
         <f>IF(error!U13=1,time!U13,"")</f>
-        <v/>
-      </c>
-      <c r="V38" t="str">
+        <v>1389</v>
+      </c>
+      <c r="V38">
         <f>IF(error!V13=1,time!V13,"")</f>
-        <v/>
-      </c>
-      <c r="W38" t="str">
+        <v>1113</v>
+      </c>
+      <c r="W38">
         <f>IF(error!W13=1,time!W13,"")</f>
-        <v/>
-      </c>
-      <c r="X38" t="str">
+        <v>1396</v>
+      </c>
+      <c r="X38">
         <f>IF(error!X13=1,time!X13,"")</f>
-        <v/>
-      </c>
-      <c r="Y38" t="str">
+        <v>986</v>
+      </c>
+      <c r="Y38">
         <f>IF(error!Y13=1,time!Y13,"")</f>
-        <v/>
-      </c>
-      <c r="Z38" t="str">
+        <v>1335</v>
+      </c>
+      <c r="Z38">
         <f>IF(error!Z13=1,time!Z13,"")</f>
-        <v/>
-      </c>
-      <c r="AA38" t="str">
+        <v>1046</v>
+      </c>
+      <c r="AA38">
         <f>IF(error!AA13=1,time!AA13,"")</f>
-        <v/>
-      </c>
-      <c r="AB38" t="str">
+        <v>1042</v>
+      </c>
+      <c r="AB38">
         <f>IF(error!AB13=1,time!AB13,"")</f>
-        <v/>
-      </c>
-      <c r="AC38" t="str">
+        <v>1529</v>
+      </c>
+      <c r="AC38">
         <f>IF(error!AC13=1,time!AC13,"")</f>
-        <v/>
-      </c>
-      <c r="AD38" t="str">
+        <v>1596</v>
+      </c>
+      <c r="AD38">
         <f>IF(error!AD13=1,time!AD13,"")</f>
-        <v/>
-      </c>
-      <c r="AE38" t="str">
+        <v>1134</v>
+      </c>
+      <c r="AE38">
         <f>IF(error!AE13=1,time!AE13,"")</f>
-        <v/>
-      </c>
-      <c r="AF38" t="str">
+        <v>1508</v>
+      </c>
+      <c r="AF38">
         <f>IF(error!AF13=1,time!AF13,"")</f>
-        <v/>
-      </c>
-      <c r="AG38" t="str">
+        <v>824</v>
+      </c>
+      <c r="AG38">
         <f>IF(error!AG13=1,time!AG13,"")</f>
-        <v/>
-      </c>
-      <c r="AH38" t="str">
+        <v>1080</v>
+      </c>
+      <c r="AH38">
         <f>IF(error!AH13=1,time!AH13,"")</f>
-        <v/>
-      </c>
-      <c r="AI38" t="str">
+        <v>623</v>
+      </c>
+      <c r="AI38">
         <f>IF(error!AI13=1,time!AI13,"")</f>
-        <v/>
-      </c>
-      <c r="AJ38" t="str">
+        <v>1266</v>
+      </c>
+      <c r="AJ38">
         <f>IF(error!AJ13=1,time!AJ13,"")</f>
-        <v/>
-      </c>
-      <c r="AK38" t="str">
+        <v>986</v>
+      </c>
+      <c r="AK38">
         <f>IF(error!AK13=1,time!AK13,"")</f>
-        <v/>
-      </c>
-      <c r="AL38" t="str">
+        <v>1079</v>
+      </c>
+      <c r="AL38">
         <f>IF(error!AL13=1,time!AL13,"")</f>
-        <v/>
-      </c>
-      <c r="AM38" t="str">
+        <v>1313</v>
+      </c>
+      <c r="AM38">
         <f>IF(error!AM13=1,time!AM13,"")</f>
-        <v/>
-      </c>
-      <c r="AN38" t="str">
+        <v>963</v>
+      </c>
+      <c r="AN38">
         <f>IF(error!AN13=1,time!AN13,"")</f>
-        <v/>
-      </c>
-      <c r="AO38" t="str">
+        <v>922</v>
+      </c>
+      <c r="AO38">
         <f>IF(error!AO13=1,time!AO13,"")</f>
-        <v/>
-      </c>
-      <c r="AP38" t="str">
+        <v>1171</v>
+      </c>
+      <c r="AP38">
         <f>IF(error!AP13=1,time!AP13,"")</f>
-        <v/>
-      </c>
-      <c r="AQ38" t="str">
+        <v>721</v>
+      </c>
+      <c r="AQ38">
         <f>IF(error!AQ13=1,time!AQ13,"")</f>
-        <v/>
-      </c>
-      <c r="AR38" t="str">
+        <v>3370</v>
+      </c>
+      <c r="AR38">
         <f>IF(error!AR13=1,time!AR13,"")</f>
-        <v/>
-      </c>
-      <c r="AS38" t="str">
+        <v>1930</v>
+      </c>
+      <c r="AS38">
         <f>IF(error!AS13=1,time!AS13,"")</f>
-        <v/>
-      </c>
-      <c r="AT38" t="str">
+        <v>3259</v>
+      </c>
+      <c r="AT38">
         <f>IF(error!AT13=1,time!AT13,"")</f>
-        <v/>
+        <v>3841</v>
       </c>
       <c r="AU38" t="str">
         <f>IF(error!AU13=1,time!AU13,"")</f>
         <v/>
       </c>
-      <c r="AV38" t="str">
+      <c r="AV38">
         <f>IF(error!AV13=1,time!AV13,"")</f>
-        <v/>
-      </c>
-      <c r="AW38" t="str">
+        <v>1044</v>
+      </c>
+      <c r="AW38">
         <f>IF(error!AW13=1,time!AW13,"")</f>
-        <v/>
-      </c>
-      <c r="AX38" t="str">
+        <v>4902</v>
+      </c>
+      <c r="AX38">
         <f>IF(error!AX13=1,time!AX13,"")</f>
-        <v/>
-      </c>
-      <c r="AY38" t="str">
+        <v>587</v>
+      </c>
+      <c r="AY38">
         <f>IF(error!AY13=1,time!AY13,"")</f>
-        <v/>
-      </c>
-      <c r="AZ38" t="str">
+        <v>5018</v>
+      </c>
+      <c r="AZ38">
         <f>IF(error!AZ13=1,time!AZ13,"")</f>
-        <v/>
-      </c>
-      <c r="BA38" t="str">
+        <v>664</v>
+      </c>
+      <c r="BA38">
         <f>IF(error!BA13=1,time!BA13,"")</f>
-        <v/>
-      </c>
-      <c r="BB38" t="str">
+        <v>4199</v>
+      </c>
+      <c r="BB38">
         <f>IF(error!BB13=1,time!BB13,"")</f>
-        <v/>
-      </c>
-      <c r="BC38" t="str">
+        <v>1051</v>
+      </c>
+      <c r="BC38">
         <f>IF(error!BC13=1,time!BC13,"")</f>
-        <v/>
-      </c>
-      <c r="BD38" t="str">
+        <v>1219</v>
+      </c>
+      <c r="BD38">
         <f>IF(error!BD13=1,time!BD13,"")</f>
-        <v/>
-      </c>
-      <c r="BE38" t="str">
+        <v>1000</v>
+      </c>
+      <c r="BE38">
         <f>IF(error!BE13=1,time!BE13,"")</f>
-        <v/>
-      </c>
-      <c r="BF38" t="str">
+        <v>2266</v>
+      </c>
+      <c r="BF38">
         <f>IF(error!BF13=1,time!BF13,"")</f>
-        <v/>
-      </c>
-      <c r="BG38" t="str">
+        <v>614</v>
+      </c>
+      <c r="BG38">
         <f>IF(error!BG13=1,time!BG13,"")</f>
-        <v/>
-      </c>
-      <c r="BH38" t="str">
+        <v>3350</v>
+      </c>
+      <c r="BH38">
         <f>IF(error!BH13=1,time!BH13,"")</f>
-        <v/>
+        <v>957</v>
       </c>
       <c r="BI38" t="str">
         <f>IF(error!BI13=1,time!BI13,"")</f>
@@ -12269,241 +13541,245 @@
       </c>
     </row>
     <row r="39" spans="1:69">
-      <c r="B39" t="str">
+      <c r="A39">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="B39">
         <f>IF(error!B14=1,time!B14,"")</f>
-        <v/>
-      </c>
-      <c r="C39" t="str">
+        <v>828</v>
+      </c>
+      <c r="C39">
         <f>IF(error!C14=1,time!C14,"")</f>
-        <v/>
-      </c>
-      <c r="D39" t="str">
+        <v>3267</v>
+      </c>
+      <c r="D39">
         <f>IF(error!D14=1,time!D14,"")</f>
-        <v/>
-      </c>
-      <c r="E39" t="str">
+        <v>2203</v>
+      </c>
+      <c r="E39">
         <f>IF(error!E14=1,time!E14,"")</f>
-        <v/>
-      </c>
-      <c r="F39" t="str">
+        <v>4685</v>
+      </c>
+      <c r="F39">
         <f>IF(error!F14=1,time!F14,"")</f>
-        <v/>
-      </c>
-      <c r="G39" t="str">
+        <v>1328</v>
+      </c>
+      <c r="G39">
         <f>IF(error!G14=1,time!G14,"")</f>
-        <v/>
-      </c>
-      <c r="H39" t="str">
+        <v>2550</v>
+      </c>
+      <c r="H39">
         <f>IF(error!H14=1,time!H14,"")</f>
-        <v/>
-      </c>
-      <c r="I39" t="str">
+        <v>1399</v>
+      </c>
+      <c r="I39">
         <f>IF(error!I14=1,time!I14,"")</f>
-        <v/>
-      </c>
-      <c r="J39" t="str">
+        <v>1432</v>
+      </c>
+      <c r="J39">
         <f>IF(error!J14=1,time!J14,"")</f>
-        <v/>
-      </c>
-      <c r="K39" t="str">
+        <v>1161</v>
+      </c>
+      <c r="K39">
         <f>IF(error!K14=1,time!K14,"")</f>
-        <v/>
-      </c>
-      <c r="L39" t="str">
+        <v>1166</v>
+      </c>
+      <c r="L39">
         <f>IF(error!L14=1,time!L14,"")</f>
-        <v/>
-      </c>
-      <c r="M39" t="str">
+        <v>1286</v>
+      </c>
+      <c r="M39">
         <f>IF(error!M14=1,time!M14,"")</f>
-        <v/>
-      </c>
-      <c r="N39" t="str">
+        <v>3831</v>
+      </c>
+      <c r="N39">
         <f>IF(error!N14=1,time!N14,"")</f>
-        <v/>
-      </c>
-      <c r="O39" t="str">
+        <v>1199</v>
+      </c>
+      <c r="O39">
         <f>IF(error!O14=1,time!O14,"")</f>
-        <v/>
-      </c>
-      <c r="P39" t="str">
+        <v>4301</v>
+      </c>
+      <c r="P39">
         <f>IF(error!P14=1,time!P14,"")</f>
-        <v/>
-      </c>
-      <c r="Q39" t="str">
+        <v>1599</v>
+      </c>
+      <c r="Q39">
         <f>IF(error!Q14=1,time!Q14,"")</f>
-        <v/>
-      </c>
-      <c r="R39" t="str">
+        <v>2433</v>
+      </c>
+      <c r="R39">
         <f>IF(error!R14=1,time!R14,"")</f>
-        <v/>
-      </c>
-      <c r="S39" t="str">
+        <v>898</v>
+      </c>
+      <c r="S39">
         <f>IF(error!S14=1,time!S14,"")</f>
-        <v/>
-      </c>
-      <c r="T39" t="str">
+        <v>1712</v>
+      </c>
+      <c r="T39">
         <f>IF(error!T14=1,time!T14,"")</f>
-        <v/>
-      </c>
-      <c r="U39" t="str">
+        <v>1099</v>
+      </c>
+      <c r="U39">
         <f>IF(error!U14=1,time!U14,"")</f>
-        <v/>
-      </c>
-      <c r="V39" t="str">
+        <v>2667</v>
+      </c>
+      <c r="V39">
         <f>IF(error!V14=1,time!V14,"")</f>
-        <v/>
-      </c>
-      <c r="W39" t="str">
+        <v>1196</v>
+      </c>
+      <c r="W39">
         <f>IF(error!W14=1,time!W14,"")</f>
-        <v/>
-      </c>
-      <c r="X39" t="str">
+        <v>998</v>
+      </c>
+      <c r="X39">
         <f>IF(error!X14=1,time!X14,"")</f>
-        <v/>
-      </c>
-      <c r="Y39" t="str">
+        <v>1417</v>
+      </c>
+      <c r="Y39">
         <f>IF(error!Y14=1,time!Y14,"")</f>
-        <v/>
-      </c>
-      <c r="Z39" t="str">
+        <v>2011</v>
+      </c>
+      <c r="Z39">
         <f>IF(error!Z14=1,time!Z14,"")</f>
-        <v/>
-      </c>
-      <c r="AA39" t="str">
+        <v>1446</v>
+      </c>
+      <c r="AA39">
         <f>IF(error!AA14=1,time!AA14,"")</f>
-        <v/>
-      </c>
-      <c r="AB39" t="str">
+        <v>2247</v>
+      </c>
+      <c r="AB39">
         <f>IF(error!AB14=1,time!AB14,"")</f>
-        <v/>
-      </c>
-      <c r="AC39" t="str">
+        <v>1417</v>
+      </c>
+      <c r="AC39">
         <f>IF(error!AC14=1,time!AC14,"")</f>
-        <v/>
-      </c>
-      <c r="AD39" t="str">
+        <v>1213</v>
+      </c>
+      <c r="AD39">
         <f>IF(error!AD14=1,time!AD14,"")</f>
-        <v/>
-      </c>
-      <c r="AE39" t="str">
+        <v>1814</v>
+      </c>
+      <c r="AE39">
         <f>IF(error!AE14=1,time!AE14,"")</f>
-        <v/>
-      </c>
-      <c r="AF39" t="str">
+        <v>1219</v>
+      </c>
+      <c r="AF39">
         <f>IF(error!AF14=1,time!AF14,"")</f>
-        <v/>
-      </c>
-      <c r="AG39" t="str">
+        <v>1296</v>
+      </c>
+      <c r="AG39">
         <f>IF(error!AG14=1,time!AG14,"")</f>
-        <v/>
-      </c>
-      <c r="AH39" t="str">
+        <v>1980</v>
+      </c>
+      <c r="AH39">
         <f>IF(error!AH14=1,time!AH14,"")</f>
-        <v/>
-      </c>
-      <c r="AI39" t="str">
+        <v>1559</v>
+      </c>
+      <c r="AI39">
         <f>IF(error!AI14=1,time!AI14,"")</f>
-        <v/>
-      </c>
-      <c r="AJ39" t="str">
+        <v>2147</v>
+      </c>
+      <c r="AJ39">
         <f>IF(error!AJ14=1,time!AJ14,"")</f>
-        <v/>
-      </c>
-      <c r="AK39" t="str">
+        <v>1780</v>
+      </c>
+      <c r="AK39">
         <f>IF(error!AK14=1,time!AK14,"")</f>
-        <v/>
-      </c>
-      <c r="AL39" t="str">
+        <v>963</v>
+      </c>
+      <c r="AL39">
         <f>IF(error!AL14=1,time!AL14,"")</f>
-        <v/>
+        <v>1596</v>
       </c>
       <c r="AM39" t="str">
         <f>IF(error!AM14=1,time!AM14,"")</f>
         <v/>
       </c>
-      <c r="AN39" t="str">
+      <c r="AN39">
         <f>IF(error!AN14=1,time!AN14,"")</f>
-        <v/>
-      </c>
-      <c r="AO39" t="str">
+        <v>846</v>
+      </c>
+      <c r="AO39">
         <f>IF(error!AO14=1,time!AO14,"")</f>
-        <v/>
-      </c>
-      <c r="AP39" t="str">
+        <v>1663</v>
+      </c>
+      <c r="AP39">
         <f>IF(error!AP14=1,time!AP14,"")</f>
-        <v/>
+        <v>3403</v>
       </c>
       <c r="AQ39" t="str">
         <f>IF(error!AQ14=1,time!AQ14,"")</f>
         <v/>
       </c>
-      <c r="AR39" t="str">
+      <c r="AR39">
         <f>IF(error!AR14=1,time!AR14,"")</f>
-        <v/>
+        <v>2215</v>
       </c>
       <c r="AS39" t="str">
         <f>IF(error!AS14=1,time!AS14,"")</f>
         <v/>
       </c>
-      <c r="AT39" t="str">
+      <c r="AT39">
         <f>IF(error!AT14=1,time!AT14,"")</f>
-        <v/>
+        <v>1251</v>
       </c>
       <c r="AU39" t="str">
         <f>IF(error!AU14=1,time!AU14,"")</f>
         <v/>
       </c>
-      <c r="AV39" t="str">
+      <c r="AV39">
         <f>IF(error!AV14=1,time!AV14,"")</f>
-        <v/>
+        <v>831</v>
       </c>
       <c r="AW39" t="str">
         <f>IF(error!AW14=1,time!AW14,"")</f>
         <v/>
       </c>
-      <c r="AX39" t="str">
+      <c r="AX39">
         <f>IF(error!AX14=1,time!AX14,"")</f>
-        <v/>
-      </c>
-      <c r="AY39" t="str">
+        <v>1882</v>
+      </c>
+      <c r="AY39">
         <f>IF(error!AY14=1,time!AY14,"")</f>
-        <v/>
-      </c>
-      <c r="AZ39" t="str">
+        <v>5004</v>
+      </c>
+      <c r="AZ39">
         <f>IF(error!AZ14=1,time!AZ14,"")</f>
-        <v/>
+        <v>2569</v>
       </c>
       <c r="BA39" t="str">
         <f>IF(error!BA14=1,time!BA14,"")</f>
         <v/>
       </c>
-      <c r="BB39" t="str">
+      <c r="BB39">
         <f>IF(error!BB14=1,time!BB14,"")</f>
-        <v/>
+        <v>1198</v>
       </c>
       <c r="BC39" t="str">
         <f>IF(error!BC14=1,time!BC14,"")</f>
         <v/>
       </c>
-      <c r="BD39" t="str">
+      <c r="BD39">
         <f>IF(error!BD14=1,time!BD14,"")</f>
-        <v/>
+        <v>911</v>
       </c>
       <c r="BE39" t="str">
         <f>IF(error!BE14=1,time!BE14,"")</f>
         <v/>
       </c>
-      <c r="BF39" t="str">
+      <c r="BF39">
         <f>IF(error!BF14=1,time!BF14,"")</f>
-        <v/>
+        <v>1334</v>
       </c>
       <c r="BG39" t="str">
         <f>IF(error!BG14=1,time!BG14,"")</f>
         <v/>
       </c>
-      <c r="BH39" t="str">
+      <c r="BH39">
         <f>IF(error!BH14=1,time!BH14,"")</f>
-        <v/>
+        <v>2683</v>
       </c>
       <c r="BI39" t="str">
         <f>IF(error!BI14=1,time!BI14,"")</f>
@@ -12568,27 +13844,27 @@
       </c>
       <c r="B47">
         <f>AVERAGE(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42)</f>
-        <v>1123.5250000000001</v>
+        <v>1139.22</v>
       </c>
       <c r="C47">
         <f>AVERAGE(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42)</f>
-        <v>1551.3684210526317</v>
+        <v>1674.957894736842</v>
       </c>
       <c r="V47">
         <f t="shared" ref="V47:AQ47" si="26">AVERAGE(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42)</f>
-        <v>1015.725</v>
+        <v>1061.01</v>
       </c>
       <c r="W47">
         <f t="shared" si="26"/>
-        <v>1244.1756756756756</v>
+        <v>1278.989247311828</v>
       </c>
       <c r="AP47">
         <f t="shared" si="26"/>
-        <v>1315.1866666666667</v>
+        <v>1361.3157894736842</v>
       </c>
       <c r="AQ47">
         <f t="shared" si="26"/>
-        <v>2146.4193548387098</v>
+        <v>2478.15</v>
       </c>
     </row>
     <row r="48" spans="1:69">
@@ -12597,27 +13873,27 @@
       </c>
       <c r="B48">
         <f>STDEV((B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))/SQRT(COUNT(B30:B42,D30:D42,F30:F42,H30:H42,J30:J42,L30:L42,N30:N42,P30:P42,R30:R42,T30:T42))</f>
-        <v>31.352194798305373</v>
+        <v>29.235396354419407</v>
       </c>
       <c r="C48">
         <f>STDEV((C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))/SQRT(COUNT(C30:C42,E30:E42,G30:G42,I30:I42,K30:K42,M30:M42,O30:O42,Q30:Q42,S30:S42,U30:U42))</f>
-        <v>93.016923270842369</v>
+        <v>94.13276573395305</v>
       </c>
       <c r="V48">
         <f>STDEV((V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))/SQRT(COUNT(V30:V42,X30:X42,Z30:Z42,AB30:AB42,AD30:AD42,AF30:AF42,AH30:AH42,AJ30:AJ42,AL30:AL42,AN30:AN42))</f>
-        <v>44.483416676073965</v>
+        <v>39.413350799089905</v>
       </c>
       <c r="W48">
         <f>STDEV((W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))/SQRT(COUNT(W30:W42,Y30:Y42,AA30:AA42,AC30:AC42,AE30:AE42,AG30:AG42,AI30:AI42,AK30:AK42,AM30:AM42,AO30:AO42))</f>
-        <v>63.607603292640107</v>
+        <v>54.501606219974747</v>
       </c>
       <c r="AP48">
         <f>STDEV((AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))/SQRT(COUNT(AP30:AP42,AR30:AR42,AT30:AT42,AV30:AV42,AX30:AX42,AZ30:AZ42,BB30:BB42,BD30:BD42,BF30:BF42,BH30:BH42))</f>
-        <v>107.70861709165054</v>
+        <v>96.094400281935677</v>
       </c>
       <c r="AQ48">
         <f>STDEV((AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))/SQRT(COUNT(AQ30:AQ42,AS30:AS42,AU30:AU42,AW30:AW42,AY30:AY42,BA30:BA42,BC30:BC42,BE30:BE42,BG30:BG42,BI30:BI42))</f>
-        <v>243.31333740581513</v>
+        <v>231.95314389233542</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -12641,15 +13917,15 @@
       </c>
       <c r="B54">
         <f>B47</f>
-        <v>1123.5250000000001</v>
+        <v>1139.22</v>
       </c>
       <c r="C54">
         <f>V47</f>
-        <v>1015.725</v>
+        <v>1061.01</v>
       </c>
       <c r="D54">
         <f>AP47</f>
-        <v>1315.1866666666667</v>
+        <v>1361.3157894736842</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -12659,15 +13935,15 @@
       </c>
       <c r="B55">
         <f>C47</f>
-        <v>1551.3684210526317</v>
+        <v>1674.957894736842</v>
       </c>
       <c r="C55">
         <f>W47</f>
-        <v>1244.1756756756756</v>
+        <v>1278.989247311828</v>
       </c>
       <c r="D55">
         <f>AQ47</f>
-        <v>2146.4193548387098</v>
+        <v>2478.15</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -12691,15 +13967,15 @@
       </c>
       <c r="B60">
         <f>B48</f>
-        <v>31.352194798305373</v>
+        <v>29.235396354419407</v>
       </c>
       <c r="C60">
         <f>V48</f>
-        <v>44.483416676073965</v>
+        <v>39.413350799089905</v>
       </c>
       <c r="D60">
         <f>AP48</f>
-        <v>107.70861709165054</v>
+        <v>96.094400281935677</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -12709,15 +13985,15 @@
       </c>
       <c r="B61">
         <f>C48</f>
-        <v>93.016923270842369</v>
+        <v>94.13276573395305</v>
       </c>
       <c r="C61">
         <f>W48</f>
-        <v>63.607603292640107</v>
+        <v>54.501606219974747</v>
       </c>
       <c r="D61">
         <f>AQ48</f>
-        <v>243.31333740581513</v>
+        <v>231.95314389233542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>